<commit_message>
Round hour formats to given value
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -10432,10 +10432,10 @@
         <v/>
       </c>
       <c r="C7" s="233" t="n">
-        <v>0.6076388888888888</v>
+        <v>0.6597222222222222</v>
       </c>
       <c r="D7" s="234" t="n">
-        <v>0.7326388888888888</v>
+        <v>0.75</v>
       </c>
       <c r="E7" s="235">
         <f>IF(C7="","",D7-C7)</f>
@@ -10480,10 +10480,10 @@
         <v/>
       </c>
       <c r="C8" s="242" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="D8" s="243" t="n">
-        <v>0.5277777777777778</v>
+        <v>0.8055555555555556</v>
       </c>
       <c r="E8" s="244">
         <f>IF(C8="","",D8-C8)</f>
@@ -10520,10 +10520,10 @@
         <v/>
       </c>
       <c r="C9" s="242" t="n">
-        <v>0.3673611111111111</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="D9" s="243" t="n">
-        <v>0.4090277777777778</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E9" s="244">
         <f>IF(C9="","",D9-C9)</f>
@@ -10560,10 +10560,10 @@
         <v/>
       </c>
       <c r="C10" s="249" t="n">
-        <v>0.6006944444444444</v>
+        <v>0.6875</v>
       </c>
       <c r="D10" s="243" t="n">
-        <v>0.7256944444444444</v>
+        <v>0.8055555555555556</v>
       </c>
       <c r="E10" s="244">
         <f>IF(C10="","",D10-C10)</f>
@@ -10600,10 +10600,10 @@
         <v/>
       </c>
       <c r="C11" s="249" t="n">
-        <v>0.4972222222222222</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="D11" s="243" t="n">
-        <v>0.5805555555555556</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="E11" s="244">
         <f>IF(C11="","",D11-C11)</f>
@@ -10640,10 +10640,10 @@
         <v/>
       </c>
       <c r="C12" s="242" t="n">
-        <v>0.56875</v>
+        <v>0.6041666666666666</v>
       </c>
       <c r="D12" s="243" t="n">
-        <v>0.7770833333333333</v>
+        <v>0.7152777777777778</v>
       </c>
       <c r="E12" s="244">
         <f>IF(C12="","",D12-C12)</f>
@@ -10680,10 +10680,10 @@
         <v/>
       </c>
       <c r="C13" s="252" t="n">
-        <v>0.4659722222222222</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="D13" s="253" t="n">
-        <v>0.5493055555555556</v>
+        <v>0.7152777777777778</v>
       </c>
       <c r="E13" s="235">
         <f>IF(C13="","",D13-C13)</f>
@@ -10720,10 +10720,10 @@
         <v/>
       </c>
       <c r="C14" s="252" t="n">
-        <v>0.5430555555555555</v>
+        <v>0.3472222222222222</v>
       </c>
       <c r="D14" s="253" t="n">
-        <v>0.5847222222222223</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E14" s="235">
         <f>IF(C14="","",D14-C14)</f>
@@ -10760,10 +10760,10 @@
         <v/>
       </c>
       <c r="C15" s="242" t="n">
-        <v>0.4340277777777778</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="D15" s="243" t="n">
-        <v>0.5173611111111112</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="E15" s="244">
         <f>IF(C15="","",D15-C15)</f>
@@ -10800,10 +10800,10 @@
         <v/>
       </c>
       <c r="C16" s="242" t="n">
-        <v>0.3979166666666666</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="D16" s="243" t="n">
-        <v>0.60625</v>
+        <v>0.6180555555555556</v>
       </c>
       <c r="E16" s="244">
         <f>IF(C16="","",D16-C16)</f>
@@ -10840,10 +10840,10 @@
         <v/>
       </c>
       <c r="C17" s="249" t="n">
-        <v>0.6472222222222223</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="D17" s="243" t="n">
-        <v>0.6888888888888889</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="E17" s="244">
         <f>IF(C17="","",D17-C17)</f>
@@ -10880,10 +10880,10 @@
         <v/>
       </c>
       <c r="C18" s="249" t="n">
-        <v>0.5055555555555555</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="D18" s="243" t="n">
-        <v>0.5472222222222223</v>
+        <v>0.5625</v>
       </c>
       <c r="E18" s="244">
         <f>IF(C18="","",D18-C18)</f>
@@ -10920,10 +10920,10 @@
         <v/>
       </c>
       <c r="C19" s="242" t="n">
-        <v>0.4520833333333333</v>
+        <v>0.6458333333333334</v>
       </c>
       <c r="D19" s="243" t="n">
-        <v>0.7020833333333333</v>
+        <v>0.7152777777777778</v>
       </c>
       <c r="E19" s="244">
         <f>IF(C19="","",D19-C19)</f>
@@ -10960,10 +10960,10 @@
         <v/>
       </c>
       <c r="C20" s="252" t="n">
-        <v>0.6583333333333333</v>
+        <v>0.7569444444444444</v>
       </c>
       <c r="D20" s="253" t="n">
-        <v>0.7416666666666667</v>
+        <v>0.8263888888888888</v>
       </c>
       <c r="E20" s="235">
         <f>IF(C20="","",D20-C20)</f>
@@ -11000,10 +11000,10 @@
         <v/>
       </c>
       <c r="C21" s="252" t="n">
-        <v>0.7194444444444444</v>
+        <v>0.6319444444444444</v>
       </c>
       <c r="D21" s="253" t="n">
-        <v>0.8027777777777778</v>
+        <v>0.7430555555555556</v>
       </c>
       <c r="E21" s="235">
         <f>IF(C21="","",D21-C21)</f>
@@ -11040,10 +11040,10 @@
         <v/>
       </c>
       <c r="C22" s="242" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="D22" s="243" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.625</v>
       </c>
       <c r="E22" s="244">
         <f>IF(C22="","",D22-C22)</f>
@@ -11080,10 +11080,10 @@
         <v/>
       </c>
       <c r="C23" s="242" t="n">
-        <v>0.3708333333333333</v>
+        <v>0.7430555555555556</v>
       </c>
       <c r="D23" s="243" t="n">
-        <v>0.4541666666666667</v>
+        <v>0.7847222222222222</v>
       </c>
       <c r="E23" s="244">
         <f>IF(C23="","",D23-C23)</f>
@@ -11119,12 +11119,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="249" t="n">
-        <v>0.4604166666666666</v>
-      </c>
-      <c r="D24" s="243" t="n">
-        <v>0.54375</v>
-      </c>
+      <c r="C24" s="249" t="n"/>
+      <c r="D24" s="243" t="n"/>
       <c r="E24" s="244">
         <f>IF(C24="","",D24-C24)</f>
         <v/>
@@ -11160,10 +11156,10 @@
         <v/>
       </c>
       <c r="C25" s="249" t="n">
-        <v>0.4854166666666667</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="D25" s="243" t="n">
-        <v>0.56875</v>
+        <v>0.6180555555555556</v>
       </c>
       <c r="E25" s="244">
         <f>IF(C25="","",D25-C25)</f>
@@ -11200,10 +11196,10 @@
         <v/>
       </c>
       <c r="C26" s="242" t="n">
-        <v>0.73125</v>
+        <v>0.4027777777777778</v>
       </c>
       <c r="D26" s="243" t="n">
-        <v>0.8145833333333333</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E26" s="244">
         <f>IF(C26="","",D26-C26)</f>
@@ -11240,10 +11236,10 @@
         <v/>
       </c>
       <c r="C27" s="252" t="n">
-        <v>0.6506944444444445</v>
+        <v>0.625</v>
       </c>
       <c r="D27" s="253" t="n">
-        <v>0.7340277777777777</v>
+        <v>0.7013888888888888</v>
       </c>
       <c r="E27" s="235">
         <f>IF(C27="","",D27-C27)</f>
@@ -11279,12 +11275,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="252" t="n">
-        <v>0.4784722222222222</v>
-      </c>
-      <c r="D28" s="253" t="n">
-        <v>0.5618055555555556</v>
-      </c>
+      <c r="C28" s="252" t="n"/>
+      <c r="D28" s="253" t="n"/>
       <c r="E28" s="235">
         <f>IF(C28="","",D28-C28)</f>
         <v/>
@@ -11319,12 +11311,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="242" t="n">
-        <v>0.6534722222222222</v>
-      </c>
-      <c r="D29" s="243" t="n">
-        <v>0.7368055555555556</v>
-      </c>
+      <c r="C29" s="242" t="n"/>
+      <c r="D29" s="243" t="n"/>
       <c r="E29" s="244">
         <f>IF(C29="","",D29-C29)</f>
         <v/>
@@ -11360,10 +11348,10 @@
         <v/>
       </c>
       <c r="C30" s="242" t="n">
-        <v>0.3569444444444445</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="D30" s="243" t="n">
-        <v>0.3986111111111111</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E30" s="244">
         <f>IF(C30="","",D30-C30)</f>
@@ -11400,10 +11388,10 @@
         <v/>
       </c>
       <c r="C31" s="249" t="n">
-        <v>0.7236111111111111</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D31" s="243" t="n">
-        <v>0.8069444444444445</v>
+        <v>0.7013888888888888</v>
       </c>
       <c r="E31" s="244">
         <f>IF(C31="","",D31-C31)</f>
@@ -11440,10 +11428,10 @@
         <v/>
       </c>
       <c r="C32" s="249" t="n">
-        <v>0.3347222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="D32" s="243" t="n">
-        <v>0.4597222222222222</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E32" s="244">
         <f>IF(C32="","",D32-C32)</f>
@@ -11480,10 +11468,10 @@
         <v/>
       </c>
       <c r="C33" s="242" t="n">
-        <v>0.6611111111111111</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="D33" s="243" t="n">
-        <v>0.7444444444444445</v>
+        <v>0.625</v>
       </c>
       <c r="E33" s="244">
         <f>IF(C33="","",D33-C33)</f>
@@ -11520,10 +11508,10 @@
         <v/>
       </c>
       <c r="C34" s="252" t="n">
-        <v>0.5756944444444444</v>
+        <v>0.3472222222222222</v>
       </c>
       <c r="D34" s="253" t="n">
-        <v>0.8256944444444444</v>
+        <v>0.3819444444444444</v>
       </c>
       <c r="E34" s="235">
         <f>IF(C34="","",D34-C34)</f>
@@ -11559,12 +11547,8 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="252" t="n">
-        <v>0.4909722222222222</v>
-      </c>
-      <c r="D35" s="253" t="n">
-        <v>0.5743055555555555</v>
-      </c>
+      <c r="C35" s="252" t="n"/>
+      <c r="D35" s="253" t="n"/>
       <c r="E35" s="235">
         <f>IF(C35="","",D35-C35)</f>
         <v/>
@@ -11599,12 +11583,8 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="242" t="n">
-        <v>0.5965277777777778</v>
-      </c>
-      <c r="D36" s="243" t="n">
-        <v>0.6798611111111111</v>
-      </c>
+      <c r="C36" s="242" t="n"/>
+      <c r="D36" s="243" t="n"/>
       <c r="E36" s="244">
         <f>IF(C36="","",D36-C36)</f>
         <v/>
@@ -11640,10 +11620,10 @@
         <v/>
       </c>
       <c r="C37" s="256" t="n">
-        <v>0.4201388888888889</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="D37" s="257" t="n">
-        <v>0.5034722222222222</v>
+        <v>0.6041666666666666</v>
       </c>
       <c r="E37" s="258">
         <f>IF(C37="","",D37-C37)</f>
@@ -12784,10 +12764,10 @@
         <v/>
       </c>
       <c r="C7" s="315" t="n">
-        <v>0.51875</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="D7" s="316" t="n">
-        <v>0.64375</v>
+        <v>0.4375</v>
       </c>
       <c r="E7" s="296">
         <f>IF(C7="","",D7-C7)</f>
@@ -12825,10 +12805,10 @@
         <v/>
       </c>
       <c r="C8" s="242" t="n">
-        <v>0.6013888888888889</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="D8" s="243" t="n">
-        <v>0.6430555555555556</v>
+        <v>0.6736111111111112</v>
       </c>
       <c r="E8" s="244">
         <f>IF(C8="","",D8-C8)</f>
@@ -12866,10 +12846,10 @@
         <v/>
       </c>
       <c r="C9" s="295" t="n">
-        <v>0.4270833333333333</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="D9" s="253" t="n">
-        <v>0.5104166666666666</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="E9" s="235">
         <f>IF(C9="","",D9-C9)</f>
@@ -12913,8 +12893,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="249" t="n"/>
-      <c r="D10" s="243" t="n"/>
+      <c r="C10" s="249" t="n">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="D10" s="243" t="n">
+        <v>0.5555555555555556</v>
+      </c>
       <c r="E10" s="244">
         <f>IF(C10="","",D10-C10)</f>
         <v/>
@@ -13057,12 +13041,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="252" t="n">
-        <v>0.5645833333333333</v>
-      </c>
-      <c r="D14" s="253" t="n">
-        <v>0.6479166666666667</v>
-      </c>
+      <c r="C14" s="252" t="n"/>
+      <c r="D14" s="253" t="n"/>
       <c r="E14" s="235">
         <f>IF(C14="","",D14-C14)</f>
         <v/>
@@ -13098,10 +13078,10 @@
         <v/>
       </c>
       <c r="C15" s="242" t="n">
-        <v>0.4</v>
+        <v>0.7430555555555556</v>
       </c>
       <c r="D15" s="243" t="n">
-        <v>0.4416666666666667</v>
+        <v>0.7847222222222222</v>
       </c>
       <c r="E15" s="244">
         <f>IF(C15="","",D15-C15)</f>
@@ -13137,8 +13117,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="242" t="n"/>
-      <c r="D16" s="243" t="n"/>
+      <c r="C16" s="242" t="n">
+        <v>0.7152777777777778</v>
+      </c>
+      <c r="D16" s="243" t="n">
+        <v>0.7569444444444444</v>
+      </c>
       <c r="E16" s="244">
         <f>IF(C16="","",D16-C16)</f>
         <v/>
@@ -13174,10 +13158,10 @@
         <v/>
       </c>
       <c r="C17" s="249" t="n">
-        <v>0.4506944444444445</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="D17" s="243" t="n">
-        <v>0.5340277777777778</v>
+        <v>0.7569444444444444</v>
       </c>
       <c r="E17" s="244">
         <f>IF(C17="","",D17-C17)</f>
@@ -13249,8 +13233,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="242" t="n"/>
-      <c r="D19" s="243" t="n"/>
+      <c r="C19" s="242" t="n">
+        <v>0.7013888888888888</v>
+      </c>
+      <c r="D19" s="243" t="n">
+        <v>0.7569444444444444</v>
+      </c>
       <c r="E19" s="244">
         <f>IF(C19="","",D19-C19)</f>
         <v/>
@@ -13286,10 +13274,10 @@
         <v/>
       </c>
       <c r="C20" s="252" t="n">
-        <v>0.7868055555555555</v>
+        <v>0.3472222222222222</v>
       </c>
       <c r="D20" s="253" t="n">
-        <v>0.8284722222222223</v>
+        <v>0.4375</v>
       </c>
       <c r="E20" s="235">
         <f>IF(C20="","",D20-C20)</f>
@@ -13326,10 +13314,10 @@
         <v/>
       </c>
       <c r="C21" s="252" t="n">
-        <v>0.4201388888888889</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="D21" s="253" t="n">
-        <v>0.5034722222222222</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="E21" s="235">
         <f>IF(C21="","",D21-C21)</f>
@@ -13365,8 +13353,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="242" t="n"/>
-      <c r="D22" s="243" t="n"/>
+      <c r="C22" s="242" t="n">
+        <v>0.5902777777777778</v>
+      </c>
+      <c r="D22" s="243" t="n">
+        <v>0.6180555555555556</v>
+      </c>
       <c r="E22" s="244">
         <f>IF(C22="","",D22-C22)</f>
         <v/>
@@ -13401,12 +13393,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="242" t="n">
-        <v>0.69375</v>
-      </c>
-      <c r="D23" s="243" t="n">
-        <v>0.7354166666666667</v>
-      </c>
+      <c r="C23" s="242" t="n"/>
+      <c r="D23" s="243" t="n"/>
       <c r="E23" s="244">
         <f>IF(C23="","",D23-C23)</f>
         <v/>
@@ -13441,8 +13429,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="249" t="n"/>
-      <c r="D24" s="243" t="n"/>
+      <c r="C24" s="249" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="D24" s="243" t="n">
+        <v>0.7013888888888888</v>
+      </c>
       <c r="E24" s="244">
         <f>IF(C24="","",D24-C24)</f>
         <v/>
@@ -13478,10 +13470,10 @@
         <v/>
       </c>
       <c r="C25" s="249" t="n">
-        <v>0.5597222222222222</v>
+        <v>0.3819444444444444</v>
       </c>
       <c r="D25" s="243" t="n">
-        <v>0.6013888888888889</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="E25" s="244">
         <f>IF(C25="","",D25-C25)</f>
@@ -13517,12 +13509,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="242" t="n">
-        <v>0.3458333333333333</v>
-      </c>
-      <c r="D26" s="243" t="n">
-        <v>0.4708333333333333</v>
-      </c>
+      <c r="C26" s="242" t="n"/>
+      <c r="D26" s="243" t="n"/>
       <c r="E26" s="244">
         <f>IF(C26="","",D26-C26)</f>
         <v/>
@@ -13558,10 +13546,10 @@
         <v/>
       </c>
       <c r="C27" s="252" t="n">
-        <v>0.6270833333333333</v>
+        <v>0.375</v>
       </c>
       <c r="D27" s="253" t="n">
-        <v>0.66875</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="E27" s="235">
         <f>IF(C27="","",D27-C27)</f>
@@ -13598,10 +13586,10 @@
         <v/>
       </c>
       <c r="C28" s="252" t="n">
-        <v>0.4194444444444445</v>
+        <v>0.375</v>
       </c>
       <c r="D28" s="253" t="n">
-        <v>0.4611111111111111</v>
+        <v>0.4097222222222222</v>
       </c>
       <c r="E28" s="235">
         <f>IF(C28="","",D28-C28)</f>
@@ -13638,10 +13626,10 @@
         <v/>
       </c>
       <c r="C29" s="242" t="n">
-        <v>0.6173611111111111</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="D29" s="243" t="n">
-        <v>0.7006944444444444</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="E29" s="244">
         <f>IF(C29="","",D29-C29)</f>
@@ -13678,10 +13666,10 @@
         <v/>
       </c>
       <c r="C30" s="242" t="n">
-        <v>0.5409722222222222</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="D30" s="243" t="n">
-        <v>0.7909722222222222</v>
+        <v>0.5625</v>
       </c>
       <c r="E30" s="244">
         <f>IF(C30="","",D30-C30)</f>
@@ -13718,10 +13706,10 @@
         <v/>
       </c>
       <c r="C31" s="249" t="n">
-        <v>0.6916666666666667</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="D31" s="243" t="n">
-        <v>0.7333333333333333</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E31" s="244">
         <f>IF(C31="","",D31-C31)</f>
@@ -13757,12 +13745,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="249" t="n">
-        <v>0.5361111111111111</v>
-      </c>
-      <c r="D32" s="243" t="n">
-        <v>0.6611111111111111</v>
-      </c>
+      <c r="C32" s="249" t="n"/>
+      <c r="D32" s="243" t="n"/>
       <c r="E32" s="244">
         <f>IF(C32="","",D32-C32)</f>
         <v/>
@@ -13833,8 +13817,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="252" t="n"/>
-      <c r="D34" s="253" t="n"/>
+      <c r="C34" s="252" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D34" s="253" t="n">
+        <v>0.3680555555555556</v>
+      </c>
       <c r="E34" s="235">
         <f>IF(C34="","",D34-C34)</f>
         <v/>
@@ -13870,10 +13858,10 @@
         <v/>
       </c>
       <c r="C35" s="252" t="n">
-        <v>0.3993055555555556</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="D35" s="253" t="n">
-        <v>0.4409722222222222</v>
+        <v>0.6527777777777778</v>
       </c>
       <c r="E35" s="235">
         <f>IF(C35="","",D35-C35)</f>
@@ -13910,10 +13898,10 @@
         <v/>
       </c>
       <c r="C36" s="242" t="n">
-        <v>0.4138888888888889</v>
+        <v>0.6736111111111112</v>
       </c>
       <c r="D36" s="243" t="n">
-        <v>0.4555555555555555</v>
+        <v>0.7152777777777778</v>
       </c>
       <c r="E36" s="244">
         <f>IF(C36="","",D36-C36)</f>
@@ -13950,10 +13938,10 @@
         <v/>
       </c>
       <c r="C37" s="306" t="n">
-        <v>0.5506944444444445</v>
+        <v>0.6041666666666666</v>
       </c>
       <c r="D37" s="307" t="n">
-        <v>0.5923611111111111</v>
+        <v>0.7847222222222222</v>
       </c>
       <c r="E37" s="308">
         <f>IF(C37="","",D37-C37)</f>
@@ -15262,10 +15250,10 @@
         <v/>
       </c>
       <c r="C8" s="249" t="n">
-        <v>0.5097222222222222</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="D8" s="243" t="n">
-        <v>0.7597222222222222</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E8" s="244">
         <f>IF(C8="","",D8-C8)</f>
@@ -15303,10 +15291,10 @@
         <v/>
       </c>
       <c r="C9" s="242" t="n">
-        <v>0.4208333333333333</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="D9" s="243" t="n">
-        <v>0.5458333333333333</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E9" s="244">
         <f>IF(C9="","",D9-C9)</f>
@@ -15380,8 +15368,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="252" t="n"/>
-      <c r="D11" s="253" t="n"/>
+      <c r="C11" s="252" t="n">
+        <v>0.5694444444444444</v>
+      </c>
+      <c r="D11" s="253" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="E11" s="235">
         <f>IF(C11="","",D11-C11)</f>
         <v/>
@@ -15418,10 +15410,10 @@
         <v/>
       </c>
       <c r="C12" s="242" t="n">
-        <v>0.6395833333333333</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="D12" s="243" t="n">
-        <v>0.68125</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E12" s="244">
         <f>IF(C12="","",D12-C12)</f>
@@ -15496,10 +15488,10 @@
         <v/>
       </c>
       <c r="C14" s="249" t="n">
-        <v>0.45625</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="D14" s="243" t="n">
-        <v>0.4979166666666667</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="E14" s="244">
         <f>IF(C14="","",D14-C14)</f>
@@ -15537,10 +15529,10 @@
         <v/>
       </c>
       <c r="C15" s="249" t="n">
-        <v>0.5479166666666667</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="D15" s="243" t="n">
-        <v>0.7979166666666667</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E15" s="244">
         <f>IF(C15="","",D15-C15)</f>
@@ -15577,12 +15569,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="242" t="n">
-        <v>0.6256944444444444</v>
-      </c>
-      <c r="D16" s="243" t="n">
-        <v>0.7090277777777778</v>
-      </c>
+      <c r="C16" s="242" t="n"/>
+      <c r="D16" s="243" t="n"/>
       <c r="E16" s="244">
         <f>IF(C16="","",D16-C16)</f>
         <v/>
@@ -15619,10 +15607,10 @@
         <v/>
       </c>
       <c r="C17" s="252" t="n">
-        <v>0.6256944444444444</v>
+        <v>0.5</v>
       </c>
       <c r="D17" s="253" t="n">
-        <v>0.7090277777777778</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E17" s="235">
         <f>IF(C17="","",D17-C17)</f>
@@ -15660,10 +15648,10 @@
         <v/>
       </c>
       <c r="C18" s="252" t="n">
-        <v>0.7041666666666667</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="D18" s="253" t="n">
-        <v>0.7458333333333333</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="E18" s="235">
         <f>IF(C18="","",D18-C18)</f>
@@ -15701,10 +15689,10 @@
         <v/>
       </c>
       <c r="C19" s="242" t="n">
-        <v>0.7659722222222223</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="D19" s="243" t="n">
-        <v>0.8076388888888889</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="E19" s="244">
         <f>IF(C19="","",D19-C19)</f>
@@ -15741,12 +15729,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="242" t="n">
-        <v>0.6951388888888889</v>
-      </c>
-      <c r="D20" s="243" t="n">
-        <v>0.7368055555555556</v>
-      </c>
+      <c r="C20" s="242" t="n"/>
+      <c r="D20" s="243" t="n"/>
       <c r="E20" s="244">
         <f>IF(C20="","",D20-C20)</f>
         <v/>
@@ -15782,12 +15766,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="249" t="n">
-        <v>0.3493055555555555</v>
-      </c>
-      <c r="D21" s="243" t="n">
-        <v>0.5993055555555555</v>
-      </c>
+      <c r="C21" s="249" t="n"/>
+      <c r="D21" s="243" t="n"/>
       <c r="E21" s="244">
         <f>IF(C21="","",D21-C21)</f>
         <v/>
@@ -15824,10 +15804,10 @@
         <v/>
       </c>
       <c r="C22" s="249" t="n">
-        <v>0.4777777777777778</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="D22" s="243" t="n">
-        <v>0.5611111111111111</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="E22" s="244">
         <f>IF(C22="","",D22-C22)</f>
@@ -15901,12 +15881,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="252" t="n">
-        <v>0.5972222222222222</v>
-      </c>
-      <c r="D24" s="253" t="n">
-        <v>0.6388888888888888</v>
-      </c>
+      <c r="C24" s="252" t="n"/>
+      <c r="D24" s="253" t="n"/>
       <c r="E24" s="235">
         <f>IF(C24="","",D24-C24)</f>
         <v/>
@@ -15943,10 +15919,10 @@
         <v/>
       </c>
       <c r="C25" s="252" t="n">
-        <v>0.4375</v>
+        <v>0.3680555555555556</v>
       </c>
       <c r="D25" s="253" t="n">
-        <v>0.5625</v>
+        <v>0.3958333333333333</v>
       </c>
       <c r="E25" s="235">
         <f>IF(C25="","",D25-C25)</f>
@@ -16020,8 +15996,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="242" t="n"/>
-      <c r="D27" s="243" t="n"/>
+      <c r="C27" s="242" t="n">
+        <v>0.4652777777777778</v>
+      </c>
+      <c r="D27" s="243" t="n">
+        <v>0.6388888888888888</v>
+      </c>
       <c r="E27" s="244">
         <f>IF(C27="","",D27-C27)</f>
         <v/>
@@ -16058,10 +16038,10 @@
         <v/>
       </c>
       <c r="C28" s="249" t="n">
-        <v>0.5951388888888889</v>
+        <v>0.7430555555555556</v>
       </c>
       <c r="D28" s="243" t="n">
-        <v>0.7201388888888889</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="E28" s="244">
         <f>IF(C28="","",D28-C28)</f>
@@ -16099,10 +16079,10 @@
         <v/>
       </c>
       <c r="C29" s="249" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="D29" s="243" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="E29" s="244">
         <f>IF(C29="","",D29-C29)</f>
@@ -16140,10 +16120,10 @@
         <v/>
       </c>
       <c r="C30" s="242" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="D30" s="243" t="n">
-        <v>0.575</v>
+        <v>0.7638888888888888</v>
       </c>
       <c r="E30" s="244">
         <f>IF(C30="","",D30-C30)</f>
@@ -16180,12 +16160,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="252" t="n">
-        <v>0.3895833333333333</v>
-      </c>
-      <c r="D31" s="253" t="n">
-        <v>0.43125</v>
-      </c>
+      <c r="C31" s="252" t="n"/>
+      <c r="D31" s="253" t="n"/>
       <c r="E31" s="235">
         <f>IF(C31="","",D31-C31)</f>
         <v/>
@@ -16221,12 +16197,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="252" t="n">
-        <v>0.6298611111111111</v>
-      </c>
-      <c r="D32" s="253" t="n">
-        <v>0.7548611111111111</v>
-      </c>
+      <c r="C32" s="252" t="n"/>
+      <c r="D32" s="253" t="n"/>
       <c r="E32" s="235">
         <f>IF(C32="","",D32-C32)</f>
         <v/>
@@ -16263,10 +16235,10 @@
         <v/>
       </c>
       <c r="C33" s="242" t="n">
-        <v>0.4625</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="D33" s="243" t="n">
-        <v>0.5875</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E33" s="244">
         <f>IF(C33="","",D33-C33)</f>
@@ -16303,12 +16275,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="242" t="n">
-        <v>0.6979166666666666</v>
-      </c>
-      <c r="D34" s="243" t="n">
-        <v>0.7395833333333334</v>
-      </c>
+      <c r="C34" s="242" t="n"/>
+      <c r="D34" s="243" t="n"/>
       <c r="E34" s="244">
         <f>IF(C34="","",D34-C34)</f>
         <v/>
@@ -16345,10 +16313,10 @@
         <v/>
       </c>
       <c r="C35" s="249" t="n">
-        <v>0.5166666666666667</v>
+        <v>0.7569444444444444</v>
       </c>
       <c r="D35" s="243" t="n">
-        <v>0.5583333333333333</v>
+        <v>0.7847222222222222</v>
       </c>
       <c r="E35" s="244">
         <f>IF(C35="","",D35-C35)</f>
@@ -16386,10 +16354,10 @@
         <v/>
       </c>
       <c r="C36" s="335" t="n">
-        <v>0.5375</v>
+        <v>0.375</v>
       </c>
       <c r="D36" s="257" t="n">
-        <v>0.6208333333333333</v>
+        <v>0.625</v>
       </c>
       <c r="E36" s="258">
         <f>IF(C36="","",D36-C36)</f>
@@ -17354,8 +17322,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="345" t="n"/>
-      <c r="D7" s="346" t="n"/>
+      <c r="C7" s="345" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="D7" s="346" t="n">
+        <v>0.7777777777777778</v>
+      </c>
       <c r="E7" s="292">
         <f>IF(C7="","",D7-C7)</f>
         <v/>
@@ -17390,8 +17362,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="252" t="n"/>
-      <c r="D8" s="253" t="n"/>
+      <c r="C8" s="252" t="n">
+        <v>0.6944444444444444</v>
+      </c>
+      <c r="D8" s="253" t="n">
+        <v>0.7291666666666666</v>
+      </c>
       <c r="E8" s="235">
         <f>IF(C8="","",D8-C8)</f>
         <v/>
@@ -17426,12 +17402,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="252" t="n">
-        <v>0.4465277777777778</v>
-      </c>
-      <c r="D9" s="253" t="n">
-        <v>0.4881944444444444</v>
-      </c>
+      <c r="C9" s="252" t="n"/>
+      <c r="D9" s="253" t="n"/>
       <c r="E9" s="235">
         <f>IF(C9="","",D9-C9)</f>
         <v/>
@@ -17467,10 +17439,10 @@
         <v/>
       </c>
       <c r="C10" s="242" t="n">
-        <v>0.3618055555555555</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="D10" s="243" t="n">
-        <v>0.4034722222222222</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="E10" s="244">
         <f>IF(C10="","",D10-C10)</f>
@@ -17506,8 +17478,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="242" t="n"/>
-      <c r="D11" s="243" t="n"/>
+      <c r="C11" s="242" t="n">
+        <v>0.7291666666666666</v>
+      </c>
+      <c r="D11" s="243" t="n">
+        <v>0.8125</v>
+      </c>
       <c r="E11" s="244">
         <f>IF(C11="","",D11-C11)</f>
         <v/>
@@ -17542,8 +17518,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="249" t="n"/>
-      <c r="D12" s="243" t="n"/>
+      <c r="C12" s="249" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="D12" s="243" t="n">
+        <v>0.7986111111111112</v>
+      </c>
       <c r="E12" s="244">
         <f>IF(C12="","",D12-C12)</f>
         <v/>
@@ -17579,10 +17559,10 @@
         <v/>
       </c>
       <c r="C13" s="249" t="n">
-        <v>0.3895833333333333</v>
+        <v>0.5625</v>
       </c>
       <c r="D13" s="243" t="n">
-        <v>0.43125</v>
+        <v>0.6458333333333334</v>
       </c>
       <c r="E13" s="244">
         <f>IF(C13="","",D13-C13)</f>
@@ -17619,10 +17599,10 @@
         <v/>
       </c>
       <c r="C14" s="242" t="n">
-        <v>0.4430555555555555</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="D14" s="243" t="n">
-        <v>0.4847222222222222</v>
+        <v>0.7152777777777778</v>
       </c>
       <c r="E14" s="244">
         <f>IF(C14="","",D14-C14)</f>
@@ -17659,10 +17639,10 @@
         <v/>
       </c>
       <c r="C15" s="252" t="n">
-        <v>0.5576388888888889</v>
+        <v>0.4375</v>
       </c>
       <c r="D15" s="253" t="n">
-        <v>0.6826388888888889</v>
+        <v>0.6041666666666666</v>
       </c>
       <c r="E15" s="235">
         <f>IF(C15="","",D15-C15)</f>
@@ -17698,12 +17678,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="319" t="n">
-        <v>0.5402777777777777</v>
-      </c>
-      <c r="D16" s="320" t="n">
-        <v>0.7069444444444445</v>
-      </c>
+      <c r="C16" s="319" t="n"/>
+      <c r="D16" s="320" t="n"/>
       <c r="E16" s="235">
         <f>IF(C16="","",D16-C16)</f>
         <v/>
@@ -17739,10 +17715,10 @@
         <v/>
       </c>
       <c r="C17" s="318" t="n">
-        <v>0.4055555555555556</v>
+        <v>0.5138888888888888</v>
       </c>
       <c r="D17" s="291" t="n">
-        <v>0.4472222222222222</v>
+        <v>0.625</v>
       </c>
       <c r="E17" s="244">
         <f>IF(C17="","",D17-C17)</f>
@@ -17779,10 +17755,10 @@
         <v/>
       </c>
       <c r="C18" s="242" t="n">
-        <v>0.4409722222222222</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="D18" s="243" t="n">
-        <v>0.4826388888888889</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E18" s="244">
         <f>IF(C18="","",D18-C18)</f>
@@ -17818,8 +17794,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="249" t="n"/>
-      <c r="D19" s="243" t="n"/>
+      <c r="C19" s="249" t="n">
+        <v>0.3541666666666667</v>
+      </c>
+      <c r="D19" s="243" t="n">
+        <v>0.375</v>
+      </c>
       <c r="E19" s="244">
         <f>IF(C19="","",D19-C19)</f>
         <v/>
@@ -17855,10 +17835,10 @@
         <v/>
       </c>
       <c r="C20" s="249" t="n">
-        <v>0.3486111111111111</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="D20" s="243" t="n">
-        <v>0.4319444444444445</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E20" s="244">
         <f>IF(C20="","",D20-C20)</f>
@@ -17895,10 +17875,10 @@
         <v/>
       </c>
       <c r="C21" s="242" t="n">
-        <v>0.68125</v>
+        <v>0.6180555555555556</v>
       </c>
       <c r="D21" s="243" t="n">
-        <v>0.7229166666666667</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="E21" s="244">
         <f>IF(C21="","",D21-C21)</f>
@@ -17934,8 +17914,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="252" t="n"/>
-      <c r="D22" s="253" t="n"/>
+      <c r="C22" s="252" t="n">
+        <v>0.6041666666666666</v>
+      </c>
+      <c r="D22" s="253" t="n">
+        <v>0.6527777777777778</v>
+      </c>
       <c r="E22" s="235">
         <f>IF(C22="","",D22-C22)</f>
         <v/>
@@ -17971,10 +17955,10 @@
         <v/>
       </c>
       <c r="C23" s="252" t="n">
-        <v>0.4270833333333333</v>
+        <v>0.5902777777777778</v>
       </c>
       <c r="D23" s="253" t="n">
-        <v>0.46875</v>
+        <v>0.8125</v>
       </c>
       <c r="E23" s="235">
         <f>IF(C23="","",D23-C23)</f>
@@ -18011,10 +17995,10 @@
         <v/>
       </c>
       <c r="C24" s="242" t="n">
-        <v>0.3951388888888889</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="D24" s="243" t="n">
-        <v>0.4784722222222222</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E24" s="244">
         <f>IF(C24="","",D24-C24)</f>
@@ -18050,12 +18034,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="242" t="n">
-        <v>0.3597222222222222</v>
-      </c>
-      <c r="D25" s="243" t="n">
-        <v>0.4430555555555555</v>
-      </c>
+      <c r="C25" s="242" t="n"/>
+      <c r="D25" s="243" t="n"/>
       <c r="E25" s="244">
         <f>IF(C25="","",D25-C25)</f>
         <v/>
@@ -18091,10 +18071,10 @@
         <v/>
       </c>
       <c r="C26" s="249" t="n">
-        <v>0.3652777777777778</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="D26" s="243" t="n">
-        <v>0.4486111111111111</v>
+        <v>0.6736111111111112</v>
       </c>
       <c r="E26" s="244">
         <f>IF(C26="","",D26-C26)</f>
@@ -18131,10 +18111,10 @@
         <v/>
       </c>
       <c r="C27" s="249" t="n">
-        <v>0.4125</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="D27" s="243" t="n">
-        <v>0.4541666666666667</v>
+        <v>0.5347222222222222</v>
       </c>
       <c r="E27" s="244">
         <f>IF(C27="","",D27-C27)</f>
@@ -18171,10 +18151,10 @@
         <v/>
       </c>
       <c r="C28" s="242" t="n">
-        <v>0.4409722222222222</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="D28" s="243" t="n">
-        <v>0.5243055555555556</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="E28" s="244">
         <f>IF(C28="","",D28-C28)</f>
@@ -18210,8 +18190,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="252" t="n"/>
-      <c r="D29" s="253" t="n"/>
+      <c r="C29" s="252" t="n">
+        <v>0.5347222222222222</v>
+      </c>
+      <c r="D29" s="253" t="n">
+        <v>0.6180555555555556</v>
+      </c>
       <c r="E29" s="235">
         <f>IF(C29="","",D29-C29)</f>
         <v/>
@@ -18246,8 +18230,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="295" t="n"/>
-      <c r="D30" s="253" t="n"/>
+      <c r="C30" s="295" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="D30" s="253" t="n">
+        <v>0.7291666666666666</v>
+      </c>
       <c r="E30" s="235">
         <f>IF(C30="","",D30-C30)</f>
         <v/>
@@ -18290,8 +18278,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="295" t="n"/>
-      <c r="D31" s="253" t="n"/>
+      <c r="C31" s="295" t="n">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="D31" s="253" t="n">
+        <v>0.5138888888888888</v>
+      </c>
       <c r="E31" s="235">
         <f>IF(C31="","",D31-C31)</f>
         <v/>
@@ -18335,10 +18327,10 @@
         <v/>
       </c>
       <c r="C32" s="295" t="n">
-        <v>0.4340277777777778</v>
+        <v>0.7430555555555556</v>
       </c>
       <c r="D32" s="253" t="n">
-        <v>0.4756944444444444</v>
+        <v>0.7847222222222222</v>
       </c>
       <c r="E32" s="235">
         <f>IF(C32="","",D32-C32)</f>
@@ -18419,10 +18411,10 @@
         <v/>
       </c>
       <c r="C34" s="249" t="n">
-        <v>0.3652777777777778</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="D34" s="243" t="n">
-        <v>0.4069444444444444</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="E34" s="244">
         <f>IF(C34="","",D34-C34)</f>
@@ -18459,10 +18451,10 @@
         <v/>
       </c>
       <c r="C35" s="242" t="n">
-        <v>0.7381944444444445</v>
+        <v>0.6041666666666666</v>
       </c>
       <c r="D35" s="243" t="n">
-        <v>0.7798611111111111</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="E35" s="244">
         <f>IF(C35="","",D35-C35)</f>
@@ -18499,10 +18491,10 @@
         <v/>
       </c>
       <c r="C36" s="252" t="n">
-        <v>0.4819444444444445</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="D36" s="253" t="n">
-        <v>0.7319444444444444</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="E36" s="235">
         <f>IF(C36="","",D36-C36)</f>
@@ -19307,10 +19299,10 @@
         <v/>
       </c>
       <c r="C7" s="290" t="n">
-        <v>0.4625</v>
+        <v>0.5625</v>
       </c>
       <c r="D7" s="291" t="n">
-        <v>0.5875</v>
+        <v>0.5972222222222222</v>
       </c>
       <c r="E7" s="292">
         <f>IF(C7="","",D7-C7)</f>
@@ -19348,10 +19340,10 @@
         <v/>
       </c>
       <c r="C8" s="249" t="n">
-        <v>0.3715277777777778</v>
+        <v>0.3819444444444444</v>
       </c>
       <c r="D8" s="243" t="n">
-        <v>0.6215277777777778</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="E8" s="244">
         <f>IF(C8="","",D8-C8)</f>
@@ -19389,10 +19381,10 @@
         <v/>
       </c>
       <c r="C9" s="249" t="n">
-        <v>0.38125</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="D9" s="243" t="n">
-        <v>0.4645833333333333</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="E9" s="244">
         <f>IF(C9="","",D9-C9)</f>
@@ -19430,10 +19422,10 @@
         <v/>
       </c>
       <c r="C10" s="295" t="n">
-        <v>0.7</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="D10" s="253" t="n">
-        <v>0.7833333333333333</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E10" s="235">
         <f>IF(C10="","",D10-C10)</f>
@@ -19471,10 +19463,10 @@
         <v/>
       </c>
       <c r="C11" s="295" t="n">
-        <v>0.6895833333333333</v>
+        <v>0.7013888888888888</v>
       </c>
       <c r="D11" s="253" t="n">
-        <v>0.73125</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="E11" s="235">
         <f>IF(C11="","",D11-C11)</f>
@@ -19512,10 +19504,10 @@
         <v/>
       </c>
       <c r="C12" s="249" t="n">
-        <v>0.3840277777777778</v>
+        <v>0.3680555555555556</v>
       </c>
       <c r="D12" s="243" t="n">
-        <v>0.5923611111111111</v>
+        <v>0.3958333333333333</v>
       </c>
       <c r="E12" s="244">
         <f>IF(C12="","",D12-C12)</f>
@@ -19553,10 +19545,10 @@
         <v/>
       </c>
       <c r="C13" s="249" t="n">
-        <v>0.6555555555555556</v>
+        <v>0.7152777777777778</v>
       </c>
       <c r="D13" s="243" t="n">
-        <v>0.7805555555555556</v>
+        <v>0.7708333333333334</v>
       </c>
       <c r="E13" s="244">
         <f>IF(C13="","",D13-C13)</f>
@@ -19594,10 +19586,10 @@
         <v/>
       </c>
       <c r="C14" s="249" t="n">
-        <v>0.3361111111111111</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="D14" s="243" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.5625</v>
       </c>
       <c r="E14" s="244">
         <f>IF(C14="","",D14-C14)</f>
@@ -19635,10 +19627,10 @@
         <v/>
       </c>
       <c r="C15" s="249" t="n">
-        <v>0.5409722222222222</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="D15" s="243" t="n">
-        <v>0.6659722222222222</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E15" s="244">
         <f>IF(C15="","",D15-C15)</f>
@@ -19676,10 +19668,10 @@
         <v/>
       </c>
       <c r="C16" s="249" t="n">
-        <v>0.4270833333333333</v>
+        <v>0.7569444444444444</v>
       </c>
       <c r="D16" s="243" t="n">
-        <v>0.5520833333333334</v>
+        <v>0.8194444444444444</v>
       </c>
       <c r="E16" s="244">
         <f>IF(C16="","",D16-C16)</f>
@@ -19717,10 +19709,10 @@
         <v/>
       </c>
       <c r="C17" s="295" t="n">
-        <v>0.3590277777777778</v>
+        <v>0.5763888888888888</v>
       </c>
       <c r="D17" s="253" t="n">
-        <v>0.4006944444444445</v>
+        <v>0.6527777777777778</v>
       </c>
       <c r="E17" s="235">
         <f>IF(C17="","",D17-C17)</f>
@@ -19758,10 +19750,10 @@
         <v/>
       </c>
       <c r="C18" s="295" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.375</v>
       </c>
       <c r="D18" s="253" t="n">
-        <v>0.45</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E18" s="235">
         <f>IF(C18="","",D18-C18)</f>
@@ -19799,10 +19791,10 @@
         <v/>
       </c>
       <c r="C19" s="249" t="n">
-        <v>0.6583333333333333</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="D19" s="243" t="n">
-        <v>0.7416666666666667</v>
+        <v>0.6736111111111112</v>
       </c>
       <c r="E19" s="244">
         <f>IF(C19="","",D19-C19)</f>
@@ -19840,10 +19832,10 @@
         <v/>
       </c>
       <c r="C20" s="249" t="n">
-        <v>0.4006944444444445</v>
+        <v>0.625</v>
       </c>
       <c r="D20" s="243" t="n">
-        <v>0.5673611111111111</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E20" s="244">
         <f>IF(C20="","",D20-C20)</f>
@@ -19880,12 +19872,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="249" t="n">
-        <v>0.5381944444444444</v>
-      </c>
-      <c r="D21" s="243" t="n">
-        <v>0.5798611111111112</v>
-      </c>
+      <c r="C21" s="249" t="n"/>
+      <c r="D21" s="243" t="n"/>
       <c r="E21" s="244">
         <f>IF(C21="","",D21-C21)</f>
         <v/>
@@ -19921,12 +19909,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="249" t="n">
-        <v>0.6625</v>
-      </c>
-      <c r="D22" s="243" t="n">
-        <v>0.7041666666666667</v>
-      </c>
+      <c r="C22" s="249" t="n"/>
+      <c r="D22" s="243" t="n"/>
       <c r="E22" s="244">
         <f>IF(C22="","",D22-C22)</f>
         <v/>
@@ -19963,10 +19947,10 @@
         <v/>
       </c>
       <c r="C23" s="249" t="n">
-        <v>0.6298611111111111</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="D23" s="243" t="n">
-        <v>0.6715277777777777</v>
+        <v>0.6527777777777778</v>
       </c>
       <c r="E23" s="244">
         <f>IF(C23="","",D23-C23)</f>
@@ -20004,12 +19988,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="295" t="n">
-        <v>0.6138888888888889</v>
-      </c>
-      <c r="D24" s="253" t="n">
-        <v>0.6555555555555556</v>
-      </c>
+      <c r="C24" s="295" t="n"/>
+      <c r="D24" s="253" t="n"/>
       <c r="E24" s="235">
         <f>IF(C24="","",D24-C24)</f>
         <v/>
@@ -20047,10 +20027,10 @@
         <v/>
       </c>
       <c r="C25" s="295" t="n">
-        <v>0.4131944444444444</v>
+        <v>0.4375</v>
       </c>
       <c r="D25" s="253" t="n">
-        <v>0.4548611111111111</v>
+        <v>0.5972222222222222</v>
       </c>
       <c r="E25" s="235">
         <f>IF(C25="","",D25-C25)</f>
@@ -20088,10 +20068,10 @@
         <v/>
       </c>
       <c r="C26" s="249" t="n">
-        <v>0.4645833333333333</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="D26" s="243" t="n">
-        <v>0.5479166666666667</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="E26" s="244">
         <f>IF(C26="","",D26-C26)</f>
@@ -20128,12 +20108,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="249" t="n">
-        <v>0.5805555555555556</v>
-      </c>
-      <c r="D27" s="243" t="n">
-        <v>0.7055555555555556</v>
-      </c>
+      <c r="C27" s="249" t="n"/>
+      <c r="D27" s="243" t="n"/>
       <c r="E27" s="244">
         <f>IF(C27="","",D27-C27)</f>
         <v/>
@@ -20169,12 +20145,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="249" t="n">
-        <v>0.48125</v>
-      </c>
-      <c r="D28" s="243" t="n">
-        <v>0.5645833333333333</v>
-      </c>
+      <c r="C28" s="249" t="n"/>
+      <c r="D28" s="243" t="n"/>
       <c r="E28" s="244">
         <f>IF(C28="","",D28-C28)</f>
         <v/>
@@ -20211,10 +20183,10 @@
         <v/>
       </c>
       <c r="C29" s="249" t="n">
-        <v>0.4215277777777778</v>
+        <v>0.3680555555555556</v>
       </c>
       <c r="D29" s="243" t="n">
-        <v>0.5048611111111111</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="E29" s="244">
         <f>IF(C29="","",D29-C29)</f>
@@ -20252,10 +20224,10 @@
         <v/>
       </c>
       <c r="C30" s="249" t="n">
-        <v>0.3416666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D30" s="243" t="n">
-        <v>0.3833333333333334</v>
+        <v>0.3680555555555556</v>
       </c>
       <c r="E30" s="244">
         <f>IF(C30="","",D30-C30)</f>
@@ -20293,10 +20265,10 @@
         <v/>
       </c>
       <c r="C31" s="295" t="n">
-        <v>0.7756944444444445</v>
+        <v>0.5972222222222222</v>
       </c>
       <c r="D31" s="253" t="n">
-        <v>0.8173611111111111</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="E31" s="235">
         <f>IF(C31="","",D31-C31)</f>
@@ -20371,10 +20343,10 @@
         <v/>
       </c>
       <c r="C33" s="249" t="n">
-        <v>0.6208333333333333</v>
+        <v>0.5902777777777778</v>
       </c>
       <c r="D33" s="243" t="n">
-        <v>0.6625</v>
+        <v>0.6319444444444444</v>
       </c>
       <c r="E33" s="244">
         <f>IF(C33="","",D33-C33)</f>
@@ -20412,10 +20384,10 @@
         <v/>
       </c>
       <c r="C34" s="300" t="n">
-        <v>0.7618055555555555</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="D34" s="300" t="n">
-        <v>0.8034722222222223</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="E34" s="301">
         <f>IF(C34="","",D34-C34)</f>
@@ -20452,12 +20424,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B34+1))</f>
         <v/>
       </c>
-      <c r="C35" s="300" t="n">
-        <v>0.4006944444444445</v>
-      </c>
-      <c r="D35" s="300" t="n">
-        <v>0.4840277777777778</v>
-      </c>
+      <c r="C35" s="300" t="n"/>
+      <c r="D35" s="300" t="n"/>
       <c r="E35" s="301">
         <f>IF(C35="","",D35-C35)</f>
         <v/>
@@ -21590,10 +21558,10 @@
         <v/>
       </c>
       <c r="C7" s="290" t="n">
-        <v>0.4819444444444445</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="D7" s="291" t="n">
-        <v>0.6486111111111111</v>
+        <v>0.7430555555555556</v>
       </c>
       <c r="E7" s="244">
         <f>IF(C7="","",D7-C7)</f>
@@ -21667,8 +21635,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="242" t="n"/>
-      <c r="D9" s="243" t="n"/>
+      <c r="C9" s="242" t="n">
+        <v>0.5138888888888888</v>
+      </c>
+      <c r="D9" s="243" t="n">
+        <v>0.5902777777777778</v>
+      </c>
       <c r="E9" s="244">
         <f>IF(C9="","",D9-C9)</f>
         <v/>
@@ -21704,12 +21676,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="252" t="n">
-        <v>0.66875</v>
-      </c>
-      <c r="D10" s="253" t="n">
-        <v>0.79375</v>
-      </c>
+      <c r="C10" s="252" t="n"/>
+      <c r="D10" s="253" t="n"/>
       <c r="E10" s="235">
         <f>IF(C10="","",D10-C10)</f>
         <v/>
@@ -21783,10 +21751,10 @@
         <v/>
       </c>
       <c r="C12" s="242" t="n">
-        <v>0.5736111111111111</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="D12" s="243" t="n">
-        <v>0.6569444444444444</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="E12" s="244">
         <f>IF(C12="","",D12-C12)</f>
@@ -21823,8 +21791,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="242" t="n"/>
-      <c r="D13" s="243" t="n"/>
+      <c r="C13" s="242" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="D13" s="243" t="n">
+        <v>0.5902777777777778</v>
+      </c>
       <c r="E13" s="244">
         <f>IF(C13="","",D13-C13)</f>
         <v/>
@@ -21861,10 +21833,10 @@
         <v/>
       </c>
       <c r="C14" s="295" t="n">
-        <v>0.6784722222222223</v>
+        <v>0.5972222222222222</v>
       </c>
       <c r="D14" s="253" t="n">
-        <v>0.8034722222222223</v>
+        <v>0.6597222222222222</v>
       </c>
       <c r="E14" s="235">
         <f>IF(C14="","",D14-C14)</f>
@@ -21946,8 +21918,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="242" t="n"/>
-      <c r="D16" s="243" t="n"/>
+      <c r="C16" s="242" t="n">
+        <v>0.6458333333333334</v>
+      </c>
+      <c r="D16" s="243" t="n">
+        <v>0.6666666666666666</v>
+      </c>
       <c r="E16" s="244">
         <f>IF(C16="","",D16-C16)</f>
         <v/>
@@ -21984,10 +21960,10 @@
         <v/>
       </c>
       <c r="C17" s="252" t="n">
-        <v>0.5722222222222222</v>
+        <v>0.3402777777777778</v>
       </c>
       <c r="D17" s="253" t="n">
-        <v>0.6138888888888889</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E17" s="235">
         <f>IF(C17="","",D17-C17)</f>
@@ -22025,10 +22001,10 @@
         <v/>
       </c>
       <c r="C18" s="252" t="n">
-        <v>0.7229166666666667</v>
+        <v>0.4027777777777778</v>
       </c>
       <c r="D18" s="253" t="n">
-        <v>0.7645833333333333</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E18" s="235">
         <f>IF(C18="","",D18-C18)</f>
@@ -22065,12 +22041,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="242" t="n">
-        <v>0.3597222222222222</v>
-      </c>
-      <c r="D19" s="243" t="n">
-        <v>0.5680555555555555</v>
-      </c>
+      <c r="C19" s="242" t="n"/>
+      <c r="D19" s="243" t="n"/>
       <c r="E19" s="244">
         <f>IF(C19="","",D19-C19)</f>
         <v/>
@@ -22106,12 +22078,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="242" t="n">
-        <v>0.6277777777777778</v>
-      </c>
-      <c r="D20" s="243" t="n">
-        <v>0.7944444444444444</v>
-      </c>
+      <c r="C20" s="242" t="n"/>
+      <c r="D20" s="243" t="n"/>
       <c r="E20" s="244">
         <f>IF(C20="","",D20-C20)</f>
         <v/>
@@ -22148,10 +22116,10 @@
         <v/>
       </c>
       <c r="C21" s="249" t="n">
-        <v>0.7673611111111112</v>
+        <v>0.375</v>
       </c>
       <c r="D21" s="243" t="n">
-        <v>0.8090277777777778</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="E21" s="244">
         <f>IF(C21="","",D21-C21)</f>
@@ -22189,10 +22157,10 @@
         <v/>
       </c>
       <c r="C22" s="249" t="n">
-        <v>0.4479166666666667</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="D22" s="243" t="n">
-        <v>0.5729166666666666</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E22" s="244">
         <f>IF(C22="","",D22-C22)</f>
@@ -22229,8 +22197,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="242" t="n"/>
-      <c r="D23" s="243" t="n"/>
+      <c r="C23" s="242" t="n">
+        <v>0.4375</v>
+      </c>
+      <c r="D23" s="243" t="n">
+        <v>0.5</v>
+      </c>
       <c r="E23" s="244">
         <f>IF(C23="","",D23-C23)</f>
         <v/>
@@ -22266,12 +22238,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="252" t="n">
-        <v>0.4736111111111111</v>
-      </c>
-      <c r="D24" s="253" t="n">
-        <v>0.5152777777777777</v>
-      </c>
+      <c r="C24" s="252" t="n"/>
+      <c r="D24" s="253" t="n"/>
       <c r="E24" s="235">
         <f>IF(C24="","",D24-C24)</f>
         <v/>
@@ -22308,10 +22276,10 @@
         <v/>
       </c>
       <c r="C25" s="252" t="n">
-        <v>0.7180555555555556</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="D25" s="253" t="n">
-        <v>0.7597222222222222</v>
+        <v>0.7986111111111112</v>
       </c>
       <c r="E25" s="235">
         <f>IF(C25="","",D25-C25)</f>
@@ -22349,10 +22317,10 @@
         <v/>
       </c>
       <c r="C26" s="242" t="n">
-        <v>0.5097222222222222</v>
+        <v>0.375</v>
       </c>
       <c r="D26" s="243" t="n">
-        <v>0.5513888888888889</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="E26" s="244">
         <f>IF(C26="","",D26-C26)</f>
@@ -22427,10 +22395,10 @@
         <v/>
       </c>
       <c r="C28" s="249" t="n">
-        <v>0.5888888888888889</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="D28" s="243" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.6875</v>
       </c>
       <c r="E28" s="244">
         <f>IF(C28="","",D28-C28)</f>
@@ -22467,12 +22435,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="249" t="n">
-        <v>0.5590277777777778</v>
-      </c>
-      <c r="D29" s="243" t="n">
-        <v>0.8090277777777778</v>
-      </c>
+      <c r="C29" s="249" t="n"/>
+      <c r="D29" s="243" t="n"/>
       <c r="E29" s="244">
         <f>IF(C29="","",D29-C29)</f>
         <v/>
@@ -22509,10 +22473,10 @@
         <v/>
       </c>
       <c r="C30" s="242" t="n">
-        <v>0.7840277777777778</v>
+        <v>0.6805555555555556</v>
       </c>
       <c r="D30" s="243" t="n">
-        <v>0.8256944444444444</v>
+        <v>0.7013888888888888</v>
       </c>
       <c r="E30" s="244">
         <f>IF(C30="","",D30-C30)</f>
@@ -22549,12 +22513,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="252" t="n">
-        <v>0.3854166666666667</v>
-      </c>
-      <c r="D31" s="253" t="n">
-        <v>0.4270833333333333</v>
-      </c>
+      <c r="C31" s="252" t="n"/>
+      <c r="D31" s="253" t="n"/>
       <c r="E31" s="235">
         <f>IF(C31="","",D31-C31)</f>
         <v/>
@@ -22591,10 +22551,10 @@
         <v/>
       </c>
       <c r="C32" s="252" t="n">
-        <v>0.3895833333333333</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="D32" s="253" t="n">
-        <v>0.43125</v>
+        <v>0.5138888888888888</v>
       </c>
       <c r="E32" s="235">
         <f>IF(C32="","",D32-C32)</f>
@@ -22631,12 +22591,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="242" t="n">
-        <v>0.3861111111111111</v>
-      </c>
-      <c r="D33" s="243" t="n">
-        <v>0.4694444444444444</v>
-      </c>
+      <c r="C33" s="242" t="n"/>
+      <c r="D33" s="243" t="n"/>
       <c r="E33" s="244">
         <f>IF(C33="","",D33-C33)</f>
         <v/>
@@ -22673,10 +22629,10 @@
         <v/>
       </c>
       <c r="C34" s="242" t="n">
-        <v>0.7208333333333333</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="D34" s="243" t="n">
-        <v>0.7625</v>
+        <v>0.7152777777777778</v>
       </c>
       <c r="E34" s="244">
         <f>IF(C34="","",D34-C34)</f>
@@ -22713,12 +22669,8 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="249" t="n">
-        <v>0.4215277777777778</v>
-      </c>
-      <c r="D35" s="243" t="n">
-        <v>0.6715277777777777</v>
-      </c>
+      <c r="C35" s="249" t="n"/>
+      <c r="D35" s="243" t="n"/>
       <c r="E35" s="244">
         <f>IF(C35="","",D35-C35)</f>
         <v/>
@@ -22754,8 +22706,12 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="249" t="n"/>
-      <c r="D36" s="243" t="n"/>
+      <c r="C36" s="249" t="n">
+        <v>0.4652777777777778</v>
+      </c>
+      <c r="D36" s="243" t="n">
+        <v>0.5416666666666666</v>
+      </c>
       <c r="E36" s="244">
         <f>IF(C36="","",D36-C36)</f>
         <v/>
@@ -22791,8 +22747,12 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="306" t="n"/>
-      <c r="D37" s="307" t="n"/>
+      <c r="C37" s="306" t="n">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D37" s="307" t="n">
+        <v>0.6180555555555556</v>
+      </c>
       <c r="E37" s="308">
         <f>IF(C37="","",D37-C37)</f>
         <v/>
@@ -24003,10 +23963,10 @@
         <v/>
       </c>
       <c r="C8" s="252" t="n">
-        <v>0.5631944444444444</v>
+        <v>0.5</v>
       </c>
       <c r="D8" s="253" t="n">
-        <v>0.6048611111111111</v>
+        <v>0.5347222222222222</v>
       </c>
       <c r="E8" s="235">
         <f>IF(C8="","",D8-C8)</f>
@@ -24042,10 +24002,10 @@
         <v/>
       </c>
       <c r="C9" s="242" t="n">
-        <v>0.3951388888888889</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="D9" s="243" t="n">
-        <v>0.4784722222222222</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="E9" s="244">
         <f>IF(C9="","",D9-C9)</f>
@@ -24116,10 +24076,10 @@
         <v/>
       </c>
       <c r="C11" s="249" t="n">
-        <v>0.4868055555555555</v>
+        <v>0.3541666666666667</v>
       </c>
       <c r="D11" s="243" t="n">
-        <v>0.6951388888888889</v>
+        <v>0.4375</v>
       </c>
       <c r="E11" s="244">
         <f>IF(C11="","",D11-C11)</f>
@@ -24190,10 +24150,10 @@
         <v/>
       </c>
       <c r="C13" s="252" t="n">
-        <v>0.5055555555555555</v>
+        <v>0.6041666666666666</v>
       </c>
       <c r="D13" s="253" t="n">
-        <v>0.5472222222222223</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E13" s="235">
         <f>IF(C13="","",D13-C13)</f>
@@ -24237,10 +24197,10 @@
         <v/>
       </c>
       <c r="C14" s="252" t="n">
-        <v>0.7611111111111111</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="D14" s="253" t="n">
-        <v>0.8027777777777778</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="E14" s="235">
         <f>IF(C14="","",D14-C14)</f>
@@ -24318,12 +24278,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="252" t="n">
-        <v>0.5298611111111111</v>
-      </c>
-      <c r="D16" s="253" t="n">
-        <v>0.5715277777777777</v>
-      </c>
+      <c r="C16" s="252" t="n"/>
+      <c r="D16" s="253" t="n"/>
       <c r="E16" s="235">
         <f>IF(C16="","",D16-C16)</f>
         <v/>
@@ -24366,10 +24322,10 @@
         <v/>
       </c>
       <c r="C17" s="242" t="n">
-        <v>0.5534722222222223</v>
+        <v>0.5138888888888888</v>
       </c>
       <c r="D17" s="243" t="n">
-        <v>0.8034722222222223</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="E17" s="244">
         <f>IF(C17="","",D17-C17)</f>
@@ -24405,10 +24361,10 @@
         <v/>
       </c>
       <c r="C18" s="249" t="n">
-        <v>0.6916666666666667</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="D18" s="243" t="n">
-        <v>0.775</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E18" s="244">
         <f>IF(C18="","",D18-C18)</f>
@@ -24443,8 +24399,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="249" t="n"/>
-      <c r="D19" s="243" t="n"/>
+      <c r="C19" s="249" t="n">
+        <v>0.5138888888888888</v>
+      </c>
+      <c r="D19" s="243" t="n">
+        <v>0.5555555555555556</v>
+      </c>
       <c r="E19" s="244">
         <f>IF(C19="","",D19-C19)</f>
         <v/>
@@ -24479,10 +24439,10 @@
         <v/>
       </c>
       <c r="C20" s="318" t="n">
-        <v>0.7055555555555556</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="D20" s="291" t="n">
-        <v>0.7888888888888889</v>
+        <v>0.8125</v>
       </c>
       <c r="E20" s="244">
         <f>IF(C20="","",D20-C20)</f>
@@ -24517,8 +24477,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="252" t="n"/>
-      <c r="D21" s="253" t="n"/>
+      <c r="C21" s="252" t="n">
+        <v>0.4097222222222222</v>
+      </c>
+      <c r="D21" s="253" t="n">
+        <v>0.5555555555555556</v>
+      </c>
       <c r="E21" s="235">
         <f>IF(C21="","",D21-C21)</f>
         <v/>
@@ -24587,12 +24551,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="318" t="n">
-        <v>0.3472222222222222</v>
-      </c>
-      <c r="D23" s="291" t="n">
-        <v>0.4305555555555556</v>
-      </c>
+      <c r="C23" s="318" t="n"/>
+      <c r="D23" s="291" t="n"/>
       <c r="E23" s="244">
         <f>IF(C23="","",D23-C23)</f>
         <v/>
@@ -24627,10 +24587,10 @@
         <v/>
       </c>
       <c r="C24" s="249" t="n">
-        <v>0.5979166666666667</v>
+        <v>0.4097222222222222</v>
       </c>
       <c r="D24" s="243" t="n">
-        <v>0.6395833333333333</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="E24" s="244">
         <f>IF(C24="","",D24-C24)</f>
@@ -24665,8 +24625,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="249" t="n"/>
-      <c r="D25" s="243" t="n"/>
+      <c r="C25" s="249" t="n">
+        <v>0.6944444444444444</v>
+      </c>
+      <c r="D25" s="243" t="n">
+        <v>0.8263888888888888</v>
+      </c>
       <c r="E25" s="244">
         <f>IF(C25="","",D25-C25)</f>
         <v/>
@@ -24700,12 +24664,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="249" t="n">
-        <v>0.5395833333333333</v>
-      </c>
-      <c r="D26" s="243" t="n">
-        <v>0.6645833333333333</v>
-      </c>
+      <c r="C26" s="249" t="n"/>
+      <c r="D26" s="243" t="n"/>
       <c r="E26" s="244">
         <f>IF(C26="","",D26-C26)</f>
         <v/>
@@ -24740,10 +24700,10 @@
         <v/>
       </c>
       <c r="C27" s="249" t="n">
-        <v>0.6534722222222222</v>
+        <v>0.5972222222222222</v>
       </c>
       <c r="D27" s="243" t="n">
-        <v>0.7784722222222222</v>
+        <v>0.6458333333333334</v>
       </c>
       <c r="E27" s="244">
         <f>IF(C27="","",D27-C27)</f>
@@ -24779,10 +24739,10 @@
         <v/>
       </c>
       <c r="C28" s="252" t="n">
-        <v>0.3361111111111111</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="D28" s="253" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.6736111111111112</v>
       </c>
       <c r="E28" s="235">
         <f>IF(C28="","",D28-C28)</f>
@@ -24818,10 +24778,10 @@
         <v/>
       </c>
       <c r="C29" s="319" t="n">
-        <v>0.7784722222222222</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="D29" s="320" t="n">
-        <v>0.8201388888888889</v>
+        <v>0.7361111111111112</v>
       </c>
       <c r="E29" s="235">
         <f>IF(C29="","",D29-C29)</f>
@@ -24857,10 +24817,10 @@
         <v/>
       </c>
       <c r="C30" s="318" t="n">
-        <v>0.4569444444444444</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="D30" s="291" t="n">
-        <v>0.5402777777777777</v>
+        <v>0.6527777777777778</v>
       </c>
       <c r="E30" s="244">
         <f>IF(C30="","",D30-C30)</f>
@@ -24896,10 +24856,10 @@
         <v/>
       </c>
       <c r="C31" s="242" t="n">
-        <v>0.5006944444444444</v>
+        <v>0.6319444444444444</v>
       </c>
       <c r="D31" s="243" t="n">
-        <v>0.5840277777777778</v>
+        <v>0.6597222222222222</v>
       </c>
       <c r="E31" s="244">
         <f>IF(C31="","",D31-C31)</f>
@@ -24934,12 +24894,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="249" t="n">
-        <v>0.6263888888888889</v>
-      </c>
-      <c r="D32" s="243" t="n">
-        <v>0.6680555555555555</v>
-      </c>
+      <c r="C32" s="249" t="n"/>
+      <c r="D32" s="243" t="n"/>
       <c r="E32" s="244">
         <f>IF(C32="","",D32-C32)</f>
         <v/>
@@ -24973,8 +24929,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="249" t="n"/>
-      <c r="D33" s="243" t="n"/>
+      <c r="C33" s="249" t="n">
+        <v>0.5486111111111112</v>
+      </c>
+      <c r="D33" s="243" t="n">
+        <v>0.6041666666666666</v>
+      </c>
       <c r="E33" s="244">
         <f>IF(C33="","",D33-C33)</f>
         <v/>
@@ -25009,10 +24969,10 @@
         <v/>
       </c>
       <c r="C34" s="242" t="n">
-        <v>0.6847222222222222</v>
+        <v>0.6805555555555556</v>
       </c>
       <c r="D34" s="243" t="n">
-        <v>0.7263888888888889</v>
+        <v>0.7013888888888888</v>
       </c>
       <c r="E34" s="244">
         <f>IF(C34="","",D34-C34)</f>
@@ -25047,12 +25007,8 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="252" t="n">
-        <v>0.6625</v>
-      </c>
-      <c r="D35" s="253" t="n">
-        <v>0.7875</v>
-      </c>
+      <c r="C35" s="252" t="n"/>
+      <c r="D35" s="253" t="n"/>
       <c r="E35" s="235">
         <f>IF(C35="","",D35-C35)</f>
         <v/>
@@ -25087,10 +25043,10 @@
         <v/>
       </c>
       <c r="C36" s="322" t="n">
-        <v>0.5131944444444444</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="D36" s="323" t="n">
-        <v>0.6381944444444444</v>
+        <v>0.6458333333333334</v>
       </c>
       <c r="E36" s="324">
         <f>IF(C36="","",D36-C36)</f>
@@ -26316,12 +26272,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="233" t="n">
-        <v>0.3451388888888889</v>
-      </c>
-      <c r="D7" s="234" t="n">
-        <v>0.4284722222222222</v>
-      </c>
+      <c r="C7" s="233" t="n"/>
+      <c r="D7" s="234" t="n"/>
       <c r="E7" s="235">
         <f>IF(C7="","",D7-C7)</f>
         <v/>
@@ -26365,12 +26317,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="242" t="n">
-        <v>0.7298611111111111</v>
-      </c>
-      <c r="D8" s="243" t="n">
-        <v>0.7715277777777778</v>
-      </c>
+      <c r="C8" s="242" t="n"/>
+      <c r="D8" s="243" t="n"/>
       <c r="E8" s="244">
         <f>IF(C8="","",D8-C8)</f>
         <v/>
@@ -26407,10 +26355,10 @@
         <v/>
       </c>
       <c r="C9" s="249" t="n">
-        <v>0.4076388888888889</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="D9" s="243" t="n">
-        <v>0.4909722222222222</v>
+        <v>0.5</v>
       </c>
       <c r="E9" s="244">
         <f>IF(C9="","",D9-C9)</f>
@@ -26446,12 +26394,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="249" t="n">
-        <v>0.6451388888888889</v>
-      </c>
-      <c r="D10" s="243" t="n">
-        <v>0.6868055555555556</v>
-      </c>
+      <c r="C10" s="249" t="n"/>
+      <c r="D10" s="243" t="n"/>
       <c r="E10" s="244">
         <f>IF(C10="","",D10-C10)</f>
         <v/>
@@ -26486,8 +26430,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="242" t="n"/>
-      <c r="D11" s="243" t="n"/>
+      <c r="C11" s="242" t="n">
+        <v>0.6736111111111112</v>
+      </c>
+      <c r="D11" s="243" t="n">
+        <v>0.7777777777777778</v>
+      </c>
       <c r="E11" s="244">
         <f>IF(C11="","",D11-C11)</f>
         <v/>
@@ -26523,10 +26471,10 @@
         <v/>
       </c>
       <c r="C12" s="252" t="n">
-        <v>0.6201388888888889</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="D12" s="253" t="n">
-        <v>0.7868055555555555</v>
+        <v>0.5138888888888888</v>
       </c>
       <c r="E12" s="235">
         <f>IF(C12="","",D12-C12)</f>
@@ -26598,8 +26546,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="242" t="n"/>
-      <c r="D14" s="243" t="n"/>
+      <c r="C14" s="242" t="n">
+        <v>0.5763888888888888</v>
+      </c>
+      <c r="D14" s="243" t="n">
+        <v>0.7638888888888888</v>
+      </c>
       <c r="E14" s="244">
         <f>IF(C14="","",D14-C14)</f>
         <v/>
@@ -26635,10 +26587,10 @@
         <v/>
       </c>
       <c r="C15" s="242" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="D15" s="243" t="n">
-        <v>0.5902777777777778</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="E15" s="244">
         <f>IF(C15="","",D15-C15)</f>
@@ -26711,10 +26663,10 @@
         <v/>
       </c>
       <c r="C17" s="249" t="n">
-        <v>0.5298611111111111</v>
+        <v>0.3402777777777778</v>
       </c>
       <c r="D17" s="243" t="n">
-        <v>0.6548611111111111</v>
+        <v>0.3680555555555556</v>
       </c>
       <c r="E17" s="244">
         <f>IF(C17="","",D17-C17)</f>
@@ -26751,10 +26703,10 @@
         <v/>
       </c>
       <c r="C18" s="242" t="n">
-        <v>0.6125</v>
+        <v>0.5972222222222222</v>
       </c>
       <c r="D18" s="243" t="n">
-        <v>0.6958333333333333</v>
+        <v>0.6736111111111112</v>
       </c>
       <c r="E18" s="244">
         <f>IF(C18="","",D18-C18)</f>
@@ -26790,8 +26742,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="252" t="n"/>
-      <c r="D19" s="253" t="n"/>
+      <c r="C19" s="252" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="D19" s="253" t="n">
+        <v>0.5833333333333334</v>
+      </c>
       <c r="E19" s="235">
         <f>IF(C19="","",D19-C19)</f>
         <v/>
@@ -26827,10 +26783,10 @@
         <v/>
       </c>
       <c r="C20" s="252" t="n">
-        <v>0.5444444444444444</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="D20" s="253" t="n">
-        <v>0.5861111111111111</v>
+        <v>0.75</v>
       </c>
       <c r="E20" s="235">
         <f>IF(C20="","",D20-C20)</f>
@@ -26866,8 +26822,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="242" t="n"/>
-      <c r="D21" s="243" t="n"/>
+      <c r="C21" s="242" t="n">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D21" s="243" t="n">
+        <v>0.5625</v>
+      </c>
       <c r="E21" s="244">
         <f>IF(C21="","",D21-C21)</f>
         <v/>
@@ -26902,12 +26862,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="242" t="n">
-        <v>0.5472222222222223</v>
-      </c>
-      <c r="D22" s="243" t="n">
-        <v>0.6305555555555555</v>
-      </c>
+      <c r="C22" s="242" t="n"/>
+      <c r="D22" s="243" t="n"/>
       <c r="E22" s="244">
         <f>IF(C22="","",D22-C22)</f>
         <v/>
@@ -26943,10 +26899,10 @@
         <v/>
       </c>
       <c r="C23" s="249" t="n">
-        <v>0.5013888888888889</v>
+        <v>0.6805555555555556</v>
       </c>
       <c r="D23" s="243" t="n">
-        <v>0.5430555555555555</v>
+        <v>0.7708333333333334</v>
       </c>
       <c r="E23" s="244">
         <f>IF(C23="","",D23-C23)</f>
@@ -26983,10 +26939,10 @@
         <v/>
       </c>
       <c r="C24" s="295" t="n">
-        <v>0.3729166666666667</v>
+        <v>0.4097222222222222</v>
       </c>
       <c r="D24" s="253" t="n">
-        <v>0.4145833333333334</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E24" s="235">
         <f>IF(C24="","",D24-C24)</f>
@@ -27031,10 +26987,10 @@
         <v/>
       </c>
       <c r="C25" s="242" t="n">
-        <v>0.3833333333333334</v>
+        <v>0.375</v>
       </c>
       <c r="D25" s="243" t="n">
-        <v>0.5916666666666667</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E25" s="244">
         <f>IF(C25="","",D25-C25)</f>
@@ -27071,10 +27027,10 @@
         <v/>
       </c>
       <c r="C26" s="252" t="n">
-        <v>0.4361111111111111</v>
+        <v>0.3402777777777778</v>
       </c>
       <c r="D26" s="253" t="n">
-        <v>0.5194444444444445</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E26" s="235">
         <f>IF(C26="","",D26-C26)</f>
@@ -27110,12 +27066,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="252" t="n">
-        <v>0.3527777777777778</v>
-      </c>
-      <c r="D27" s="253" t="n">
-        <v>0.4777777777777778</v>
-      </c>
+      <c r="C27" s="252" t="n"/>
+      <c r="D27" s="253" t="n"/>
       <c r="E27" s="235">
         <f>IF(C27="","",D27-C27)</f>
         <v/>
@@ -27151,10 +27103,10 @@
         <v/>
       </c>
       <c r="C28" s="242" t="n">
-        <v>0.4694444444444444</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="D28" s="243" t="n">
-        <v>0.5111111111111111</v>
+        <v>0.5138888888888888</v>
       </c>
       <c r="E28" s="244">
         <f>IF(C28="","",D28-C28)</f>
@@ -27191,10 +27143,10 @@
         <v/>
       </c>
       <c r="C29" s="242" t="n">
-        <v>0.5701388888888889</v>
+        <v>0.375</v>
       </c>
       <c r="D29" s="243" t="n">
-        <v>0.6118055555555556</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="E29" s="244">
         <f>IF(C29="","",D29-C29)</f>
@@ -27230,8 +27182,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="249" t="n"/>
-      <c r="D30" s="243" t="n"/>
+      <c r="C30" s="249" t="n">
+        <v>0.6388888888888888</v>
+      </c>
+      <c r="D30" s="243" t="n">
+        <v>0.8194444444444444</v>
+      </c>
       <c r="E30" s="244">
         <f>IF(C30="","",D30-C30)</f>
         <v/>
@@ -27267,10 +27223,10 @@
         <v/>
       </c>
       <c r="C31" s="249" t="n">
-        <v>0.3520833333333334</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="D31" s="243" t="n">
-        <v>0.39375</v>
+        <v>0.6597222222222222</v>
       </c>
       <c r="E31" s="244">
         <f>IF(C31="","",D31-C31)</f>
@@ -27307,10 +27263,10 @@
         <v/>
       </c>
       <c r="C32" s="242" t="n">
-        <v>0.6541666666666667</v>
+        <v>0.5625</v>
       </c>
       <c r="D32" s="243" t="n">
-        <v>0.6958333333333333</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E32" s="244">
         <f>IF(C32="","",D32-C32)</f>
@@ -27346,12 +27302,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="252" t="n">
-        <v>0.35625</v>
-      </c>
-      <c r="D33" s="253" t="n">
-        <v>0.4395833333333333</v>
-      </c>
+      <c r="C33" s="252" t="n"/>
+      <c r="D33" s="253" t="n"/>
       <c r="E33" s="235">
         <f>IF(C33="","",D33-C33)</f>
         <v/>
@@ -27387,10 +27339,10 @@
         <v/>
       </c>
       <c r="C34" s="252" t="n">
-        <v>0.40625</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="D34" s="253" t="n">
-        <v>0.4479166666666667</v>
+        <v>0.7152777777777778</v>
       </c>
       <c r="E34" s="235">
         <f>IF(C34="","",D34-C34)</f>
@@ -27434,8 +27386,12 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="295" t="n"/>
-      <c r="D35" s="253" t="n"/>
+      <c r="C35" s="295" t="n">
+        <v>0.6041666666666666</v>
+      </c>
+      <c r="D35" s="253" t="n">
+        <v>0.6736111111111112</v>
+      </c>
       <c r="E35" s="235">
         <f>IF(C35="","",D35-C35)</f>
         <v/>
@@ -27478,8 +27434,12 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="242" t="n"/>
-      <c r="D36" s="243" t="n"/>
+      <c r="C36" s="242" t="n">
+        <v>0.6180555555555556</v>
+      </c>
+      <c r="D36" s="243" t="n">
+        <v>0.6875</v>
+      </c>
       <c r="E36" s="244">
         <f>IF(C36="","",D36-C36)</f>
         <v/>
@@ -27514,8 +27474,12 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="335" t="n"/>
-      <c r="D37" s="257" t="n"/>
+      <c r="C37" s="335" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="D37" s="257" t="n">
+        <v>0.5625</v>
+      </c>
       <c r="E37" s="258">
         <f>IF(C37="","",D37-C37)</f>
         <v/>
@@ -28834,12 +28798,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="290" t="n">
-        <v>0.4416666666666667</v>
-      </c>
-      <c r="D7" s="291" t="n">
-        <v>0.5666666666666667</v>
-      </c>
+      <c r="C7" s="290" t="n"/>
+      <c r="D7" s="291" t="n"/>
       <c r="E7" s="244">
         <f>IF(C7="","",D7-C7)</f>
         <v/>
@@ -28875,10 +28835,10 @@
         <v/>
       </c>
       <c r="C8" s="242" t="n">
-        <v>0.4611111111111111</v>
+        <v>0.3541666666666667</v>
       </c>
       <c r="D8" s="243" t="n">
-        <v>0.5444444444444444</v>
+        <v>0.3958333333333333</v>
       </c>
       <c r="E8" s="244">
         <f>IF(C8="","",D8-C8)</f>
@@ -28915,10 +28875,10 @@
         <v/>
       </c>
       <c r="C9" s="252" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="D9" s="253" t="n">
-        <v>0.7972222222222223</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="E9" s="235">
         <f>IF(C9="","",D9-C9)</f>
@@ -28954,12 +28914,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="252" t="n">
-        <v>0.3375</v>
-      </c>
-      <c r="D10" s="253" t="n">
-        <v>0.3791666666666667</v>
-      </c>
+      <c r="C10" s="252" t="n"/>
+      <c r="D10" s="253" t="n"/>
       <c r="E10" s="235">
         <f>IF(C10="","",D10-C10)</f>
         <v/>
@@ -28995,10 +28951,10 @@
         <v/>
       </c>
       <c r="C11" s="242" t="n">
-        <v>0.5291666666666667</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="D11" s="243" t="n">
-        <v>0.6125</v>
+        <v>0.75</v>
       </c>
       <c r="E11" s="244">
         <f>IF(C11="","",D11-C11)</f>
@@ -29034,12 +28990,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="242" t="n">
-        <v>0.6375</v>
-      </c>
-      <c r="D12" s="243" t="n">
-        <v>0.6791666666666667</v>
-      </c>
+      <c r="C12" s="242" t="n"/>
+      <c r="D12" s="243" t="n"/>
       <c r="E12" s="244">
         <f>IF(C12="","",D12-C12)</f>
         <v/>
@@ -29182,8 +29134,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="252" t="n"/>
-      <c r="D16" s="253" t="n"/>
+      <c r="C16" s="252" t="n">
+        <v>0.3958333333333333</v>
+      </c>
+      <c r="D16" s="253" t="n">
+        <v>0.4305555555555556</v>
+      </c>
       <c r="E16" s="235">
         <f>IF(C16="","",D16-C16)</f>
         <v/>
@@ -29254,8 +29210,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="242" t="n"/>
-      <c r="D18" s="243" t="n"/>
+      <c r="C18" s="242" t="n">
+        <v>0.4722222222222222</v>
+      </c>
+      <c r="D18" s="243" t="n">
+        <v>0.5069444444444444</v>
+      </c>
       <c r="E18" s="244">
         <f>IF(C18="","",D18-C18)</f>
         <v/>
@@ -29291,10 +29251,10 @@
         <v/>
       </c>
       <c r="C19" s="242" t="n">
-        <v>0.5826388888888889</v>
+        <v>0.4027777777777778</v>
       </c>
       <c r="D19" s="243" t="n">
-        <v>0.6243055555555556</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E19" s="244">
         <f>IF(C19="","",D19-C19)</f>
@@ -29330,12 +29290,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="249" t="n">
-        <v>0.7270833333333333</v>
-      </c>
-      <c r="D20" s="243" t="n">
-        <v>0.76875</v>
-      </c>
+      <c r="C20" s="249" t="n"/>
+      <c r="D20" s="243" t="n"/>
       <c r="E20" s="244">
         <f>IF(C20="","",D20-C20)</f>
         <v/>
@@ -29371,10 +29327,10 @@
         <v/>
       </c>
       <c r="C21" s="249" t="n">
-        <v>0.5215277777777778</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D21" s="243" t="n">
-        <v>0.6048611111111111</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="E21" s="244">
         <f>IF(C21="","",D21-C21)</f>
@@ -29411,10 +29367,10 @@
         <v/>
       </c>
       <c r="C22" s="242" t="n">
-        <v>0.3895833333333333</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="D22" s="243" t="n">
-        <v>0.55625</v>
+        <v>0.5625</v>
       </c>
       <c r="E22" s="244">
         <f>IF(C22="","",D22-C22)</f>
@@ -29450,12 +29406,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="252" t="n">
-        <v>0.3979166666666666</v>
-      </c>
-      <c r="D23" s="253" t="n">
-        <v>0.48125</v>
-      </c>
+      <c r="C23" s="252" t="n"/>
+      <c r="D23" s="253" t="n"/>
       <c r="E23" s="235">
         <f>IF(C23="","",D23-C23)</f>
         <v/>
@@ -29491,10 +29443,10 @@
         <v/>
       </c>
       <c r="C24" s="252" t="n">
-        <v>0.6777777777777778</v>
+        <v>0.6388888888888888</v>
       </c>
       <c r="D24" s="253" t="n">
-        <v>0.7611111111111111</v>
+        <v>0.7013888888888888</v>
       </c>
       <c r="E24" s="235">
         <f>IF(C24="","",D24-C24)</f>
@@ -29567,10 +29519,10 @@
         <v/>
       </c>
       <c r="C26" s="242" t="n">
-        <v>0.4847222222222222</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="D26" s="243" t="n">
-        <v>0.5263888888888889</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E26" s="244">
         <f>IF(C26="","",D26-C26)</f>
@@ -29607,10 +29559,10 @@
         <v/>
       </c>
       <c r="C27" s="249" t="n">
-        <v>0.4743055555555555</v>
+        <v>0.3402777777777778</v>
       </c>
       <c r="D27" s="243" t="n">
-        <v>0.5159722222222223</v>
+        <v>0.3819444444444444</v>
       </c>
       <c r="E27" s="244">
         <f>IF(C27="","",D27-C27)</f>
@@ -29646,8 +29598,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="249" t="n"/>
-      <c r="D28" s="243" t="n"/>
+      <c r="C28" s="249" t="n">
+        <v>0.5277777777777778</v>
+      </c>
+      <c r="D28" s="243" t="n">
+        <v>0.6388888888888888</v>
+      </c>
       <c r="E28" s="244">
         <f>IF(C28="","",D28-C28)</f>
         <v/>
@@ -29683,10 +29639,10 @@
         <v/>
       </c>
       <c r="C29" s="242" t="n">
-        <v>0.5638888888888889</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="D29" s="243" t="n">
-        <v>0.6472222222222223</v>
+        <v>0.8125</v>
       </c>
       <c r="E29" s="244">
         <f>IF(C29="","",D29-C29)</f>
@@ -29723,10 +29679,10 @@
         <v/>
       </c>
       <c r="C30" s="252" t="n">
-        <v>0.5451388888888888</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="D30" s="253" t="n">
-        <v>0.5868055555555556</v>
+        <v>0.7638888888888888</v>
       </c>
       <c r="E30" s="235">
         <f>IF(C30="","",D30-C30)</f>
@@ -29763,10 +29719,10 @@
         <v/>
       </c>
       <c r="C31" s="252" t="n">
-        <v>0.5395833333333333</v>
+        <v>0.3402777777777778</v>
       </c>
       <c r="D31" s="253" t="n">
-        <v>0.6645833333333333</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="E31" s="235">
         <f>IF(C31="","",D31-C31)</f>
@@ -29803,10 +29759,10 @@
         <v/>
       </c>
       <c r="C32" s="242" t="n">
-        <v>0.5729166666666666</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="D32" s="243" t="n">
-        <v>0.6145833333333334</v>
+        <v>0.5625</v>
       </c>
       <c r="E32" s="244">
         <f>IF(C32="","",D32-C32)</f>
@@ -29843,10 +29799,10 @@
         <v/>
       </c>
       <c r="C33" s="242" t="n">
-        <v>0.6819444444444445</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="D33" s="243" t="n">
-        <v>0.7236111111111111</v>
+        <v>0.5</v>
       </c>
       <c r="E33" s="244">
         <f>IF(C33="","",D33-C33)</f>
@@ -29883,10 +29839,10 @@
         <v/>
       </c>
       <c r="C34" s="249" t="n">
-        <v>0.35</v>
+        <v>0.4027777777777778</v>
       </c>
       <c r="D34" s="243" t="n">
-        <v>0.4333333333333333</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E34" s="244">
         <f>IF(C34="","",D34-C34)</f>
@@ -29922,8 +29878,12 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="249" t="n"/>
-      <c r="D35" s="243" t="n"/>
+      <c r="C35" s="249" t="n">
+        <v>0.6180555555555556</v>
+      </c>
+      <c r="D35" s="243" t="n">
+        <v>0.6736111111111112</v>
+      </c>
       <c r="E35" s="244">
         <f>IF(C35="","",D35-C35)</f>
         <v/>
@@ -29958,12 +29918,8 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="306" t="n">
-        <v>0.3569444444444445</v>
-      </c>
-      <c r="D36" s="307" t="n">
-        <v>0.6069444444444444</v>
-      </c>
+      <c r="C36" s="306" t="n"/>
+      <c r="D36" s="307" t="n"/>
       <c r="E36" s="308">
         <f>IF(C36="","",D36-C36)</f>
         <v/>
@@ -31204,10 +31160,10 @@
         <v/>
       </c>
       <c r="C7" s="315" t="n">
-        <v>0.6430555555555556</v>
+        <v>0.7708333333333334</v>
       </c>
       <c r="D7" s="316" t="n">
-        <v>0.6847222222222222</v>
+        <v>0.8125</v>
       </c>
       <c r="E7" s="296">
         <f>IF(C7="","",D7-C7)</f>
@@ -31245,10 +31201,10 @@
         <v/>
       </c>
       <c r="C8" s="252" t="n">
-        <v>0.7027777777777777</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="D8" s="253" t="n">
-        <v>0.7861111111111111</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="E8" s="235">
         <f>IF(C8="","",D8-C8)</f>
@@ -31285,12 +31241,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="242" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="D9" s="243" t="n">
-        <v>0.7833333333333333</v>
-      </c>
+      <c r="C9" s="242" t="n"/>
+      <c r="D9" s="243" t="n"/>
       <c r="E9" s="244">
         <f>IF(C9="","",D9-C9)</f>
         <v/>
@@ -31327,10 +31279,10 @@
         <v/>
       </c>
       <c r="C10" s="242" t="n">
-        <v>0.7347222222222223</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="D10" s="243" t="n">
-        <v>0.7763888888888889</v>
+        <v>0.8194444444444444</v>
       </c>
       <c r="E10" s="244">
         <f>IF(C10="","",D10-C10)</f>
@@ -31367,12 +31319,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="249" t="n">
-        <v>0.3541666666666667</v>
-      </c>
-      <c r="D11" s="243" t="n">
-        <v>0.4791666666666667</v>
-      </c>
+      <c r="C11" s="249" t="n"/>
+      <c r="D11" s="243" t="n"/>
       <c r="E11" s="244">
         <f>IF(C11="","",D11-C11)</f>
         <v/>
@@ -31408,12 +31356,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="249" t="n">
-        <v>0.6784722222222223</v>
-      </c>
-      <c r="D12" s="243" t="n">
-        <v>0.7618055555555555</v>
-      </c>
+      <c r="C12" s="249" t="n"/>
+      <c r="D12" s="243" t="n"/>
       <c r="E12" s="244">
         <f>IF(C12="","",D12-C12)</f>
         <v/>
@@ -31449,8 +31393,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="242" t="n"/>
-      <c r="D13" s="243" t="n"/>
+      <c r="C13" s="242" t="n">
+        <v>0.4722222222222222</v>
+      </c>
+      <c r="D13" s="243" t="n">
+        <v>0.5833333333333334</v>
+      </c>
       <c r="E13" s="244">
         <f>IF(C13="","",D13-C13)</f>
         <v/>
@@ -31486,8 +31434,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="252" t="n"/>
-      <c r="D14" s="253" t="n"/>
+      <c r="C14" s="252" t="n">
+        <v>0.6944444444444444</v>
+      </c>
+      <c r="D14" s="253" t="n">
+        <v>0.7222222222222222</v>
+      </c>
       <c r="E14" s="235">
         <f>IF(C14="","",D14-C14)</f>
         <v/>
@@ -31524,10 +31476,10 @@
         <v/>
       </c>
       <c r="C15" s="252" t="n">
-        <v>0.6229166666666667</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="D15" s="253" t="n">
-        <v>0.7895833333333333</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E15" s="235">
         <f>IF(C15="","",D15-C15)</f>
@@ -31565,10 +31517,10 @@
         <v/>
       </c>
       <c r="C16" s="242" t="n">
-        <v>0.6173611111111111</v>
+        <v>0.6527777777777778</v>
       </c>
       <c r="D16" s="243" t="n">
-        <v>0.6590277777777778</v>
+        <v>0.6805555555555556</v>
       </c>
       <c r="E16" s="244">
         <f>IF(C16="","",D16-C16)</f>
@@ -31606,10 +31558,10 @@
         <v/>
       </c>
       <c r="C17" s="242" t="n">
-        <v>0.5527777777777778</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="D17" s="243" t="n">
-        <v>0.5944444444444444</v>
+        <v>0.6875</v>
       </c>
       <c r="E17" s="244">
         <f>IF(C17="","",D17-C17)</f>
@@ -31647,10 +31599,10 @@
         <v/>
       </c>
       <c r="C18" s="249" t="n">
-        <v>0.4625</v>
+        <v>0.5763888888888888</v>
       </c>
       <c r="D18" s="243" t="n">
-        <v>0.6708333333333333</v>
+        <v>0.6180555555555556</v>
       </c>
       <c r="E18" s="244">
         <f>IF(C18="","",D18-C18)</f>
@@ -31688,10 +31640,10 @@
         <v/>
       </c>
       <c r="C19" s="249" t="n">
-        <v>0.3979166666666666</v>
+        <v>0.7708333333333334</v>
       </c>
       <c r="D19" s="243" t="n">
-        <v>0.4395833333333333</v>
+        <v>0.7986111111111112</v>
       </c>
       <c r="E19" s="244">
         <f>IF(C19="","",D19-C19)</f>
@@ -31729,10 +31681,10 @@
         <v/>
       </c>
       <c r="C20" s="242" t="n">
-        <v>0.4284722222222222</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="D20" s="243" t="n">
-        <v>0.4701388888888889</v>
+        <v>0.7569444444444444</v>
       </c>
       <c r="E20" s="244">
         <f>IF(C20="","",D20-C20)</f>
@@ -31770,10 +31722,10 @@
         <v/>
       </c>
       <c r="C21" s="252" t="n">
-        <v>0.5430555555555555</v>
+        <v>0.3680555555555556</v>
       </c>
       <c r="D21" s="253" t="n">
-        <v>0.5847222222222223</v>
+        <v>0.4375</v>
       </c>
       <c r="E21" s="235">
         <f>IF(C21="","",D21-C21)</f>
@@ -31810,12 +31762,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="252" t="n">
-        <v>0.4715277777777778</v>
-      </c>
-      <c r="D22" s="253" t="n">
-        <v>0.7215277777777778</v>
-      </c>
+      <c r="C22" s="252" t="n"/>
+      <c r="D22" s="253" t="n"/>
       <c r="E22" s="235">
         <f>IF(C22="","",D22-C22)</f>
         <v/>
@@ -31851,12 +31799,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="242" t="n">
-        <v>0.4409722222222222</v>
-      </c>
-      <c r="D23" s="243" t="n">
-        <v>0.5243055555555556</v>
-      </c>
+      <c r="C23" s="242" t="n"/>
+      <c r="D23" s="243" t="n"/>
       <c r="E23" s="244">
         <f>IF(C23="","",D23-C23)</f>
         <v/>
@@ -31893,10 +31837,10 @@
         <v/>
       </c>
       <c r="C24" s="242" t="n">
-        <v>0.7131944444444445</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="D24" s="243" t="n">
-        <v>0.7965277777777777</v>
+        <v>0.6875</v>
       </c>
       <c r="E24" s="244">
         <f>IF(C24="","",D24-C24)</f>
@@ -31933,12 +31877,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="249" t="n">
-        <v>0.4618055555555556</v>
-      </c>
-      <c r="D25" s="243" t="n">
-        <v>0.5034722222222222</v>
-      </c>
+      <c r="C25" s="249" t="n"/>
+      <c r="D25" s="243" t="n"/>
       <c r="E25" s="244">
         <f>IF(C25="","",D25-C25)</f>
         <v/>
@@ -31975,10 +31915,10 @@
         <v/>
       </c>
       <c r="C26" s="249" t="n">
-        <v>0.775</v>
+        <v>0.7291666666666666</v>
       </c>
       <c r="D26" s="243" t="n">
-        <v>0.8166666666666667</v>
+        <v>0.7708333333333334</v>
       </c>
       <c r="E26" s="244">
         <f>IF(C26="","",D26-C26)</f>
@@ -32016,10 +31956,10 @@
         <v/>
       </c>
       <c r="C27" s="242" t="n">
-        <v>0.4354166666666667</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="D27" s="243" t="n">
-        <v>0.4770833333333334</v>
+        <v>0.6736111111111112</v>
       </c>
       <c r="E27" s="244">
         <f>IF(C27="","",D27-C27)</f>
@@ -32057,10 +31997,10 @@
         <v/>
       </c>
       <c r="C28" s="252" t="n">
-        <v>0.4409722222222222</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="D28" s="253" t="n">
-        <v>0.5659722222222222</v>
+        <v>0.6319444444444444</v>
       </c>
       <c r="E28" s="235">
         <f>IF(C28="","",D28-C28)</f>
@@ -32097,8 +32037,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="252" t="n"/>
-      <c r="D29" s="253" t="n"/>
+      <c r="C29" s="252" t="n">
+        <v>0.5277777777777778</v>
+      </c>
+      <c r="D29" s="253" t="n">
+        <v>0.6319444444444444</v>
+      </c>
       <c r="E29" s="235">
         <f>IF(C29="","",D29-C29)</f>
         <v/>
@@ -32134,12 +32078,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="242" t="n">
-        <v>0.6604166666666667</v>
-      </c>
-      <c r="D30" s="243" t="n">
-        <v>0.74375</v>
-      </c>
+      <c r="C30" s="242" t="n"/>
+      <c r="D30" s="243" t="n"/>
       <c r="E30" s="244">
         <f>IF(C30="","",D30-C30)</f>
         <v/>
@@ -32175,8 +32115,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="242" t="n"/>
-      <c r="D31" s="243" t="n"/>
+      <c r="C31" s="242" t="n">
+        <v>0.5902777777777778</v>
+      </c>
+      <c r="D31" s="243" t="n">
+        <v>0.7777777777777778</v>
+      </c>
       <c r="E31" s="244">
         <f>IF(C31="","",D31-C31)</f>
         <v/>
@@ -32213,10 +32157,10 @@
         <v/>
       </c>
       <c r="C32" s="249" t="n">
-        <v>0.3722222222222222</v>
+        <v>0.6736111111111112</v>
       </c>
       <c r="D32" s="243" t="n">
-        <v>0.4555555555555555</v>
+        <v>0.7847222222222222</v>
       </c>
       <c r="E32" s="244">
         <f>IF(C32="","",D32-C32)</f>
@@ -32254,10 +32198,10 @@
         <v/>
       </c>
       <c r="C33" s="249" t="n">
-        <v>0.5666666666666667</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="D33" s="243" t="n">
-        <v>0.6083333333333333</v>
+        <v>0.6736111111111112</v>
       </c>
       <c r="E33" s="244">
         <f>IF(C33="","",D33-C33)</f>
@@ -32295,10 +32239,10 @@
         <v/>
       </c>
       <c r="C34" s="242" t="n">
-        <v>0.4965277777777778</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="D34" s="243" t="n">
-        <v>0.6215277777777778</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E34" s="244">
         <f>IF(C34="","",D34-C34)</f>
@@ -32335,8 +32279,12 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="252" t="n"/>
-      <c r="D35" s="253" t="n"/>
+      <c r="C35" s="252" t="n">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="D35" s="253" t="n">
+        <v>0.6041666666666666</v>
+      </c>
       <c r="E35" s="235">
         <f>IF(C35="","",D35-C35)</f>
         <v/>
@@ -32372,12 +32320,8 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="252" t="n">
-        <v>0.4291666666666666</v>
-      </c>
-      <c r="D36" s="253" t="n">
-        <v>0.4708333333333333</v>
-      </c>
+      <c r="C36" s="252" t="n"/>
+      <c r="D36" s="253" t="n"/>
       <c r="E36" s="235">
         <f>IF(C36="","",D36-C36)</f>
         <v/>
@@ -32413,12 +32357,8 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="256" t="n">
-        <v>0.5673611111111111</v>
-      </c>
-      <c r="D37" s="257" t="n">
-        <v>0.6923611111111111</v>
-      </c>
+      <c r="C37" s="256" t="n"/>
+      <c r="D37" s="257" t="n"/>
       <c r="E37" s="258">
         <f>IF(C37="","",D37-C37)</f>
         <v/>
@@ -33146,10 +33086,10 @@
         <v/>
       </c>
       <c r="C7" s="345" t="n">
-        <v>0.4638888888888889</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="D7" s="346" t="n">
-        <v>0.5055555555555555</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E7" s="292">
         <f>IF(C7="","",D7-C7)</f>
@@ -33186,10 +33126,10 @@
         <v/>
       </c>
       <c r="C8" s="249" t="n">
-        <v>0.7513888888888889</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="D8" s="243" t="n">
-        <v>0.7930555555555555</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E8" s="244">
         <f>IF(C8="","",D8-C8)</f>
@@ -33226,10 +33166,10 @@
         <v/>
       </c>
       <c r="C9" s="249" t="n">
-        <v>0.4034722222222222</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="D9" s="243" t="n">
-        <v>0.4451388888888889</v>
+        <v>0.5625</v>
       </c>
       <c r="E9" s="244">
         <f>IF(C9="","",D9-C9)</f>
@@ -33266,10 +33206,10 @@
         <v/>
       </c>
       <c r="C10" s="242" t="n">
-        <v>0.3965277777777778</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="D10" s="243" t="n">
-        <v>0.4381944444444444</v>
+        <v>0.7708333333333334</v>
       </c>
       <c r="E10" s="244">
         <f>IF(C10="","",D10-C10)</f>
@@ -33342,10 +33282,10 @@
         <v/>
       </c>
       <c r="C12" s="252" t="n">
-        <v>0.5069444444444444</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="D12" s="253" t="n">
-        <v>0.6736111111111112</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E12" s="235">
         <f>IF(C12="","",D12-C12)</f>
@@ -33382,10 +33322,10 @@
         <v/>
       </c>
       <c r="C13" s="242" t="n">
-        <v>0.3965277777777778</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="D13" s="243" t="n">
-        <v>0.6048611111111111</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E13" s="244">
         <f>IF(C13="","",D13-C13)</f>
@@ -33421,8 +33361,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="242" t="n"/>
-      <c r="D14" s="243" t="n"/>
+      <c r="C14" s="242" t="n">
+        <v>0.3541666666666667</v>
+      </c>
+      <c r="D14" s="243" t="n">
+        <v>0.4652777777777778</v>
+      </c>
       <c r="E14" s="244">
         <f>IF(C14="","",D14-C14)</f>
         <v/>
@@ -33458,10 +33402,10 @@
         <v/>
       </c>
       <c r="C15" s="249" t="n">
-        <v>0.5861111111111111</v>
+        <v>0.5</v>
       </c>
       <c r="D15" s="243" t="n">
-        <v>0.6277777777777778</v>
+        <v>0.6319444444444444</v>
       </c>
       <c r="E15" s="244">
         <f>IF(C15="","",D15-C15)</f>
@@ -33534,10 +33478,10 @@
         <v/>
       </c>
       <c r="C17" s="242" t="n">
-        <v>0.5236111111111111</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="D17" s="243" t="n">
-        <v>0.6069444444444444</v>
+        <v>0.5972222222222222</v>
       </c>
       <c r="E17" s="244">
         <f>IF(C17="","",D17-C17)</f>
@@ -33574,10 +33518,10 @@
         <v/>
       </c>
       <c r="C18" s="252" t="n">
-        <v>0.5520833333333334</v>
+        <v>0.75</v>
       </c>
       <c r="D18" s="253" t="n">
-        <v>0.6354166666666666</v>
+        <v>0.8125</v>
       </c>
       <c r="E18" s="235">
         <f>IF(C18="","",D18-C18)</f>
@@ -33613,12 +33557,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="252" t="n">
-        <v>0.5368055555555555</v>
-      </c>
-      <c r="D19" s="253" t="n">
-        <v>0.6618055555555555</v>
-      </c>
+      <c r="C19" s="252" t="n"/>
+      <c r="D19" s="253" t="n"/>
       <c r="E19" s="235">
         <f>IF(C19="","",D19-C19)</f>
         <v/>
@@ -33654,10 +33594,10 @@
         <v/>
       </c>
       <c r="C20" s="242" t="n">
-        <v>0.6659722222222222</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="D20" s="243" t="n">
-        <v>0.8326388888888889</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E20" s="244">
         <f>IF(C20="","",D20-C20)</f>
@@ -33694,10 +33634,10 @@
         <v/>
       </c>
       <c r="C21" s="242" t="n">
-        <v>0.6868055555555556</v>
+        <v>0.6805555555555556</v>
       </c>
       <c r="D21" s="243" t="n">
-        <v>0.8118055555555556</v>
+        <v>0.7013888888888888</v>
       </c>
       <c r="E21" s="244">
         <f>IF(C21="","",D21-C21)</f>
@@ -33733,8 +33673,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="249" t="n"/>
-      <c r="D22" s="243" t="n"/>
+      <c r="C22" s="249" t="n">
+        <v>0.5694444444444444</v>
+      </c>
+      <c r="D22" s="243" t="n">
+        <v>0.5902777777777778</v>
+      </c>
       <c r="E22" s="244">
         <f>IF(C22="","",D22-C22)</f>
         <v/>
@@ -33770,10 +33714,10 @@
         <v/>
       </c>
       <c r="C23" s="249" t="n">
-        <v>0.4131944444444444</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="D23" s="243" t="n">
-        <v>0.6631944444444444</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E23" s="244">
         <f>IF(C23="","",D23-C23)</f>
@@ -33845,8 +33789,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="252" t="n"/>
-      <c r="D25" s="253" t="n"/>
+      <c r="C25" s="252" t="n">
+        <v>0.3472222222222222</v>
+      </c>
+      <c r="D25" s="253" t="n">
+        <v>0.5347222222222222</v>
+      </c>
       <c r="E25" s="235">
         <f>IF(C25="","",D25-C25)</f>
         <v/>
@@ -33882,10 +33830,10 @@
         <v/>
       </c>
       <c r="C26" s="252" t="n">
-        <v>0.6361111111111111</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="D26" s="253" t="n">
-        <v>0.6777777777777778</v>
+        <v>0.6180555555555556</v>
       </c>
       <c r="E26" s="235">
         <f>IF(C26="","",D26-C26)</f>
@@ -33921,8 +33869,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="242" t="n"/>
-      <c r="D27" s="243" t="n"/>
+      <c r="C27" s="242" t="n">
+        <v>0.5138888888888888</v>
+      </c>
+      <c r="D27" s="243" t="n">
+        <v>0.5347222222222222</v>
+      </c>
       <c r="E27" s="244">
         <f>IF(C27="","",D27-C27)</f>
         <v/>
@@ -33958,10 +33910,10 @@
         <v/>
       </c>
       <c r="C28" s="242" t="n">
-        <v>0.3409722222222222</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="D28" s="243" t="n">
-        <v>0.5076388888888889</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="E28" s="244">
         <f>IF(C28="","",D28-C28)</f>
@@ -33997,12 +33949,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="249" t="n">
-        <v>0.3354166666666666</v>
-      </c>
-      <c r="D29" s="243" t="n">
-        <v>0.5854166666666667</v>
-      </c>
+      <c r="C29" s="249" t="n"/>
+      <c r="D29" s="243" t="n"/>
       <c r="E29" s="244">
         <f>IF(C29="","",D29-C29)</f>
         <v/>
@@ -34038,10 +33986,10 @@
         <v/>
       </c>
       <c r="C30" s="249" t="n">
-        <v>0.4979166666666667</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="D30" s="243" t="n">
-        <v>0.5395833333333333</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="E30" s="244">
         <f>IF(C30="","",D30-C30)</f>
@@ -34078,10 +34026,10 @@
         <v/>
       </c>
       <c r="C31" s="242" t="n">
-        <v>0.7319444444444444</v>
+        <v>0.6527777777777778</v>
       </c>
       <c r="D31" s="243" t="n">
-        <v>0.7736111111111111</v>
+        <v>0.7986111111111112</v>
       </c>
       <c r="E31" s="244">
         <f>IF(C31="","",D31-C31)</f>
@@ -34118,10 +34066,10 @@
         <v/>
       </c>
       <c r="C32" s="252" t="n">
-        <v>0.7194444444444444</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="D32" s="253" t="n">
-        <v>0.7611111111111111</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="E32" s="235">
         <f>IF(C32="","",D32-C32)</f>
@@ -34157,8 +34105,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="252" t="n"/>
-      <c r="D33" s="253" t="n"/>
+      <c r="C33" s="252" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="D33" s="253" t="n">
+        <v>0.5</v>
+      </c>
       <c r="E33" s="235">
         <f>IF(C33="","",D33-C33)</f>
         <v/>
@@ -34194,10 +34146,10 @@
         <v/>
       </c>
       <c r="C34" s="242" t="n">
-        <v>0.7340277777777777</v>
+        <v>0.3402777777777778</v>
       </c>
       <c r="D34" s="243" t="n">
-        <v>0.7756944444444445</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="E34" s="244">
         <f>IF(C34="","",D34-C34)</f>
@@ -34233,12 +34185,8 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="242" t="n">
-        <v>0.6520833333333333</v>
-      </c>
-      <c r="D35" s="243" t="n">
-        <v>0.7354166666666667</v>
-      </c>
+      <c r="C35" s="242" t="n"/>
+      <c r="D35" s="243" t="n"/>
       <c r="E35" s="244">
         <f>IF(C35="","",D35-C35)</f>
         <v/>
@@ -34274,10 +34222,10 @@
         <v/>
       </c>
       <c r="C36" s="249" t="n">
-        <v>0.6298611111111111</v>
+        <v>0.6944444444444444</v>
       </c>
       <c r="D36" s="243" t="n">
-        <v>0.6715277777777777</v>
+        <v>0.7986111111111112</v>
       </c>
       <c r="E36" s="244">
         <f>IF(C36="","",D36-C36)</f>
@@ -34313,8 +34261,12 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="249" t="n"/>
-      <c r="D37" s="243" t="n"/>
+      <c r="C37" s="249" t="n">
+        <v>0.7916666666666666</v>
+      </c>
+      <c r="D37" s="243" t="n">
+        <v>0.8263888888888888</v>
+      </c>
       <c r="E37" s="244">
         <f>IF(C37="","",D37-C37)</f>
         <v/>
@@ -35066,8 +35018,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="345" t="n"/>
-      <c r="D7" s="346" t="n"/>
+      <c r="C7" s="345" t="n">
+        <v>0.4722222222222222</v>
+      </c>
+      <c r="D7" s="346" t="n">
+        <v>0.7222222222222222</v>
+      </c>
       <c r="E7" s="292">
         <f>IF(C7="","",D7-C7)</f>
         <v/>
@@ -35104,10 +35060,10 @@
         <v/>
       </c>
       <c r="C8" s="252" t="n">
-        <v>0.4416666666666667</v>
+        <v>0.3541666666666667</v>
       </c>
       <c r="D8" s="253" t="n">
-        <v>0.525</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="E8" s="235">
         <f>IF(C8="","",D8-C8)</f>
@@ -35144,10 +35100,10 @@
         <v/>
       </c>
       <c r="C9" s="252" t="n">
-        <v>0.3951388888888889</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="D9" s="253" t="n">
-        <v>0.4784722222222222</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="E9" s="235">
         <f>IF(C9="","",D9-C9)</f>
@@ -35184,10 +35140,10 @@
         <v/>
       </c>
       <c r="C10" s="242" t="n">
-        <v>0.5638888888888889</v>
+        <v>0.3611111111111111</v>
       </c>
       <c r="D10" s="243" t="n">
-        <v>0.6055555555555555</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E10" s="244">
         <f>IF(C10="","",D10-C10)</f>
@@ -35224,10 +35180,10 @@
         <v/>
       </c>
       <c r="C11" s="242" t="n">
-        <v>0.4770833333333334</v>
+        <v>0.6736111111111112</v>
       </c>
       <c r="D11" s="243" t="n">
-        <v>0.51875</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="E11" s="244">
         <f>IF(C11="","",D11-C11)</f>
@@ -35263,8 +35219,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="249" t="n"/>
-      <c r="D12" s="243" t="n"/>
+      <c r="C12" s="249" t="n">
+        <v>0.5069444444444444</v>
+      </c>
+      <c r="D12" s="243" t="n">
+        <v>0.5347222222222222</v>
+      </c>
       <c r="E12" s="244">
         <f>IF(C12="","",D12-C12)</f>
         <v/>
@@ -35299,8 +35259,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="249" t="n"/>
-      <c r="D13" s="243" t="n"/>
+      <c r="C13" s="249" t="n">
+        <v>0.7291666666666666</v>
+      </c>
+      <c r="D13" s="243" t="n">
+        <v>0.8125</v>
+      </c>
       <c r="E13" s="244">
         <f>IF(C13="","",D13-C13)</f>
         <v/>
@@ -35336,10 +35300,10 @@
         <v/>
       </c>
       <c r="C14" s="242" t="n">
-        <v>0.5097222222222222</v>
+        <v>0.6180555555555556</v>
       </c>
       <c r="D14" s="243" t="n">
-        <v>0.6763888888888889</v>
+        <v>0.6875</v>
       </c>
       <c r="E14" s="244">
         <f>IF(C14="","",D14-C14)</f>
@@ -35376,10 +35340,10 @@
         <v/>
       </c>
       <c r="C15" s="252" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.6875</v>
       </c>
       <c r="D15" s="253" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.7430555555555556</v>
       </c>
       <c r="E15" s="235">
         <f>IF(C15="","",D15-C15)</f>
@@ -35415,12 +35379,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="319" t="n">
-        <v>0.5819444444444445</v>
-      </c>
-      <c r="D16" s="320" t="n">
-        <v>0.6236111111111111</v>
-      </c>
+      <c r="C16" s="319" t="n"/>
+      <c r="D16" s="320" t="n"/>
       <c r="E16" s="235">
         <f>IF(C16="","",D16-C16)</f>
         <v/>
@@ -35455,8 +35415,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="318" t="n"/>
-      <c r="D17" s="291" t="n"/>
+      <c r="C17" s="318" t="n">
+        <v>0.5902777777777778</v>
+      </c>
+      <c r="D17" s="291" t="n">
+        <v>0.7430555555555556</v>
+      </c>
       <c r="E17" s="244">
         <f>IF(C17="","",D17-C17)</f>
         <v/>
@@ -35491,8 +35455,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="242" t="n"/>
-      <c r="D18" s="243" t="n"/>
+      <c r="C18" s="242" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="D18" s="243" t="n">
+        <v>0.6597222222222222</v>
+      </c>
       <c r="E18" s="244">
         <f>IF(C18="","",D18-C18)</f>
         <v/>
@@ -35527,8 +35495,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="249" t="n"/>
-      <c r="D19" s="243" t="n"/>
+      <c r="C19" s="249" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="D19" s="243" t="n">
+        <v>0.6805555555555556</v>
+      </c>
       <c r="E19" s="244">
         <f>IF(C19="","",D19-C19)</f>
         <v/>
@@ -35564,10 +35536,10 @@
         <v/>
       </c>
       <c r="C20" s="249" t="n">
-        <v>0.6201388888888889</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="D20" s="243" t="n">
-        <v>0.7034722222222223</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E20" s="244">
         <f>IF(C20="","",D20-C20)</f>
@@ -35603,12 +35575,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="242" t="n">
-        <v>0.5388888888888889</v>
-      </c>
-      <c r="D21" s="243" t="n">
-        <v>0.5805555555555556</v>
-      </c>
+      <c r="C21" s="242" t="n"/>
+      <c r="D21" s="243" t="n"/>
       <c r="E21" s="244">
         <f>IF(C21="","",D21-C21)</f>
         <v/>
@@ -35644,10 +35612,10 @@
         <v/>
       </c>
       <c r="C22" s="252" t="n">
-        <v>0.6236111111111111</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="D22" s="253" t="n">
-        <v>0.7902777777777777</v>
+        <v>0.7916666666666666</v>
       </c>
       <c r="E22" s="235">
         <f>IF(C22="","",D22-C22)</f>
@@ -35684,10 +35652,10 @@
         <v/>
       </c>
       <c r="C23" s="252" t="n">
-        <v>0.4416666666666667</v>
+        <v>0.5972222222222222</v>
       </c>
       <c r="D23" s="253" t="n">
-        <v>0.4833333333333333</v>
+        <v>0.6319444444444444</v>
       </c>
       <c r="E23" s="235">
         <f>IF(C23="","",D23-C23)</f>
@@ -35759,8 +35727,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="242" t="n"/>
-      <c r="D25" s="243" t="n"/>
+      <c r="C25" s="242" t="n">
+        <v>0.6388888888888888</v>
+      </c>
+      <c r="D25" s="243" t="n">
+        <v>0.7777777777777778</v>
+      </c>
       <c r="E25" s="244">
         <f>IF(C25="","",D25-C25)</f>
         <v/>
@@ -35796,10 +35768,10 @@
         <v/>
       </c>
       <c r="C26" s="249" t="n">
-        <v>0.4625</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="D26" s="243" t="n">
-        <v>0.5875</v>
+        <v>0.7361111111111112</v>
       </c>
       <c r="E26" s="244">
         <f>IF(C26="","",D26-C26)</f>
@@ -35836,10 +35808,10 @@
         <v/>
       </c>
       <c r="C27" s="249" t="n">
-        <v>0.68125</v>
+        <v>0.5138888888888888</v>
       </c>
       <c r="D27" s="243" t="n">
-        <v>0.80625</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="E27" s="244">
         <f>IF(C27="","",D27-C27)</f>
@@ -35876,10 +35848,10 @@
         <v/>
       </c>
       <c r="C28" s="242" t="n">
-        <v>0.4340277777777778</v>
+        <v>0.3958333333333333</v>
       </c>
       <c r="D28" s="243" t="n">
-        <v>0.5173611111111112</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E28" s="244">
         <f>IF(C28="","",D28-C28)</f>
@@ -35916,10 +35888,10 @@
         <v/>
       </c>
       <c r="C29" s="252" t="n">
-        <v>0.5270833333333333</v>
+        <v>0.6041666666666666</v>
       </c>
       <c r="D29" s="253" t="n">
-        <v>0.6104166666666667</v>
+        <v>0.75</v>
       </c>
       <c r="E29" s="235">
         <f>IF(C29="","",D29-C29)</f>
@@ -35956,10 +35928,10 @@
         <v/>
       </c>
       <c r="C30" s="252" t="n">
-        <v>0.5284722222222222</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="D30" s="253" t="n">
-        <v>0.5701388888888889</v>
+        <v>0.7430555555555556</v>
       </c>
       <c r="E30" s="235">
         <f>IF(C30="","",D30-C30)</f>
@@ -35995,8 +35967,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="242" t="n"/>
-      <c r="D31" s="243" t="n"/>
+      <c r="C31" s="242" t="n">
+        <v>0.3958333333333333</v>
+      </c>
+      <c r="D31" s="243" t="n">
+        <v>0.6458333333333334</v>
+      </c>
       <c r="E31" s="244">
         <f>IF(C31="","",D31-C31)</f>
         <v/>
@@ -36031,12 +36007,8 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="242" t="n">
-        <v>0.38125</v>
-      </c>
-      <c r="D32" s="243" t="n">
-        <v>0.4229166666666667</v>
-      </c>
+      <c r="C32" s="242" t="n"/>
+      <c r="D32" s="243" t="n"/>
       <c r="E32" s="244">
         <f>IF(C32="","",D32-C32)</f>
         <v/>
@@ -36072,10 +36044,10 @@
         <v/>
       </c>
       <c r="C33" s="249" t="n">
-        <v>0.3652777777777778</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="D33" s="243" t="n">
-        <v>0.4069444444444444</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E33" s="244">
         <f>IF(C33="","",D33-C33)</f>
@@ -36111,8 +36083,12 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="249" t="n"/>
-      <c r="D34" s="243" t="n"/>
+      <c r="C34" s="249" t="n">
+        <v>0.4305555555555556</v>
+      </c>
+      <c r="D34" s="243" t="n">
+        <v>0.6805555555555556</v>
+      </c>
       <c r="E34" s="244">
         <f>IF(C34="","",D34-C34)</f>
         <v/>
@@ -36183,12 +36159,8 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="351" t="n">
-        <v>0.3451388888888889</v>
-      </c>
-      <c r="D36" s="352" t="n">
-        <v>0.3868055555555556</v>
-      </c>
+      <c r="C36" s="351" t="n"/>
+      <c r="D36" s="352" t="n"/>
       <c r="E36" s="353">
         <f>IF(C36="","",D36-C36)</f>
         <v/>

</xml_diff>

<commit_message>
Change hours_each_week -> horus_each_month
Also change the corresponding code of course.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -10276,7 +10276,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D8" s="220" t="n">
-        <v>0.5965277777777778</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="E8" s="213">
         <f>IF(C8="","",D8-C8)</f>
@@ -10316,7 +10316,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D9" s="220" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="E9" s="213">
         <f>IF(C9="","",D9-C9)</f>
@@ -10396,7 +10396,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D11" s="220" t="n">
-        <v>0.4930555555555556</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E11" s="213">
         <f>IF(C11="","",D11-C11)</f>
@@ -10436,7 +10436,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D12" s="220" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E12" s="213">
         <f>IF(C12="","",D12-C12)</f>
@@ -10548,7 +10548,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D15" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E15" s="213">
         <f>IF(C15="","",D15-C15)</f>
@@ -10588,7 +10588,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D16" s="220" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E16" s="213">
         <f>IF(C16="","",D16-C16)</f>
@@ -10628,7 +10628,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D17" s="220" t="n">
-        <v>0.5</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="E17" s="213">
         <f>IF(C17="","",D17-C17)</f>
@@ -10668,7 +10668,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D18" s="220" t="n">
-        <v>0.4791666666666667</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E18" s="213">
         <f>IF(C18="","",D18-C18)</f>
@@ -10708,7 +10708,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D19" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6527777777777778</v>
       </c>
       <c r="E19" s="213">
         <f>IF(C19="","",D19-C19)</f>
@@ -10820,7 +10820,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D22" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E22" s="213">
         <f>IF(C22="","",D22-C22)</f>
@@ -10860,7 +10860,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D23" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E23" s="213">
         <f>IF(C23="","",D23-C23)</f>
@@ -10900,7 +10900,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D24" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5138888888888888</v>
       </c>
       <c r="E24" s="213">
         <f>IF(C24="","",D24-C24)</f>
@@ -10940,7 +10940,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D25" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E25" s="213">
         <f>IF(C25="","",D25-C25)</f>
@@ -10980,7 +10980,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D26" s="220" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E26" s="213">
         <f>IF(C26="","",D26-C26)</f>
@@ -11092,7 +11092,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D29" s="220" t="n">
-        <v>0.625</v>
+        <v>0.5</v>
       </c>
       <c r="E29" s="213">
         <f>IF(C29="","",D29-C29)</f>
@@ -11132,7 +11132,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D30" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E30" s="213">
         <f>IF(C30="","",D30-C30)</f>
@@ -11172,7 +11172,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D31" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="E31" s="213">
         <f>IF(C31="","",D31-C31)</f>
@@ -11212,7 +11212,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D32" s="220" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5902777777777778</v>
       </c>
       <c r="E32" s="213">
         <f>IF(C32="","",D32-C32)</f>
@@ -11252,7 +11252,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D33" s="220" t="n">
-        <v>0.4791666666666667</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E33" s="213">
         <f>IF(C33="","",D33-C33)</f>
@@ -11364,7 +11364,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D36" s="220" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E36" s="213">
         <f>IF(C36="","",D36-C36)</f>
@@ -11404,7 +11404,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D37" s="226" t="n">
-        <v>0.6590277777777778</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E37" s="227">
         <f>IF(C37="","",D37-C37)</f>
@@ -12585,7 +12585,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D8" s="220" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E8" s="213">
         <f>IF(C8="","",D8-C8)</f>
@@ -12626,7 +12626,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D9" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E9" s="213">
         <f>IF(C9="","",D9-C9)</f>
@@ -12670,7 +12670,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D10" s="220" t="n">
-        <v>0.4930555555555556</v>
+        <v>0.6458333333333334</v>
       </c>
       <c r="E10" s="213">
         <f>IF(C10="","",D10-C10)</f>
@@ -12710,7 +12710,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D11" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6041666666666666</v>
       </c>
       <c r="E11" s="213">
         <f>IF(C11="","",D11-C11)</f>
@@ -12750,7 +12750,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D12" s="220" t="n">
-        <v>0.4791666666666667</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E12" s="213">
         <f>IF(C12="","",D12-C12)</f>
@@ -12862,7 +12862,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D15" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="E15" s="213">
         <f>IF(C15="","",D15-C15)</f>
@@ -12902,7 +12902,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D16" s="220" t="n">
-        <v>0.5138888888888888</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="E16" s="213">
         <f>IF(C16="","",D16-C16)</f>
@@ -12942,7 +12942,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D17" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.6590277777777778</v>
       </c>
       <c r="E17" s="213">
         <f>IF(C17="","",D17-C17)</f>
@@ -12982,7 +12982,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D18" s="220" t="n">
-        <v>0.5138888888888888</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E18" s="213">
         <f>IF(C18="","",D18-C18)</f>
@@ -13022,7 +13022,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D19" s="220" t="n">
-        <v>0.5277777777777778</v>
+        <v>0.5347222222222222</v>
       </c>
       <c r="E19" s="213">
         <f>IF(C19="","",D19-C19)</f>
@@ -13174,7 +13174,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D23" s="220" t="n">
-        <v>0.4305555555555556</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E23" s="213">
         <f>IF(C23="","",D23-C23)</f>
@@ -13214,7 +13214,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D24" s="220" t="n">
-        <v>0.5965277777777778</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E24" s="213">
         <f>IF(C24="","",D24-C24)</f>
@@ -13254,7 +13254,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D25" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E25" s="213">
         <f>IF(C25="","",D25-C25)</f>
@@ -13294,7 +13294,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D26" s="220" t="n">
-        <v>0.5625</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E26" s="213">
         <f>IF(C26="","",D26-C26)</f>
@@ -13406,7 +13406,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D29" s="220" t="n">
-        <v>0.5138888888888888</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E29" s="213">
         <f>IF(C29="","",D29-C29)</f>
@@ -13446,7 +13446,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D30" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E30" s="213">
         <f>IF(C30="","",D30-C30)</f>
@@ -13486,7 +13486,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D31" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="E31" s="213">
         <f>IF(C31="","",D31-C31)</f>
@@ -13526,7 +13526,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D32" s="220" t="n">
-        <v>0.5625</v>
+        <v>0.4375</v>
       </c>
       <c r="E32" s="213">
         <f>IF(C32="","",D32-C32)</f>
@@ -13566,7 +13566,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D33" s="220" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="E33" s="213">
         <f>IF(C33="","",D33-C33)</f>
@@ -13678,7 +13678,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D36" s="220" t="n">
-        <v>0.5347222222222222</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E36" s="213">
         <f>IF(C36="","",D36-C36)</f>
@@ -13718,7 +13718,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D37" s="269" t="n">
-        <v>0.5965277777777778</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="E37" s="270">
         <f>IF(C37="","",D37-C37)</f>
@@ -14993,7 +14993,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D7" s="212" t="n">
-        <v>0.4375</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="E7" s="213">
         <f>IF(C7="","",D7-C7)</f>
@@ -15034,7 +15034,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D8" s="220" t="n">
-        <v>0.5069444444444444</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E8" s="213">
         <f>IF(C8="","",D8-C8)</f>
@@ -15075,7 +15075,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D9" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E9" s="213">
         <f>IF(C9="","",D9-C9)</f>
@@ -15190,7 +15190,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D12" s="220" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="E12" s="213">
         <f>IF(C12="","",D12-C12)</f>
@@ -15231,7 +15231,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D13" s="220" t="n">
-        <v>0.5486111111111112</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E13" s="213">
         <f>IF(C13="","",D13-C13)</f>
@@ -15272,7 +15272,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D14" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="E14" s="213">
         <f>IF(C14="","",D14-C14)</f>
@@ -15313,7 +15313,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D15" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E15" s="213">
         <f>IF(C15="","",D15-C15)</f>
@@ -15354,7 +15354,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D16" s="220" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="E16" s="213">
         <f>IF(C16="","",D16-C16)</f>
@@ -15469,7 +15469,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D19" s="220" t="n">
-        <v>0.5486111111111112</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E19" s="213">
         <f>IF(C19="","",D19-C19)</f>
@@ -15510,7 +15510,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D20" s="220" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E20" s="213">
         <f>IF(C20="","",D20-C20)</f>
@@ -15551,7 +15551,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D21" s="220" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.6381944444444444</v>
       </c>
       <c r="E21" s="213">
         <f>IF(C21="","",D21-C21)</f>
@@ -15592,7 +15592,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D22" s="220" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.5347222222222222</v>
       </c>
       <c r="E22" s="213">
         <f>IF(C22="","",D22-C22)</f>
@@ -15633,7 +15633,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D23" s="220" t="n">
-        <v>0.5625</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E23" s="213">
         <f>IF(C23="","",D23-C23)</f>
@@ -15748,7 +15748,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D26" s="220" t="n">
-        <v>0.5902777777777778</v>
+        <v>0.4375</v>
       </c>
       <c r="E26" s="213">
         <f>IF(C26="","",D26-C26)</f>
@@ -15789,7 +15789,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D27" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="E27" s="213">
         <f>IF(C27="","",D27-C27)</f>
@@ -15830,7 +15830,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D28" s="220" t="n">
-        <v>0.5347222222222222</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E28" s="213">
         <f>IF(C28="","",D28-C28)</f>
@@ -15871,7 +15871,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D29" s="220" t="n">
-        <v>0.4930555555555556</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E29" s="213">
         <f>IF(C29="","",D29-C29)</f>
@@ -15912,7 +15912,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D30" s="220" t="n">
-        <v>0.5069444444444444</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E30" s="213">
         <f>IF(C30="","",D30-C30)</f>
@@ -16027,7 +16027,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D33" s="220" t="n">
-        <v>0.5625</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E33" s="213">
         <f>IF(C33="","",D33-C33)</f>
@@ -16068,7 +16068,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D34" s="220" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.4375</v>
       </c>
       <c r="E34" s="213">
         <f>IF(C34="","",D34-C34)</f>
@@ -16150,7 +16150,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D36" s="226" t="n">
-        <v>0.5347222222222222</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E36" s="227">
         <f>IF(C36="","",D36-C36)</f>
@@ -17119,7 +17119,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D7" s="278" t="n">
-        <v>0.4375</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E7" s="259">
         <f>IF(C7="","",D7-C7)</f>
@@ -17231,7 +17231,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D10" s="220" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.4375</v>
       </c>
       <c r="E10" s="213">
         <f>IF(C10="","",D10-C10)</f>
@@ -17271,7 +17271,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D11" s="220" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E11" s="213">
         <f>IF(C11="","",D11-C11)</f>
@@ -17311,7 +17311,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D12" s="220" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5</v>
       </c>
       <c r="E12" s="213">
         <f>IF(C12="","",D12-C12)</f>
@@ -17351,7 +17351,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D13" s="220" t="n">
-        <v>0.625</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="E13" s="213">
         <f>IF(C13="","",D13-C13)</f>
@@ -17391,7 +17391,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D14" s="220" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E14" s="213">
         <f>IF(C14="","",D14-C14)</f>
@@ -17503,7 +17503,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D17" s="212" t="n">
-        <v>0.4791666666666667</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E17" s="213">
         <f>IF(C17="","",D17-C17)</f>
@@ -17543,7 +17543,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D18" s="220" t="n">
-        <v>0.4791666666666667</v>
+        <v>0.5763888888888888</v>
       </c>
       <c r="E18" s="213">
         <f>IF(C18="","",D18-C18)</f>
@@ -17583,7 +17583,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D19" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E19" s="213">
         <f>IF(C19="","",D19-C19)</f>
@@ -17623,7 +17623,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D20" s="220" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E20" s="213">
         <f>IF(C20="","",D20-C20)</f>
@@ -17663,7 +17663,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D21" s="220" t="n">
-        <v>0.4930555555555556</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E21" s="213">
         <f>IF(C21="","",D21-C21)</f>
@@ -17775,7 +17775,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D24" s="220" t="n">
-        <v>0.4375</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E24" s="213">
         <f>IF(C24="","",D24-C24)</f>
@@ -17815,7 +17815,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D25" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E25" s="213">
         <f>IF(C25="","",D25-C25)</f>
@@ -17855,7 +17855,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D26" s="220" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E26" s="213">
         <f>IF(C26="","",D26-C26)</f>
@@ -17895,7 +17895,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D27" s="220" t="n">
-        <v>0.5763888888888888</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E27" s="213">
         <f>IF(C27="","",D27-C27)</f>
@@ -17935,7 +17935,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D28" s="220" t="n">
-        <v>0.5486111111111112</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E28" s="213">
         <f>IF(C28="","",D28-C28)</f>
@@ -18051,7 +18051,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D31" s="220" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="E31" s="213">
         <f>IF(C31="","",D31-C31)</f>
@@ -18095,7 +18095,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D32" s="220" t="n">
-        <v>0.5902777777777778</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E32" s="213">
         <f>IF(C32="","",D32-C32)</f>
@@ -18139,7 +18139,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D33" s="220" t="n">
-        <v>0.5</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="E33" s="213">
         <f>IF(C33="","",D33-C33)</f>
@@ -18179,7 +18179,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D34" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.6381944444444444</v>
       </c>
       <c r="E34" s="213">
         <f>IF(C34="","",D34-C34)</f>
@@ -18219,7 +18219,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D35" s="220" t="n">
-        <v>0.4375</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="E35" s="213">
         <f>IF(C35="","",D35-C35)</f>
@@ -19059,7 +19059,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D7" s="212" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E7" s="259">
         <f>IF(C7="","",D7-C7)</f>
@@ -19100,7 +19100,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D8" s="220" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.5965277777777778</v>
       </c>
       <c r="E8" s="213">
         <f>IF(C8="","",D8-C8)</f>
@@ -19141,7 +19141,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D9" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.6173611111111111</v>
       </c>
       <c r="E9" s="213">
         <f>IF(C9="","",D9-C9)</f>
@@ -19256,7 +19256,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D12" s="220" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="E12" s="213">
         <f>IF(C12="","",D12-C12)</f>
@@ -19297,7 +19297,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D13" s="220" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E13" s="213">
         <f>IF(C13="","",D13-C13)</f>
@@ -19338,7 +19338,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D14" s="220" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E14" s="213">
         <f>IF(C14="","",D14-C14)</f>
@@ -19379,7 +19379,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D15" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.5</v>
       </c>
       <c r="E15" s="213">
         <f>IF(C15="","",D15-C15)</f>
@@ -19420,7 +19420,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D16" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E16" s="213">
         <f>IF(C16="","",D16-C16)</f>
@@ -19535,7 +19535,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D19" s="220" t="n">
-        <v>0.5625</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E19" s="213">
         <f>IF(C19="","",D19-C19)</f>
@@ -19576,7 +19576,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D20" s="220" t="n">
-        <v>0.5965277777777778</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E20" s="213">
         <f>IF(C20="","",D20-C20)</f>
@@ -19617,7 +19617,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D21" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="E21" s="213">
         <f>IF(C21="","",D21-C21)</f>
@@ -19658,7 +19658,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D22" s="220" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E22" s="213">
         <f>IF(C22="","",D22-C22)</f>
@@ -19699,7 +19699,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D23" s="220" t="n">
-        <v>0.6173611111111111</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E23" s="213">
         <f>IF(C23="","",D23-C23)</f>
@@ -19816,7 +19816,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D26" s="220" t="n">
-        <v>0.5347222222222222</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E26" s="213">
         <f>IF(C26="","",D26-C26)</f>
@@ -19857,7 +19857,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D27" s="220" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E27" s="213">
         <f>IF(C27="","",D27-C27)</f>
@@ -19898,7 +19898,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D28" s="220" t="n">
-        <v>0.6590277777777778</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E28" s="213">
         <f>IF(C28="","",D28-C28)</f>
@@ -19980,7 +19980,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D30" s="220" t="n">
-        <v>0.5486111111111112</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E30" s="213">
         <f>IF(C30="","",D30-C30)</f>
@@ -20095,7 +20095,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D33" s="220" t="n">
-        <v>0.625</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="E33" s="213">
         <f>IF(C33="","",D33-C33)</f>
@@ -20136,7 +20136,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D34" s="262" t="n">
-        <v>0.5208333333333334</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E34" s="263">
         <f>IF(C34="","",D34-C34)</f>
@@ -21310,7 +21310,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D7" s="212" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6173611111111111</v>
       </c>
       <c r="E7" s="213">
         <f>IF(C7="","",D7-C7)</f>
@@ -21351,7 +21351,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D8" s="220" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="E8" s="213">
         <f>IF(C8="","",D8-C8)</f>
@@ -21392,7 +21392,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D9" s="220" t="n">
-        <v>0.6041666666666666</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="E9" s="213">
         <f>IF(C9="","",D9-C9)</f>
@@ -21507,7 +21507,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D12" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E12" s="213">
         <f>IF(C12="","",D12-C12)</f>
@@ -21548,7 +21548,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D13" s="220" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.5347222222222222</v>
       </c>
       <c r="E13" s="213">
         <f>IF(C13="","",D13-C13)</f>
@@ -21589,7 +21589,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D14" s="220" t="n">
-        <v>0.5208333333333334</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E14" s="213">
         <f>IF(C14="","",D14-C14)</f>
@@ -21634,7 +21634,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D15" s="220" t="n">
-        <v>0.4791666666666667</v>
+        <v>0.6381944444444444</v>
       </c>
       <c r="E15" s="213">
         <f>IF(C15="","",D15-C15)</f>
@@ -21675,7 +21675,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D16" s="220" t="n">
-        <v>0.6458333333333334</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E16" s="213">
         <f>IF(C16="","",D16-C16)</f>
@@ -21790,7 +21790,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D19" s="220" t="n">
-        <v>0.6041666666666666</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E19" s="213">
         <f>IF(C19="","",D19-C19)</f>
@@ -21831,7 +21831,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D20" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E20" s="213">
         <f>IF(C20="","",D20-C20)</f>
@@ -21872,7 +21872,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D21" s="220" t="n">
-        <v>0.5416666666666666</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="E21" s="213">
         <f>IF(C21="","",D21-C21)</f>
@@ -21913,7 +21913,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D22" s="220" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.5</v>
       </c>
       <c r="E22" s="213">
         <f>IF(C22="","",D22-C22)</f>
@@ -21954,7 +21954,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D23" s="220" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.6381944444444444</v>
       </c>
       <c r="E23" s="213">
         <f>IF(C23="","",D23-C23)</f>
@@ -22110,7 +22110,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D27" s="220" t="n">
-        <v>0.5763888888888888</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E27" s="213">
         <f>IF(C27="","",D27-C27)</f>
@@ -22151,7 +22151,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D28" s="220" t="n">
-        <v>0.5277777777777778</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E28" s="213">
         <f>IF(C28="","",D28-C28)</f>
@@ -22192,7 +22192,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D29" s="220" t="n">
-        <v>0.5069444444444444</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="E29" s="213">
         <f>IF(C29="","",D29-C29)</f>
@@ -22233,7 +22233,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D30" s="220" t="n">
-        <v>0.5486111111111112</v>
+        <v>0.5416666666666666</v>
       </c>
       <c r="E30" s="213">
         <f>IF(C30="","",D30-C30)</f>
@@ -22348,7 +22348,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D33" s="220" t="n">
-        <v>0.5486111111111112</v>
+        <v>0.5138888888888888</v>
       </c>
       <c r="E33" s="213">
         <f>IF(C33="","",D33-C33)</f>
@@ -22389,7 +22389,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D34" s="220" t="n">
-        <v>0.5625</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E34" s="213">
         <f>IF(C34="","",D34-C34)</f>
@@ -22430,7 +22430,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D35" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="E35" s="213">
         <f>IF(C35="","",D35-C35)</f>
@@ -22471,7 +22471,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D36" s="220" t="n">
-        <v>0.5277777777777778</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E36" s="213">
         <f>IF(C36="","",D36-C36)</f>
@@ -22512,7 +22512,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D37" s="269" t="n">
-        <v>0.6527777777777778</v>
+        <v>0.5965277777777778</v>
       </c>
       <c r="E37" s="270">
         <f>IF(C37="","",D37-C37)</f>
@@ -23762,7 +23762,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D9" s="220" t="n">
-        <v>0.5208333333333334</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E9" s="213">
         <f>IF(C9="","",D9-C9)</f>
@@ -23801,7 +23801,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D10" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.5965277777777778</v>
       </c>
       <c r="E10" s="213">
         <f>IF(C10="","",D10-C10)</f>
@@ -23840,7 +23840,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D11" s="220" t="n">
-        <v>0.5625</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E11" s="213">
         <f>IF(C11="","",D11-C11)</f>
@@ -23918,7 +23918,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D13" s="220" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.5347222222222222</v>
       </c>
       <c r="E13" s="213">
         <f>IF(C13="","",D13-C13)</f>
@@ -24035,7 +24035,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D16" s="220" t="n">
-        <v>0.5138888888888888</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E16" s="213">
         <f>IF(C16="","",D16-C16)</f>
@@ -24078,7 +24078,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D17" s="220" t="n">
-        <v>0.6173611111111111</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E17" s="213">
         <f>IF(C17="","",D17-C17)</f>
@@ -24117,7 +24117,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D18" s="220" t="n">
-        <v>0.5965277777777778</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E18" s="213">
         <f>IF(C18="","",D18-C18)</f>
@@ -24156,7 +24156,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D19" s="220" t="n">
-        <v>0.5347222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="E19" s="213">
         <f>IF(C19="","",D19-C19)</f>
@@ -24195,7 +24195,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D20" s="212" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E20" s="213">
         <f>IF(C20="","",D20-C20)</f>
@@ -24304,7 +24304,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D23" s="212" t="n">
-        <v>0.5208333333333334</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E23" s="213">
         <f>IF(C23="","",D23-C23)</f>
@@ -24343,7 +24343,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D24" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E24" s="213">
         <f>IF(C24="","",D24-C24)</f>
@@ -24382,7 +24382,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D25" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E25" s="213">
         <f>IF(C25="","",D25-C25)</f>
@@ -24421,7 +24421,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D26" s="220" t="n">
-        <v>0.5208333333333334</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E26" s="213">
         <f>IF(C26="","",D26-C26)</f>
@@ -24460,7 +24460,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D27" s="220" t="n">
-        <v>0.5277777777777778</v>
+        <v>0.6381944444444444</v>
       </c>
       <c r="E27" s="213">
         <f>IF(C27="","",D27-C27)</f>
@@ -24569,7 +24569,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D30" s="212" t="n">
-        <v>0.6527777777777778</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E30" s="213">
         <f>IF(C30="","",D30-C30)</f>
@@ -24608,7 +24608,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D31" s="220" t="n">
-        <v>0.6458333333333334</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E31" s="213">
         <f>IF(C31="","",D31-C31)</f>
@@ -24647,7 +24647,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D32" s="220" t="n">
-        <v>0.5</v>
+        <v>0.5763888888888888</v>
       </c>
       <c r="E32" s="213">
         <f>IF(C32="","",D32-C32)</f>
@@ -24725,7 +24725,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D34" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6381944444444444</v>
       </c>
       <c r="E34" s="213">
         <f>IF(C34="","",D34-C34)</f>
@@ -26025,7 +26025,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D7" s="212" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E7" s="213">
         <f>IF(C7="","",D7-C7)</f>
@@ -26070,7 +26070,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D8" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E8" s="213">
         <f>IF(C8="","",D8-C8)</f>
@@ -26111,7 +26111,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D9" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E9" s="213">
         <f>IF(C9="","",D9-C9)</f>
@@ -26151,7 +26151,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D10" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.6590277777777778</v>
       </c>
       <c r="E10" s="213">
         <f>IF(C10="","",D10-C10)</f>
@@ -26191,7 +26191,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D11" s="220" t="n">
-        <v>0.5763888888888888</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E11" s="213">
         <f>IF(C11="","",D11-C11)</f>
@@ -26303,7 +26303,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D14" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="E14" s="213">
         <f>IF(C14="","",D14-C14)</f>
@@ -26343,7 +26343,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D15" s="220" t="n">
-        <v>0.5138888888888888</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E15" s="213">
         <f>IF(C15="","",D15-C15)</f>
@@ -26383,7 +26383,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D16" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E16" s="213">
         <f>IF(C16="","",D16-C16)</f>
@@ -26423,7 +26423,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D17" s="220" t="n">
-        <v>0.5208333333333334</v>
+        <v>0.5625</v>
       </c>
       <c r="E17" s="213">
         <f>IF(C17="","",D17-C17)</f>
@@ -26463,7 +26463,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D18" s="220" t="n">
-        <v>0.5965277777777778</v>
+        <v>0.4375</v>
       </c>
       <c r="E18" s="213">
         <f>IF(C18="","",D18-C18)</f>
@@ -26575,7 +26575,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D21" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4375</v>
       </c>
       <c r="E21" s="213">
         <f>IF(C21="","",D21-C21)</f>
@@ -26615,7 +26615,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D22" s="220" t="n">
-        <v>0.5277777777777778</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E22" s="213">
         <f>IF(C22="","",D22-C22)</f>
@@ -26655,7 +26655,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D23" s="220" t="n">
-        <v>0.6381944444444444</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E23" s="213">
         <f>IF(C23="","",D23-C23)</f>
@@ -26695,7 +26695,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D24" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.6381944444444444</v>
       </c>
       <c r="E24" s="213">
         <f>IF(C24="","",D24-C24)</f>
@@ -26739,7 +26739,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D25" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E25" s="213">
         <f>IF(C25="","",D25-C25)</f>
@@ -26851,7 +26851,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D28" s="220" t="n">
-        <v>0.5763888888888888</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="E28" s="213">
         <f>IF(C28="","",D28-C28)</f>
@@ -26931,7 +26931,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D30" s="220" t="n">
-        <v>0.5965277777777778</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="E30" s="213">
         <f>IF(C30="","",D30-C30)</f>
@@ -26971,7 +26971,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D31" s="220" t="n">
-        <v>0.6041666666666666</v>
+        <v>0.6527777777777778</v>
       </c>
       <c r="E31" s="213">
         <f>IF(C31="","",D31-C31)</f>
@@ -27011,7 +27011,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D32" s="220" t="n">
-        <v>0.5</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E32" s="213">
         <f>IF(C32="","",D32-C32)</f>
@@ -27127,7 +27127,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D35" s="220" t="n">
-        <v>0.6319444444444444</v>
+        <v>0.6173611111111111</v>
       </c>
       <c r="E35" s="213">
         <f>IF(C35="","",D35-C35)</f>
@@ -27171,7 +27171,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D36" s="220" t="n">
-        <v>0.4791666666666667</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E36" s="213">
         <f>IF(C36="","",D36-C36)</f>
@@ -27211,7 +27211,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D37" s="226" t="n">
-        <v>0.5208333333333334</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E37" s="227">
         <f>IF(C37="","",D37-C37)</f>
@@ -28535,7 +28535,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D7" s="212" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E7" s="213">
         <f>IF(C7="","",D7-C7)</f>
@@ -28575,7 +28575,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D8" s="220" t="n">
-        <v>0.5</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="E8" s="213">
         <f>IF(C8="","",D8-C8)</f>
@@ -28687,7 +28687,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D11" s="220" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.6458333333333334</v>
       </c>
       <c r="E11" s="213">
         <f>IF(C11="","",D11-C11)</f>
@@ -28727,7 +28727,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D12" s="220" t="n">
-        <v>0.5208333333333334</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E12" s="213">
         <f>IF(C12="","",D12-C12)</f>
@@ -28767,7 +28767,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D13" s="220" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E13" s="213">
         <f>IF(C13="","",D13-C13)</f>
@@ -28807,7 +28807,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D14" s="220" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E14" s="213">
         <f>IF(C14="","",D14-C14)</f>
@@ -28847,7 +28847,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D15" s="220" t="n">
-        <v>0.5347222222222222</v>
+        <v>0.6527777777777778</v>
       </c>
       <c r="E15" s="213">
         <f>IF(C15="","",D15-C15)</f>
@@ -28959,7 +28959,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D18" s="220" t="n">
-        <v>0.4791666666666667</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="E18" s="213">
         <f>IF(C18="","",D18-C18)</f>
@@ -28999,7 +28999,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D19" s="220" t="n">
-        <v>0.4305555555555556</v>
+        <v>0.5347222222222222</v>
       </c>
       <c r="E19" s="213">
         <f>IF(C19="","",D19-C19)</f>
@@ -29039,7 +29039,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D20" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E20" s="213">
         <f>IF(C20="","",D20-C20)</f>
@@ -29079,7 +29079,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D21" s="220" t="n">
-        <v>0.5</v>
+        <v>0.625</v>
       </c>
       <c r="E21" s="213">
         <f>IF(C21="","",D21-C21)</f>
@@ -29119,7 +29119,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D22" s="220" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E22" s="213">
         <f>IF(C22="","",D22-C22)</f>
@@ -29231,7 +29231,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D25" s="220" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="E25" s="213">
         <f>IF(C25="","",D25-C25)</f>
@@ -29271,7 +29271,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D26" s="220" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="E26" s="213">
         <f>IF(C26="","",D26-C26)</f>
@@ -29311,7 +29311,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D27" s="220" t="n">
-        <v>0.6111111111111112</v>
+        <v>0.5208333333333334</v>
       </c>
       <c r="E27" s="213">
         <f>IF(C27="","",D27-C27)</f>
@@ -29351,7 +29351,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D28" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E28" s="213">
         <f>IF(C28="","",D28-C28)</f>
@@ -29391,7 +29391,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D29" s="220" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E29" s="213">
         <f>IF(C29="","",D29-C29)</f>
@@ -29503,7 +29503,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D32" s="220" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.6458333333333334</v>
       </c>
       <c r="E32" s="213">
         <f>IF(C32="","",D32-C32)</f>
@@ -29543,7 +29543,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D33" s="220" t="n">
-        <v>0.5763888888888888</v>
+        <v>0.4375</v>
       </c>
       <c r="E33" s="213">
         <f>IF(C33="","",D33-C33)</f>
@@ -29583,7 +29583,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D34" s="220" t="n">
-        <v>0.4791666666666667</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E34" s="213">
         <f>IF(C34="","",D34-C34)</f>
@@ -29623,7 +29623,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D35" s="220" t="n">
-        <v>0.4930555555555556</v>
+        <v>0.625</v>
       </c>
       <c r="E35" s="213">
         <f>IF(C35="","",D35-C35)</f>
@@ -29663,7 +29663,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D36" s="269" t="n">
-        <v>0.5069444444444444</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E36" s="270">
         <f>IF(C36="","",D36-C36)</f>
@@ -30982,7 +30982,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D9" s="220" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.4513888888888889</v>
       </c>
       <c r="E9" s="213">
         <f>IF(C9="","",D9-C9)</f>
@@ -31023,7 +31023,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D10" s="220" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.4375</v>
       </c>
       <c r="E10" s="213">
         <f>IF(C10="","",D10-C10)</f>
@@ -31064,7 +31064,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D11" s="220" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E11" s="213">
         <f>IF(C11="","",D11-C11)</f>
@@ -31105,7 +31105,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D12" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5965277777777778</v>
       </c>
       <c r="E12" s="213">
         <f>IF(C12="","",D12-C12)</f>
@@ -31146,7 +31146,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D13" s="220" t="n">
-        <v>0.5069444444444444</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E13" s="213">
         <f>IF(C13="","",D13-C13)</f>
@@ -31261,7 +31261,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D16" s="220" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E16" s="213">
         <f>IF(C16="","",D16-C16)</f>
@@ -31302,7 +31302,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D17" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E17" s="213">
         <f>IF(C17="","",D17-C17)</f>
@@ -31343,7 +31343,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D18" s="220" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.4375</v>
       </c>
       <c r="E18" s="213">
         <f>IF(C18="","",D18-C18)</f>
@@ -31384,7 +31384,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D19" s="220" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E19" s="213">
         <f>IF(C19="","",D19-C19)</f>
@@ -31425,7 +31425,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D20" s="220" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="E20" s="213">
         <f>IF(C20="","",D20-C20)</f>
@@ -31540,7 +31540,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D23" s="220" t="n">
-        <v>0.4305555555555556</v>
+        <v>0.5902777777777778</v>
       </c>
       <c r="E23" s="213">
         <f>IF(C23="","",D23-C23)</f>
@@ -31581,7 +31581,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D24" s="220" t="n">
-        <v>0.4375</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E24" s="213">
         <f>IF(C24="","",D24-C24)</f>
@@ -31622,7 +31622,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D25" s="220" t="n">
-        <v>0.4930555555555556</v>
+        <v>0.5277777777777778</v>
       </c>
       <c r="E25" s="213">
         <f>IF(C25="","",D25-C25)</f>
@@ -31663,7 +31663,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D26" s="220" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="E26" s="213">
         <f>IF(C26="","",D26-C26)</f>
@@ -31704,7 +31704,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D27" s="220" t="n">
-        <v>0.5965277777777778</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E27" s="213">
         <f>IF(C27="","",D27-C27)</f>
@@ -31819,7 +31819,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D30" s="220" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E30" s="213">
         <f>IF(C30="","",D30-C30)</f>
@@ -31860,7 +31860,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D31" s="220" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E31" s="213">
         <f>IF(C31="","",D31-C31)</f>
@@ -31901,7 +31901,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D32" s="220" t="n">
-        <v>0.4513888888888889</v>
+        <v>0.6590277777777778</v>
       </c>
       <c r="E32" s="213">
         <f>IF(C32="","",D32-C32)</f>
@@ -31942,7 +31942,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D33" s="220" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.625</v>
       </c>
       <c r="E33" s="213">
         <f>IF(C33="","",D33-C33)</f>
@@ -31983,7 +31983,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D34" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5069444444444444</v>
       </c>
       <c r="E34" s="213">
         <f>IF(C34="","",D34-C34)</f>
@@ -32098,7 +32098,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D37" s="226" t="n">
-        <v>0.4652777777777778</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="E37" s="227">
         <f>IF(C37="","",D37-C37)</f>
@@ -32830,7 +32830,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D7" s="278" t="n">
-        <v>0.6173611111111111</v>
+        <v>0.4375</v>
       </c>
       <c r="E7" s="259">
         <f>IF(C7="","",D7-C7)</f>
@@ -32870,7 +32870,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D8" s="220" t="n">
-        <v>0.4930555555555556</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="E8" s="213">
         <f>IF(C8="","",D8-C8)</f>
@@ -32910,7 +32910,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D9" s="220" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E9" s="213">
         <f>IF(C9="","",D9-C9)</f>
@@ -32950,7 +32950,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D10" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E10" s="213">
         <f>IF(C10="","",D10-C10)</f>
@@ -33062,7 +33062,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D13" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6173611111111111</v>
       </c>
       <c r="E13" s="213">
         <f>IF(C13="","",D13-C13)</f>
@@ -33102,7 +33102,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D14" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.4375</v>
       </c>
       <c r="E14" s="213">
         <f>IF(C14="","",D14-C14)</f>
@@ -33142,7 +33142,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D15" s="220" t="n">
-        <v>0.4375</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="E15" s="213">
         <f>IF(C15="","",D15-C15)</f>
@@ -33182,7 +33182,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D16" s="220" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E16" s="213">
         <f>IF(C16="","",D16-C16)</f>
@@ -33222,7 +33222,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D17" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5965277777777778</v>
       </c>
       <c r="E17" s="213">
         <f>IF(C17="","",D17-C17)</f>
@@ -33334,7 +33334,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D20" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E20" s="213">
         <f>IF(C20="","",D20-C20)</f>
@@ -33374,7 +33374,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D21" s="220" t="n">
-        <v>0.5694444444444444</v>
+        <v>0.4236111111111111</v>
       </c>
       <c r="E21" s="213">
         <f>IF(C21="","",D21-C21)</f>
@@ -33414,7 +33414,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D22" s="220" t="n">
-        <v>0.4513888888888889</v>
+        <v>0.4652777777777778</v>
       </c>
       <c r="E22" s="213">
         <f>IF(C22="","",D22-C22)</f>
@@ -33454,7 +33454,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D23" s="220" t="n">
-        <v>0.5347222222222222</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E23" s="213">
         <f>IF(C23="","",D23-C23)</f>
@@ -33494,7 +33494,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D24" s="220" t="n">
-        <v>0.5138888888888888</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E24" s="213">
         <f>IF(C24="","",D24-C24)</f>
@@ -33606,7 +33606,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D27" s="220" t="n">
-        <v>0.5069444444444444</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E27" s="213">
         <f>IF(C27="","",D27-C27)</f>
@@ -33646,7 +33646,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D28" s="220" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E28" s="213">
         <f>IF(C28="","",D28-C28)</f>
@@ -33686,7 +33686,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D29" s="220" t="n">
-        <v>0.5</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E29" s="213">
         <f>IF(C29="","",D29-C29)</f>
@@ -33726,7 +33726,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D30" s="220" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.4791666666666667</v>
       </c>
       <c r="E30" s="213">
         <f>IF(C30="","",D30-C30)</f>
@@ -33766,7 +33766,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D31" s="220" t="n">
-        <v>0.6319444444444444</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="E31" s="213">
         <f>IF(C31="","",D31-C31)</f>
@@ -33878,7 +33878,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D34" s="220" t="n">
-        <v>0.5486111111111112</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E34" s="213">
         <f>IF(C34="","",D34-C34)</f>
@@ -33918,7 +33918,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D35" s="220" t="n">
-        <v>0.4305555555555556</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E35" s="213">
         <f>IF(C35="","",D35-C35)</f>
@@ -33958,7 +33958,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D36" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4375</v>
       </c>
       <c r="E36" s="213">
         <f>IF(C36="","",D36-C36)</f>
@@ -33998,7 +33998,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D37" s="220" t="n">
-        <v>0.4861111111111111</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E37" s="213">
         <f>IF(C37="","",D37-C37)</f>
@@ -34755,7 +34755,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D7" s="278" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5625</v>
       </c>
       <c r="E7" s="259">
         <f>IF(C7="","",D7-C7)</f>
@@ -34868,7 +34868,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D10" s="220" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.5486111111111112</v>
       </c>
       <c r="E10" s="213">
         <f>IF(C10="","",D10-C10)</f>
@@ -34908,7 +34908,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D11" s="220" t="n">
-        <v>0.6173611111111111</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E11" s="213">
         <f>IF(C11="","",D11-C11)</f>
@@ -34948,7 +34948,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D12" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E12" s="213">
         <f>IF(C12="","",D12-C12)</f>
@@ -34988,7 +34988,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D13" s="220" t="n">
-        <v>0.4305555555555556</v>
+        <v>0.4375</v>
       </c>
       <c r="E13" s="213">
         <f>IF(C13="","",D13-C13)</f>
@@ -35028,7 +35028,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D14" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.4930555555555556</v>
       </c>
       <c r="E14" s="213">
         <f>IF(C14="","",D14-C14)</f>
@@ -35140,7 +35140,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D17" s="212" t="n">
-        <v>0.4166666666666667</v>
+        <v>0.4305555555555556</v>
       </c>
       <c r="E17" s="213">
         <f>IF(C17="","",D17-C17)</f>
@@ -35180,7 +35180,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D18" s="220" t="n">
-        <v>0.4791666666666667</v>
+        <v>0.4375</v>
       </c>
       <c r="E18" s="213">
         <f>IF(C18="","",D18-C18)</f>
@@ -35220,7 +35220,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D19" s="220" t="n">
-        <v>0.4236111111111111</v>
+        <v>0.5965277777777778</v>
       </c>
       <c r="E19" s="213">
         <f>IF(C19="","",D19-C19)</f>
@@ -35412,7 +35412,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D24" s="220" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5902777777777778</v>
       </c>
       <c r="E24" s="213">
         <f>IF(C24="","",D24-C24)</f>
@@ -35452,7 +35452,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D25" s="220" t="n">
-        <v>0.4930555555555556</v>
+        <v>0.4722222222222222</v>
       </c>
       <c r="E25" s="213">
         <f>IF(C25="","",D25-C25)</f>
@@ -35492,7 +35492,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D26" s="220" t="n">
-        <v>0.4583333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E26" s="213">
         <f>IF(C26="","",D26-C26)</f>
@@ -35532,7 +35532,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D27" s="220" t="n">
-        <v>0.4375</v>
+        <v>0.5138888888888888</v>
       </c>
       <c r="E27" s="213">
         <f>IF(C27="","",D27-C27)</f>
@@ -35572,7 +35572,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D28" s="220" t="n">
-        <v>0.6041666666666666</v>
+        <v>0.6173611111111111</v>
       </c>
       <c r="E28" s="213">
         <f>IF(C28="","",D28-C28)</f>
@@ -35684,7 +35684,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D31" s="220" t="n">
-        <v>0.4722222222222222</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E31" s="213">
         <f>IF(C31="","",D31-C31)</f>
@@ -35724,7 +35724,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D32" s="220" t="n">
-        <v>0.5277777777777778</v>
+        <v>0.5694444444444444</v>
       </c>
       <c r="E32" s="213">
         <f>IF(C32="","",D32-C32)</f>
@@ -35764,7 +35764,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D33" s="220" t="n">
-        <v>0.6381944444444444</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="E33" s="213">
         <f>IF(C33="","",D33-C33)</f>
@@ -35804,7 +35804,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D34" s="220" t="n">
-        <v>0.4375</v>
+        <v>0.6173611111111111</v>
       </c>
       <c r="E34" s="213">
         <f>IF(C34="","",D34-C34)</f>
@@ -35844,7 +35844,7 @@
         <v>0.4166666666666667</v>
       </c>
       <c r="D35" s="220" t="n">
-        <v>0.5347222222222222</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E35" s="213">
         <f>IF(C35="","",D35-C35)</f>

</xml_diff>

<commit_message>
Generate hours on a monthly bases instead of yearly
This is generally the better way to do it, because it reduceses the
spray of the hours. However, it is still not perfect and needs some
tweaking.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1114,7 +1114,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>42735</v>
+        <v>43465</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -1239,7 +1239,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.25</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -1264,9 +1264,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.1458333333333333</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -1290,9 +1288,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -1340,7 +1336,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -1364,7 +1362,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.08958333333333333</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -1389,7 +1389,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -1415,7 +1415,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.1180555555555556</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -1440,9 +1440,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -1466,9 +1464,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -1516,7 +1512,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -1540,7 +1538,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -1565,7 +1565,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -1591,7 +1591,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1944444444444444</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -1616,9 +1616,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n">
-        <v>0.05555555555555555</v>
-      </c>
+      <c r="C22" s="71" t="n"/>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -1642,9 +1640,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.1597222222222222</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -1692,7 +1688,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.05555555555555555</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -1716,7 +1714,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -1768,7 +1768,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -1794,9 +1794,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n">
-        <v>0.1527777777777778</v>
-      </c>
+      <c r="C29" s="71" t="n"/>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -1821,9 +1819,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.1388888888888889</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -1873,7 +1869,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.2361111111111111</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -1898,7 +1896,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -1924,7 +1924,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.1527777777777778</v>
+        <v>0.0625</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -1951,7 +1951,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.1875</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -1977,9 +1977,7 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n">
-        <v>0.1527777777777778</v>
-      </c>
+      <c r="C36" s="71" t="n"/>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -2004,9 +2002,7 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C37" s="73" t="n"/>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -2485,7 +2481,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43008</v>
+        <v>43738</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -2611,7 +2607,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.02083333333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -2636,9 +2632,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.0763888888888889</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -2662,9 +2656,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.1180555555555556</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -2712,7 +2704,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.1388888888888889</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -2736,7 +2730,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.1597222222222222</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -2761,7 +2757,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.1180555555555556</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -2787,7 +2783,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.02777777777777778</v>
+        <v>0.25</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -2812,9 +2808,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.1597222222222222</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -2838,9 +2832,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -2888,7 +2880,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -2912,7 +2906,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -2937,7 +2933,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.06944444444444445</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -2963,7 +2959,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.02083333333333333</v>
+        <v>0.1180555555555556</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -2988,9 +2984,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n">
-        <v>0.1041666666666667</v>
-      </c>
+      <c r="C22" s="71" t="n"/>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -3014,9 +3008,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.2291666666666667</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -3064,7 +3056,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -3088,7 +3082,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.06944444444444445</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -3113,7 +3109,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.0625</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -3140,7 +3136,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -3166,9 +3162,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n">
-        <v>0.08958333333333333</v>
-      </c>
+      <c r="C29" s="71" t="n"/>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -3193,9 +3187,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.2361111111111111</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -3245,7 +3237,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.1388888888888889</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -3270,7 +3264,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.08958333333333333</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -3296,7 +3292,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.2361111111111111</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -3323,7 +3319,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0</v>
+        <v>0.09722222222222222</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -3349,9 +3345,7 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C36" s="71" t="n"/>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -3376,9 +3370,7 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C37" s="73" t="n"/>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -3857,7 +3849,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43039</v>
+        <v>43769</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -4006,7 +3998,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.1458333333333333</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -4030,7 +4024,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.1944444444444444</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -4055,7 +4051,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.01388888888888889</v>
+        <v>0.25</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -4081,7 +4077,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.2430555555555556</v>
+        <v>0.25</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -4106,9 +4102,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.1458333333333333</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -4132,9 +4126,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.02777777777777778</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -4182,7 +4174,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -4206,7 +4200,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.0763888888888889</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -4231,7 +4227,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.25</v>
+        <v>0.09722222222222222</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -4257,7 +4253,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.2361111111111111</v>
+        <v>0.25</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -4282,9 +4278,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -4308,9 +4302,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -4358,7 +4350,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.1597222222222222</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -4382,7 +4376,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -4407,7 +4403,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -4433,7 +4429,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.1319444444444444</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -4458,9 +4454,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n">
-        <v>0.1180555555555556</v>
-      </c>
+      <c r="C26" s="73" t="n"/>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -4484,9 +4478,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n">
-        <v>0.006944444444444444</v>
-      </c>
+      <c r="C27" s="73" t="n"/>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -4536,7 +4528,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -4561,7 +4555,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -4587,7 +4583,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.006944444444444444</v>
+        <v>0.1597222222222222</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -4614,7 +4610,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.03472222222222222</v>
+        <v>0.25</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -4640,9 +4636,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C33" s="73" t="n"/>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -4667,9 +4661,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n">
-        <v>0.03472222222222222</v>
-      </c>
+      <c r="C34" s="73" t="n"/>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -4719,7 +4711,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -5223,7 +5217,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43069</v>
+        <v>43799</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -5348,7 +5342,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -5373,7 +5369,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.01388888888888889</v>
+        <v>0.25</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -5399,7 +5395,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.01388888888888889</v>
+        <v>0.08958333333333333</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -5424,9 +5420,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.06944444444444445</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -5450,9 +5444,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.1041666666666667</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -5500,7 +5492,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.1736111111111111</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -5524,7 +5518,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.1111111111111111</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -5549,7 +5545,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.25</v>
+        <v>0.2291666666666667</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -5575,7 +5571,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.125</v>
+        <v>0.04861111111111111</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -5600,9 +5596,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0.08958333333333333</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -5626,9 +5620,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.02777777777777778</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -5676,7 +5668,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.0763888888888889</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -5700,7 +5694,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -5725,7 +5721,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1798611111111111</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -5751,7 +5747,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.01388888888888889</v>
+        <v>0.25</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -5776,9 +5772,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>0.01388888888888889</v>
-      </c>
+      <c r="C24" s="71" t="n"/>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -5802,9 +5796,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.1597222222222222</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -5852,7 +5844,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.01388888888888889</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -5877,7 +5871,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.1798611111111111</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -5903,7 +5899,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.02083333333333333</v>
+        <v>0.006944444444444444</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -5929,9 +5925,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.03472222222222222</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -5956,9 +5950,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n">
-        <v>0.02777777777777778</v>
-      </c>
+      <c r="C31" s="73" t="n"/>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -5983,9 +5975,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n">
-        <v>0.1111111111111111</v>
-      </c>
+      <c r="C32" s="73" t="n"/>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -6085,9 +6075,7 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n">
-        <v>0.2430555555555556</v>
-      </c>
+      <c r="C36" s="71" t="n"/>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -6591,7 +6579,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>42766</v>
+        <v>43496</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -6740,7 +6728,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -6764,7 +6754,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.1319444444444444</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -6789,7 +6781,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.0763888888888889</v>
+        <v>0.25</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -6815,7 +6807,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.2013888888888889</v>
+        <v>0.2083333333333333</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -6840,9 +6832,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -6866,9 +6856,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.1111111111111111</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -6916,7 +6904,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.05555555555555555</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -6940,7 +6930,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.1388888888888889</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -6965,7 +6957,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.05555555555555555</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -7016,9 +7008,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.1388888888888889</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -7042,9 +7032,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.0763888888888889</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -7092,7 +7080,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.2152777777777778</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -7116,7 +7106,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.08958333333333333</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -7141,7 +7133,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.09722222222222222</v>
+        <v>0.08958333333333333</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -7167,7 +7159,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.1319444444444444</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -7192,9 +7184,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n">
-        <v>0.1458333333333333</v>
-      </c>
+      <c r="C26" s="73" t="n"/>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -7218,9 +7208,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n">
-        <v>0.2430555555555556</v>
-      </c>
+      <c r="C27" s="73" t="n"/>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -7270,7 +7258,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.1736111111111111</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -7295,7 +7285,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -7321,7 +7313,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.09722222222222222</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -7348,7 +7340,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.25</v>
+        <v>0.0763888888888889</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -7374,9 +7366,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C33" s="73" t="n"/>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -7401,9 +7391,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C34" s="73" t="n"/>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -7957,7 +7945,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>42794</v>
+        <v>43524</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -8106,7 +8094,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.2361111111111111</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -8130,7 +8120,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -8155,7 +8147,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -8181,7 +8173,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.1875</v>
+        <v>0.0763888888888889</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -8206,9 +8198,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.1736111111111111</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -8232,9 +8222,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.08958333333333333</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -8282,7 +8270,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.05555555555555555</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -8306,7 +8296,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.06944444444444445</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -8357,7 +8349,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.2430555555555556</v>
+        <v>0.25</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -8382,9 +8374,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.2291666666666667</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -8408,9 +8398,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.08958333333333333</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -8458,7 +8446,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -8482,7 +8472,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.1111111111111111</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -8533,7 +8525,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.05555555555555555</v>
+        <v>0.2430555555555556</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -8558,9 +8550,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C26" s="73" t="n"/>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -8584,9 +8574,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n">
-        <v>0.2083333333333333</v>
-      </c>
+      <c r="C27" s="73" t="n"/>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -8636,7 +8624,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -8661,7 +8651,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.04861111111111111</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -8687,7 +8679,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.2222222222222222</v>
+        <v>0.1319444444444444</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -8714,7 +8706,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.25</v>
+        <v>0.2430555555555556</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -8740,9 +8732,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n">
-        <v>0.0763888888888889</v>
-      </c>
+      <c r="C33" s="73" t="n"/>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -8767,9 +8757,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n">
-        <v>0.2083333333333333</v>
-      </c>
+      <c r="C34" s="73" t="n"/>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -8819,7 +8807,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.1180555555555556</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -8844,7 +8834,9 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n"/>
+      <c r="C37" s="73" t="n">
+        <v>0.02083333333333333</v>
+      </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -9323,7 +9315,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>42825</v>
+        <v>43555</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -9449,7 +9441,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.25</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -9475,7 +9467,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -9500,9 +9492,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.1111111111111111</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -9526,9 +9516,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.1319444444444444</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -9576,7 +9564,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -9600,7 +9590,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -9625,7 +9617,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.08958333333333333</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -9651,7 +9643,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04861111111111111</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -9676,9 +9668,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.1041666666666667</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -9702,9 +9692,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0.0763888888888889</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -9752,7 +9740,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -9776,7 +9766,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.2013888888888889</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -9801,7 +9793,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -9827,7 +9819,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.2361111111111111</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -9852,9 +9844,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -9878,9 +9868,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C24" s="71" t="n"/>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -9928,7 +9916,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.1388888888888889</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -9952,7 +9942,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.06944444444444445</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -9978,7 +9970,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.04861111111111111</v>
+        <v>0.125</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -10005,7 +9997,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.2013888888888889</v>
+        <v>0.0763888888888889</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -10031,9 +10023,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -10058,9 +10048,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C31" s="73" t="n"/>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -10110,7 +10098,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -10135,7 +10125,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -10161,7 +10153,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08958333333333333</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -10188,7 +10180,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.09722222222222222</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -10693,7 +10685,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>42855</v>
+        <v>43585</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -10818,9 +10810,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C7" s="69" t="n"/>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -10844,9 +10834,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -10894,7 +10882,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -10918,7 +10908,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -10943,7 +10935,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1798611111111111</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -10969,7 +10961,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.1180555555555556</v>
+        <v>0.1527777777777778</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -10994,9 +10986,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.09722222222222222</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -11020,9 +11010,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -11070,7 +11058,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -11094,7 +11084,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -11119,7 +11111,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -11170,9 +11162,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C21" s="71" t="n"/>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -11196,9 +11186,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C22" s="71" t="n"/>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -11246,7 +11234,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.1041666666666667</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -11270,7 +11260,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -11295,7 +11287,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.0763888888888889</v>
+        <v>0.1798611111111111</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -11321,7 +11313,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.01388888888888889</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -11347,9 +11339,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C28" s="71" t="n"/>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -11374,9 +11364,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C29" s="71" t="n"/>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -11426,7 +11414,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.1458333333333333</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -11451,7 +11441,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.01388888888888889</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -11477,7 +11469,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1180555555555556</v>
+        <v>0.1736111111111111</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -11504,7 +11496,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.02777777777777778</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -11530,9 +11522,7 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C35" s="71" t="n"/>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -11557,9 +11547,7 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C36" s="71" t="n"/>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -12063,7 +12051,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>42886</v>
+        <v>43616</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -12188,7 +12176,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -12212,7 +12202,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.2361111111111111</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -12237,7 +12229,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.1319444444444444</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -12263,7 +12255,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1527777777777778</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -12288,9 +12280,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.2013888888888889</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -12314,9 +12304,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.04861111111111111</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -12364,7 +12352,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.1180555555555556</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -12388,7 +12378,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.1319444444444444</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -12413,7 +12405,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.25</v>
+        <v>0.09722222222222222</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -12439,7 +12431,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.04861111111111111</v>
+        <v>0.25</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -12464,9 +12456,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -12490,9 +12480,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -12540,7 +12528,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.1319444444444444</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -12564,7 +12554,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -12589,7 +12581,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -12615,7 +12607,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -12640,9 +12632,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.06944444444444445</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -12666,9 +12656,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C26" s="73" t="n"/>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -12717,7 +12705,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -12742,7 +12732,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.1458333333333333</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -12768,7 +12760,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.1944444444444444</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -12795,7 +12787,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -12821,9 +12813,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n">
-        <v>0.1111111111111111</v>
-      </c>
+      <c r="C32" s="73" t="n"/>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -12848,9 +12838,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C33" s="73" t="n"/>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -12900,7 +12888,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.2013888888888889</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -12925,7 +12915,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.2013888888888889</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -13429,7 +13421,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>42916</v>
+        <v>43646</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -13555,7 +13547,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -13581,7 +13573,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -13606,9 +13598,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.2083333333333333</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -13632,9 +13622,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.2222222222222222</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -13682,7 +13670,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -13706,7 +13696,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.2013888888888889</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -13731,7 +13723,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.04861111111111111</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -13757,7 +13749,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.06944444444444445</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -13782,9 +13774,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.05555555555555555</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -13808,9 +13798,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0.0763888888888889</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -13858,7 +13846,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -13882,7 +13872,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.1458333333333333</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -13907,7 +13899,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.06944444444444445</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -13933,7 +13925,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.1388888888888889</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -13958,9 +13950,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -13984,9 +13974,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>0.06944444444444445</v>
-      </c>
+      <c r="C24" s="71" t="n"/>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -14034,7 +14022,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -14058,7 +14048,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -14084,7 +14076,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -14111,7 +14103,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.0625</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -14137,9 +14129,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.1944444444444444</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -14164,9 +14154,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C31" s="73" t="n"/>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -14216,7 +14204,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.1111111111111111</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -14241,7 +14231,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -14267,7 +14259,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.0763888888888889</v>
+        <v>0.25</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -14294,7 +14286,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.2013888888888889</v>
+        <v>0.08958333333333333</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -14320,9 +14312,7 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C37" s="73" t="n"/>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -14801,7 +14791,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>42947</v>
+        <v>43677</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -14926,9 +14916,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C7" s="69" t="n"/>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -14976,7 +14964,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -15000,7 +14990,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -15025,7 +15017,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -15051,7 +15043,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.1319444444444444</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -15076,9 +15068,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.1798611111111111</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -15102,9 +15092,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -15152,7 +15140,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -15176,7 +15166,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.0763888888888889</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -15201,7 +15193,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.1597222222222222</v>
+        <v>0.25</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -15227,7 +15219,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.05555555555555555</v>
+        <v>0.125</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -15252,9 +15244,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -15278,9 +15268,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n">
-        <v>0.2013888888888889</v>
-      </c>
+      <c r="C21" s="71" t="n"/>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -15328,7 +15316,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.06944444444444445</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -15352,7 +15342,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.1111111111111111</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -15428,9 +15420,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C27" s="73" t="n"/>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -15455,9 +15445,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n">
-        <v>0.2430555555555556</v>
-      </c>
+      <c r="C28" s="71" t="n"/>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -15507,7 +15495,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.1111111111111111</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -15532,7 +15522,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.04861111111111111</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -15558,7 +15550,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.25</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -15585,7 +15577,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.25</v>
+        <v>0.0625</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -15611,9 +15603,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C34" s="73" t="n"/>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -15638,9 +15628,7 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n">
-        <v>0.1180555555555556</v>
-      </c>
+      <c r="C35" s="71" t="n"/>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -15690,7 +15678,9 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n"/>
+      <c r="C37" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -16169,7 +16159,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>42978</v>
+        <v>43708</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -16294,7 +16284,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -16319,7 +16311,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.25</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -16345,7 +16337,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.04861111111111111</v>
+        <v>0.1319444444444444</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -16370,9 +16362,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.1319444444444444</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -16396,9 +16386,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.1111111111111111</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -16446,7 +16434,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -16470,7 +16460,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.06944444444444445</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -16495,7 +16487,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1180555555555556</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -16521,7 +16513,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.006944444444444444</v>
+        <v>0.25</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -16546,9 +16538,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -16572,9 +16562,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -16622,7 +16610,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -16646,7 +16636,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -16671,7 +16663,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -16697,7 +16689,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.0625</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -16722,9 +16714,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>0</v>
-      </c>
+      <c r="C24" s="71" t="n"/>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -16748,9 +16738,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -16798,7 +16786,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -16823,7 +16813,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -16849,7 +16841,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -16876,7 +16868,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -16902,9 +16894,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n">
-        <v>0.1041666666666667</v>
-      </c>
+      <c r="C31" s="73" t="n"/>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -16929,9 +16919,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n">
-        <v>0.25</v>
-      </c>
+      <c r="C32" s="73" t="n"/>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -16981,7 +16969,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -17006,7 +16996,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.25</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -17032,7 +17024,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.08958333333333333</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>

</xml_diff>

<commit_message>
Fix bug where min_hours wouldn't work
The bug was inside of generate_hours.decrease_hours.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1114,7 +1114,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43465</v>
+        <v>42735</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -1239,7 +1239,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -1264,7 +1264,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -1288,7 +1290,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.09375</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -1312,7 +1316,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -1337,7 +1343,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -1363,7 +1369,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.08958333333333333</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -1389,7 +1395,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -1415,7 +1421,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -1440,7 +1446,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -1464,7 +1472,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.07291666666666667</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -1488,7 +1498,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.07291666666666667</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -1513,7 +1525,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -1539,7 +1551,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -1565,7 +1577,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.125</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -1591,7 +1603,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -1616,7 +1628,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -1640,7 +1654,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.1041666666666667</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -1664,7 +1680,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -1689,7 +1707,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.05555555555555555</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -1715,7 +1733,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -1741,7 +1759,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -1768,7 +1786,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -1794,7 +1812,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -1819,7 +1839,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -1844,7 +1866,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -1870,7 +1894,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.2361111111111111</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -1897,7 +1921,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.25</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -1924,7 +1948,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -1951,7 +1975,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -1977,7 +2001,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.1145833333333333</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -2002,7 +2028,9 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n"/>
+      <c r="C37" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -2481,7 +2509,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43738</v>
+        <v>43008</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -2607,7 +2635,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.09375</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -2632,7 +2660,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -2656,7 +2686,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -2680,7 +2712,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -2705,7 +2739,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -2731,7 +2765,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.1597222222222222</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -2757,7 +2791,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -2783,7 +2817,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -2808,7 +2842,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -2832,7 +2868,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -2856,7 +2894,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -2881,7 +2921,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -2907,7 +2947,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -2933,7 +2973,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -2959,7 +2999,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1180555555555556</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -2984,7 +3024,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -3008,7 +3050,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -3032,7 +3076,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -3057,7 +3103,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -3083,7 +3129,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -3109,7 +3155,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -3136,7 +3182,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -3162,7 +3208,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -3187,7 +3235,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -3212,7 +3262,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.09375</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -3238,7 +3290,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -3265,7 +3317,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.08958333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -3292,7 +3344,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -3319,7 +3371,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.09722222222222222</v>
+        <v>0.15625</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -3345,7 +3397,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -3370,7 +3424,9 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n"/>
+      <c r="C37" s="73" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -3849,7 +3905,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43769</v>
+        <v>43039</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -3974,7 +4030,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -3999,7 +4057,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -4025,7 +4083,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.1944444444444444</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -4051,7 +4109,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.25</v>
+        <v>0.0625</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -4077,7 +4135,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -4102,7 +4160,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -4126,7 +4186,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.1145833333333333</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -4150,7 +4212,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.1145833333333333</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -4175,7 +4239,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -4201,7 +4265,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.0763888888888889</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -4227,7 +4291,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.09722222222222222</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -4253,7 +4317,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.25</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -4278,7 +4342,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.07291666666666667</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -4302,7 +4368,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -4326,7 +4394,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -4351,7 +4421,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1597222222222222</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -4377,7 +4447,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -4403,7 +4473,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -4429,7 +4499,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.1319444444444444</v>
+        <v>0.0625</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -4454,7 +4524,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -4478,7 +4550,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -4503,7 +4577,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.1458333333333333</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -4529,7 +4605,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -4556,7 +4632,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -4583,7 +4659,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.1597222222222222</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -4610,7 +4686,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -4636,7 +4712,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.1041666666666667</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -4661,7 +4739,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -4686,7 +4766,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -4712,7 +4794,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.1875</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -5217,7 +5299,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43799</v>
+        <v>43069</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -5343,7 +5425,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -5369,7 +5451,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -5395,7 +5477,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.08958333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -5420,7 +5502,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.1354166666666667</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -5444,7 +5528,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.1354166666666667</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -5468,7 +5554,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -5493,7 +5581,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.1736111111111111</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -5519,7 +5607,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -5545,7 +5633,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -5571,7 +5659,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.04861111111111111</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -5596,7 +5684,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -5620,7 +5710,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -5644,7 +5736,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -5669,7 +5763,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.0763888888888889</v>
+        <v>0.0625</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -5721,7 +5815,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1798611111111111</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -5747,7 +5841,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -5772,7 +5866,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -5796,7 +5892,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -5820,7 +5918,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -5845,7 +5945,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.01388888888888889</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -5872,7 +5972,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.1798611111111111</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -5899,7 +5999,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.006944444444444444</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -5925,7 +6025,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.09375</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -5950,7 +6052,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.09375</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -5975,7 +6079,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -6000,7 +6106,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -6025,7 +6133,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -6050,7 +6160,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -6075,7 +6187,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -6100,7 +6214,9 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n"/>
+      <c r="C37" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -6579,7 +6695,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43496</v>
+        <v>42766</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -6704,7 +6820,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -6729,7 +6847,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -6755,7 +6873,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.1319444444444444</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -6781,7 +6899,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -6807,7 +6925,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.09375</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -6832,7 +6950,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -6856,7 +6976,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -6880,7 +7002,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -6905,7 +7029,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.05555555555555555</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -6931,7 +7055,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -6957,7 +7081,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.05555555555555555</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -6983,7 +7107,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.25</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -7008,7 +7132,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -7032,7 +7158,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -7056,7 +7184,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -7081,7 +7211,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.2152777777777778</v>
+        <v>0.09375</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -7107,7 +7237,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.08958333333333333</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -7133,7 +7263,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.08958333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -7159,7 +7289,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.1319444444444444</v>
+        <v>0.0625</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -7184,7 +7314,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -7208,7 +7340,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -7233,7 +7367,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.09375</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -7259,7 +7395,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.1736111111111111</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -7313,7 +7449,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.09722222222222222</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -7340,7 +7476,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.0763888888888889</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -7366,7 +7502,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -7391,7 +7529,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -7945,7 +8085,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43524</v>
+        <v>42794</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -8070,7 +8210,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -8095,7 +8237,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.2361111111111111</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -8173,7 +8315,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.0763888888888889</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -8198,7 +8340,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -8222,7 +8366,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -8246,7 +8392,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.1354166666666667</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -8271,7 +8419,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.05555555555555555</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -8297,7 +8445,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -8323,7 +8471,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.25</v>
+        <v>0.15625</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -8349,7 +8497,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -8374,7 +8522,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -8398,7 +8548,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -8422,7 +8574,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -8447,7 +8601,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -8473,7 +8627,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -8499,7 +8653,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -8525,7 +8679,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.2430555555555556</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -8550,7 +8704,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -8574,7 +8730,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -8599,7 +8757,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -8625,7 +8785,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -8652,7 +8812,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.04861111111111111</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -8679,7 +8839,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.1319444444444444</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -8706,7 +8866,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.2430555555555556</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -8732,7 +8892,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -8757,7 +8919,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -8782,7 +8946,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.07291666666666667</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -8808,7 +8974,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.1180555555555556</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -8835,7 +9001,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.02083333333333333</v>
+        <v>0.0625</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -9315,7 +9481,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43555</v>
+        <v>42825</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -9441,7 +9607,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -9467,7 +9633,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -9492,7 +9658,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -9516,7 +9684,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -9540,7 +9710,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -9565,7 +9737,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -9591,7 +9763,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -9617,7 +9789,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -9643,7 +9815,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.04861111111111111</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -9668,7 +9840,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -9692,7 +9866,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -9716,7 +9892,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.07291666666666667</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -9741,7 +9919,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.25</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -9767,7 +9945,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.2013888888888889</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -9793,7 +9971,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.25</v>
+        <v>0.0625</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -9819,7 +9997,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -9844,7 +10022,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.1458333333333333</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -9868,7 +10048,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.1041666666666667</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -9892,7 +10074,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -9917,7 +10101,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -9943,7 +10127,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -9970,7 +10154,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.125</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -9997,7 +10181,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.0763888888888889</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -10023,7 +10207,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -10048,7 +10234,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -10073,7 +10261,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -10099,7 +10289,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -10126,7 +10316,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -10153,7 +10343,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.08958333333333333</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -10180,7 +10370,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.09722222222222222</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -10685,7 +10875,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43585</v>
+        <v>42855</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -10810,7 +11000,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -10834,7 +11026,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -10858,7 +11052,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -10883,7 +11079,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -10909,7 +11105,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -10935,7 +11131,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.1798611111111111</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -10961,7 +11157,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.1527777777777778</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -10986,7 +11182,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -11010,7 +11208,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.1145833333333333</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -11034,7 +11234,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -11059,7 +11261,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.25</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -11085,7 +11287,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -11111,7 +11313,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -11137,7 +11339,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -11162,7 +11364,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -11186,7 +11390,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -11210,7 +11416,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -11235,7 +11443,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.09375</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -11261,7 +11469,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -11287,7 +11495,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.1798611111111111</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -11313,7 +11521,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.01388888888888889</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -11339,7 +11547,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -11364,7 +11574,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -11389,7 +11601,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.1041666666666667</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -11415,7 +11629,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -11442,7 +11656,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.01388888888888889</v>
+        <v>0.125</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -11469,7 +11683,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1736111111111111</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -11496,7 +11710,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.02777777777777778</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -11522,7 +11736,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -11547,7 +11763,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -11572,7 +11790,9 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n"/>
+      <c r="C37" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -12051,7 +12271,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43616</v>
+        <v>42886</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -12177,7 +12397,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -12203,7 +12423,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.2361111111111111</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -12229,7 +12449,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.1319444444444444</v>
+        <v>0.125</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -12255,7 +12475,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.1527777777777778</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -12280,7 +12500,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -12304,7 +12526,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -12328,7 +12552,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -12353,7 +12579,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.1180555555555556</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -12379,7 +12605,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.1319444444444444</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -12405,7 +12631,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.09722222222222222</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -12431,7 +12657,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -12456,7 +12682,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.07291666666666667</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -12480,7 +12708,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -12504,7 +12734,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -12529,7 +12761,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1319444444444444</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -12555,7 +12787,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -12581,7 +12813,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -12607,7 +12839,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -12632,7 +12864,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.1458333333333333</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -12656,7 +12890,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.1354166666666667</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -12680,7 +12916,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.1145833333333333</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -12706,7 +12944,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -12733,7 +12971,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -12760,7 +12998,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.1944444444444444</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -12787,7 +13025,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -12813,7 +13051,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -12838,7 +13078,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.1145833333333333</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -12863,7 +13105,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.07291666666666667</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -12889,7 +13133,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.2013888888888889</v>
+        <v>0.09375</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -12916,7 +13160,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.2013888888888889</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -13421,7 +13665,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43646</v>
+        <v>42916</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -13547,7 +13791,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.25</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -13573,7 +13817,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -13598,7 +13842,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.1458333333333333</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -13622,7 +13868,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -13646,7 +13894,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -13671,7 +13921,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -13697,7 +13947,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.2013888888888889</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -13723,7 +13973,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -13749,7 +13999,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -13774,7 +14024,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.0625</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -13798,7 +14050,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -13822,7 +14076,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.1354166666666667</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -13847,7 +14103,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.25</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -13873,7 +14129,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -13899,7 +14155,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -13925,7 +14181,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1388888888888889</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -13950,7 +14206,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -13974,7 +14232,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.07291666666666667</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -13998,7 +14258,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.07291666666666667</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -14023,7 +14285,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -14049,7 +14311,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -14076,7 +14338,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -14103,7 +14365,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -14129,7 +14391,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -14154,7 +14418,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -14179,7 +14445,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -14205,7 +14473,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -14232,7 +14500,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -14259,7 +14527,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.25</v>
+        <v>0.0625</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -14286,7 +14554,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.08958333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -14312,7 +14580,9 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n"/>
+      <c r="C37" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -14791,7 +15061,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43677</v>
+        <v>42947</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -14916,7 +15186,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -14940,7 +15212,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -14991,7 +15265,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -15017,7 +15291,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -15043,7 +15317,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -15068,7 +15342,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -15092,7 +15368,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -15116,7 +15394,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.09375</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -15141,7 +15421,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.25</v>
+        <v>0.0625</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -15167,7 +15447,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.0763888888888889</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -15193,7 +15473,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -15219,7 +15499,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.125</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -15244,7 +15524,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -15268,7 +15550,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -15292,7 +15576,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -15317,7 +15603,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -15343,7 +15629,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -15369,7 +15655,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -15395,7 +15681,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -15420,7 +15706,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -15445,7 +15733,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.07291666666666667</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -15470,7 +15760,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -15496,7 +15788,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -15523,7 +15815,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.04861111111111111</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -15550,7 +15842,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -15577,7 +15869,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -15603,7 +15895,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -15628,7 +15922,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -15653,7 +15949,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -15679,7 +15977,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.25</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -16159,7 +16457,7 @@
         </is>
       </c>
       <c r="B3" s="51" t="n">
-        <v>43708</v>
+        <v>42978</v>
       </c>
       <c r="C3" s="52" t="n"/>
       <c r="D3" s="53" t="inlineStr">
@@ -16285,7 +16583,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.0625</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -16311,7 +16609,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -16337,7 +16635,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.1319444444444444</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -16362,7 +16660,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -16386,7 +16686,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -16410,7 +16712,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.04166666666666666</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -16435,7 +16739,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.25</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -16461,7 +16765,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.06944444444444445</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -16487,7 +16791,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.1180555555555556</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -16513,7 +16817,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -16538,7 +16842,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -16562,7 +16868,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.09375</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -16586,7 +16894,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.1458333333333333</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -16611,7 +16921,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -16637,7 +16947,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -16663,7 +16973,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -16689,7 +16999,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.09375</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -16714,7 +17024,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -16738,7 +17050,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.09375</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -16762,7 +17076,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.1666666666666667</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -16787,7 +17103,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -16814,7 +17130,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.125</v>
+        <v>0.0625</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -16841,7 +17157,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.25</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -16868,7 +17184,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -16894,7 +17210,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.1354166666666667</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -16919,7 +17237,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -16944,7 +17264,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.05208333333333334</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -16970,7 +17292,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -16997,7 +17319,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.25</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -17024,7 +17346,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.08958333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>

</xml_diff>

<commit_message>
Add start and end date
The hours generator will now only generate hours that are in the
specified date range. The xlsx file isn't really made for this however,
so currently there is some manual labor that is needed to make the xlsx
file work with it (such as setting the monthly hours manually in the
xlsx)
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1238,9 +1238,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C7" s="69" t="n"/>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -1264,9 +1262,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -1290,9 +1286,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.09375</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -1316,9 +1310,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -1342,9 +1334,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -1368,9 +1358,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.07291666666666667</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -1394,9 +1382,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -1420,9 +1406,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.05208333333333334</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -1446,9 +1430,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -1472,9 +1454,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.07291666666666667</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -1498,9 +1478,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0.07291666666666667</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -1524,9 +1502,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.1145833333333333</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -1550,9 +1526,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.1145833333333333</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -1576,9 +1550,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -1602,9 +1574,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C21" s="71" t="n"/>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -1628,9 +1598,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C22" s="71" t="n"/>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -1654,9 +1622,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.1041666666666667</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -1680,9 +1646,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C24" s="71" t="n"/>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -1706,9 +1670,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -1732,9 +1694,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C26" s="73" t="n"/>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -1758,9 +1718,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C27" s="73" t="n"/>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -1785,9 +1743,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C28" s="71" t="n"/>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -1812,9 +1768,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C29" s="71" t="n"/>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -1839,9 +1793,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.05208333333333334</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -1866,9 +1818,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C31" s="73" t="n"/>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -1893,9 +1843,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C32" s="73" t="n"/>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -1920,9 +1868,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n">
-        <v>0.05208333333333334</v>
-      </c>
+      <c r="C33" s="73" t="n"/>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -1947,9 +1893,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C34" s="73" t="n"/>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -1974,9 +1918,7 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n">
-        <v>0.07291666666666667</v>
-      </c>
+      <c r="C35" s="71" t="n"/>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -2001,9 +1943,7 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n">
-        <v>0.1145833333333333</v>
-      </c>
+      <c r="C36" s="71" t="n"/>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -2028,9 +1968,7 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C37" s="73" t="n"/>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -2635,7 +2573,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.09375</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -2661,7 +2599,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -2713,7 +2651,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -2739,7 +2677,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -2791,7 +2729,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -2817,7 +2755,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -2843,7 +2781,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.125</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -2869,7 +2807,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.15625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -2895,7 +2833,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -2921,7 +2859,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -2947,7 +2885,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -2973,7 +2911,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.0625</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -2999,7 +2937,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -3025,7 +2963,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -3051,7 +2989,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -3077,7 +3015,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -3129,7 +3067,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -3155,7 +3093,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.0625</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -3182,7 +3120,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -3209,7 +3147,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -3236,7 +3174,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -3263,7 +3201,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.09375</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -3290,7 +3228,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -3344,7 +3282,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -3371,7 +3309,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.15625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -3398,7 +3336,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -3425,7 +3363,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -4031,7 +3969,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -4056,9 +3994,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -4082,9 +4018,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -4108,9 +4042,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -4134,9 +4066,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -4160,9 +4090,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -4186,9 +4114,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.1145833333333333</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -4212,9 +4138,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.1145833333333333</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -4238,9 +4162,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -4264,9 +4186,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -4290,9 +4210,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -4316,9 +4234,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.05208333333333334</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -4342,9 +4258,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.07291666666666667</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -4368,9 +4282,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -4394,9 +4306,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C21" s="71" t="n"/>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -4420,9 +4330,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n">
-        <v>0.07291666666666667</v>
-      </c>
+      <c r="C22" s="71" t="n"/>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -4446,9 +4354,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -4472,9 +4378,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C24" s="71" t="n"/>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -4498,9 +4402,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -4524,9 +4426,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C26" s="73" t="n"/>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -4550,9 +4450,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C27" s="73" t="n"/>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -4577,9 +4475,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n">
-        <v>0.1458333333333333</v>
-      </c>
+      <c r="C28" s="71" t="n"/>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -4604,9 +4500,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C29" s="71" t="n"/>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -4631,9 +4525,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -4658,9 +4550,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n">
-        <v>0.1458333333333333</v>
-      </c>
+      <c r="C31" s="73" t="n"/>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -4685,9 +4575,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C32" s="73" t="n"/>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -4712,9 +4600,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n">
-        <v>0.1041666666666667</v>
-      </c>
+      <c r="C33" s="73" t="n"/>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -4739,9 +4625,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C34" s="73" t="n"/>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -4766,9 +4650,7 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C35" s="71" t="n"/>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -4793,9 +4675,7 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C36" s="71" t="n"/>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -5424,9 +5304,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C7" s="69" t="n"/>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -5450,9 +5328,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -5476,9 +5352,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -5502,9 +5376,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.1354166666666667</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -5528,9 +5400,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.1354166666666667</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -5554,9 +5424,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -5580,9 +5448,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.1354166666666667</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -5606,9 +5472,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.05208333333333334</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -5632,9 +5496,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -5658,9 +5520,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.1354166666666667</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -5684,9 +5544,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -5710,9 +5568,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -5736,9 +5592,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -5762,9 +5616,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -5788,9 +5640,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C21" s="71" t="n"/>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -5814,9 +5664,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n">
-        <v>0.05208333333333334</v>
-      </c>
+      <c r="C22" s="71" t="n"/>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -5840,9 +5688,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -5866,9 +5712,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C24" s="71" t="n"/>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -5892,9 +5736,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -5918,9 +5760,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C26" s="73" t="n"/>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -5944,9 +5784,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n">
-        <v>0.1145833333333333</v>
-      </c>
+      <c r="C27" s="73" t="n"/>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -5971,9 +5809,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n">
-        <v>0.1354166666666667</v>
-      </c>
+      <c r="C28" s="71" t="n"/>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -5998,9 +5834,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C29" s="71" t="n"/>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -6025,9 +5859,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.09375</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -6052,9 +5884,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n">
-        <v>0.09375</v>
-      </c>
+      <c r="C31" s="73" t="n"/>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -6079,9 +5909,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C32" s="73" t="n"/>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -6106,9 +5934,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C33" s="73" t="n"/>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -6133,9 +5959,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C34" s="73" t="n"/>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -6160,9 +5984,7 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C35" s="71" t="n"/>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -6187,9 +6009,7 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C36" s="71" t="n"/>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -6214,9 +6034,7 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C37" s="73" t="n"/>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -6820,9 +6638,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C7" s="69" t="n"/>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -6846,9 +6662,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -6872,9 +6686,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -6898,9 +6710,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.1145833333333333</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -6924,9 +6734,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.09375</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -6950,9 +6758,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -6976,9 +6782,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -7002,9 +6806,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.05208333333333334</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -7028,9 +6830,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -7054,9 +6854,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -7080,9 +6878,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0.07291666666666667</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -7106,9 +6902,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.05208333333333334</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -7132,9 +6926,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -7158,9 +6950,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -7184,9 +6974,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C21" s="71" t="n"/>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -7210,9 +6998,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n">
-        <v>0.09375</v>
-      </c>
+      <c r="C22" s="71" t="n"/>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -7236,9 +7022,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.07291666666666667</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -7262,9 +7046,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C24" s="71" t="n"/>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -7288,9 +7070,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -7314,9 +7094,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C26" s="73" t="n"/>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -7340,9 +7118,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C27" s="73" t="n"/>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -7367,9 +7143,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n">
-        <v>0.09375</v>
-      </c>
+      <c r="C28" s="71" t="n"/>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -7394,9 +7168,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C29" s="71" t="n"/>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -7421,9 +7193,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -7448,9 +7218,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C31" s="73" t="n"/>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -7475,9 +7243,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C32" s="73" t="n"/>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -7502,9 +7268,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C33" s="73" t="n"/>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -7529,9 +7293,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n">
-        <v>0.0625</v>
-      </c>
+      <c r="C34" s="73" t="n"/>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -8210,9 +7972,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C7" s="69" t="n"/>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -8236,9 +7996,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -8262,9 +8020,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -8288,9 +8044,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -8314,9 +8068,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -8340,9 +8092,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -8366,9 +8116,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.15625</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -8392,9 +8140,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.1354166666666667</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -8418,9 +8164,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.1145833333333333</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -8444,9 +8188,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.07291666666666667</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -8470,9 +8212,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0.15625</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -8496,9 +8236,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.1666666666666667</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -8522,9 +8260,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -8548,9 +8284,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.04166666666666666</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -8575,7 +8309,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -8679,7 +8413,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -8705,7 +8439,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -8758,7 +8492,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -8866,7 +8600,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -8947,7 +8681,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.0625</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -8974,7 +8708,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.0625</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -9001,7 +8735,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.15625</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -9607,7 +9341,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.125</v>
+        <v>0.09375</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -9815,7 +9549,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -9841,7 +9575,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -9893,7 +9627,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -9919,7 +9653,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -9945,7 +9679,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -9971,7 +9705,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -9997,7 +9731,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -10023,7 +9757,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -10049,7 +9783,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -10101,7 +9835,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -10127,7 +9861,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -10154,7 +9888,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -10181,7 +9915,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -10235,7 +9969,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -10262,7 +9996,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -10289,7 +10023,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -10343,7 +10077,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.0625</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -10370,7 +10104,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -11001,7 +10735,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -11027,7 +10761,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -11079,7 +10813,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -11209,7 +10943,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -11261,7 +10995,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -11313,7 +11047,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -11365,7 +11099,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.09375</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -11391,7 +11125,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -11417,7 +11151,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -11443,7 +11177,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -11469,7 +11203,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -11521,7 +11255,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -11548,7 +11282,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -11575,7 +11309,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -11602,7 +11336,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -11656,7 +11390,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -11683,7 +11417,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -11710,7 +11444,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.15625</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -11791,7 +11525,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -12397,7 +12131,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -12423,7 +12157,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -12449,7 +12183,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.125</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -12475,7 +12209,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -12501,7 +12235,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.15625</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -12527,7 +12261,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -12553,7 +12287,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -12579,7 +12313,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -12683,7 +12417,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -12709,7 +12443,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -12735,7 +12469,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -12787,7 +12521,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -12813,7 +12547,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -12839,7 +12573,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -12865,7 +12599,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -12891,7 +12625,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -12917,7 +12651,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -12944,7 +12678,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -12971,7 +12705,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -13052,7 +12786,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -13079,7 +12813,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -13106,7 +12840,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -13133,7 +12867,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -13160,7 +12894,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -13791,7 +13525,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -13817,7 +13551,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.0625</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -13843,7 +13577,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -13921,7 +13655,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -13973,7 +13707,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -13999,7 +13733,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -14025,7 +13759,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.0625</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -14051,7 +13785,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -14077,7 +13811,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -14103,7 +13837,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -14129,7 +13863,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -14181,7 +13915,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -14233,7 +13967,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -14259,7 +13993,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -14285,7 +14019,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -14338,7 +14072,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -14392,7 +14126,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.15625</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -14446,7 +14180,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -14473,7 +14207,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -14527,7 +14261,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -14554,7 +14288,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -14581,7 +14315,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -15187,7 +14921,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -15213,7 +14947,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.125</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -15239,7 +14973,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -15265,7 +14999,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -15317,7 +15051,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -15343,7 +15077,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -15395,7 +15129,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -15421,7 +15155,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.0625</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -15447,7 +15181,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -15499,7 +15233,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -15525,7 +15259,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -15551,7 +15285,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -15577,7 +15311,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -15629,7 +15363,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -15681,7 +15415,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -15707,7 +15441,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.125</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -15734,7 +15468,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -15761,7 +15495,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.15625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -15788,7 +15522,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -15815,7 +15549,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -15842,7 +15576,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -15869,7 +15603,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -15923,7 +15657,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -15950,7 +15684,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -15977,7 +15711,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -16583,7 +16317,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -16661,7 +16395,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -16713,7 +16447,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -16739,7 +16473,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -16791,7 +16525,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.09375</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -16843,7 +16577,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -16869,7 +16603,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -16895,7 +16629,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -16921,7 +16655,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -16947,7 +16681,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -16973,7 +16707,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -16999,7 +16733,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -17025,7 +16759,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -17051,7 +16785,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -17077,7 +16811,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -17103,7 +16837,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -17130,7 +16864,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -17157,7 +16891,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -17184,7 +16918,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.0625</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -17211,7 +16945,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -17238,7 +16972,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -17265,7 +16999,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -17292,7 +17026,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -17346,7 +17080,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>

</xml_diff>

<commit_message>
Reformat python files with black
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -2573,7 +2573,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -2599,7 +2599,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -2625,7 +2625,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -2651,7 +2651,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -2677,7 +2677,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -2729,7 +2729,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -2755,7 +2755,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -2781,7 +2781,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -2807,7 +2807,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -2833,7 +2833,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -2937,7 +2937,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -2963,7 +2963,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -2989,7 +2989,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -3067,7 +3067,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.09375</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -3093,7 +3093,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -3120,7 +3120,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.0625</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -3147,7 +3147,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -3174,7 +3174,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.09375</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -3201,7 +3201,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -3336,7 +3336,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.0625</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -3363,7 +3363,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -3969,7 +3969,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.09375</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -8309,7 +8309,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -8335,7 +8335,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -8387,7 +8387,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -8413,7 +8413,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -8465,7 +8465,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -8519,7 +8519,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -8546,7 +8546,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -8600,7 +8600,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -8627,7 +8627,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -8681,7 +8681,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -8708,7 +8708,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -8735,7 +8735,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.15625</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -9341,7 +9341,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.09375</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -9393,7 +9393,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -9419,7 +9419,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -9523,7 +9523,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -9549,7 +9549,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -9575,7 +9575,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.09375</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -9627,7 +9627,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.15625</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -9653,7 +9653,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -9679,7 +9679,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -9705,7 +9705,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -9731,7 +9731,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -9757,7 +9757,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -9809,7 +9809,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -9888,7 +9888,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -9915,7 +9915,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.125</v>
+        <v>0.15625</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -9942,7 +9942,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -9969,7 +9969,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -9996,7 +9996,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.0625</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -10023,7 +10023,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.15625</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -10050,7 +10050,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -10077,7 +10077,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -10104,7 +10104,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -10735,7 +10735,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -10761,7 +10761,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -10813,7 +10813,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -10839,7 +10839,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -10865,7 +10865,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -10891,7 +10891,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -10917,7 +10917,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -10943,7 +10943,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.15625</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -10995,7 +10995,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -11047,7 +11047,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -11073,7 +11073,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -11099,7 +11099,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -11151,7 +11151,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -11177,7 +11177,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -11282,7 +11282,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -11363,7 +11363,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -11390,7 +11390,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -11417,7 +11417,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -11444,7 +11444,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.15625</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -11471,7 +11471,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -11498,7 +11498,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -11525,7 +11525,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -12131,7 +12131,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.125</v>
+        <v>0.09375</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -12157,7 +12157,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -12183,7 +12183,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.0625</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -12209,7 +12209,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -12235,7 +12235,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -12261,7 +12261,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -12287,7 +12287,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -12313,7 +12313,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -12339,7 +12339,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.0625</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -12391,7 +12391,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -12417,7 +12417,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -12443,7 +12443,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -12469,7 +12469,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.09375</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -12495,7 +12495,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -12521,7 +12521,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -12547,7 +12547,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -12573,7 +12573,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -12599,7 +12599,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -12678,7 +12678,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.09375</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -12705,7 +12705,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -12786,7 +12786,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.15625</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -12840,7 +12840,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -12894,7 +12894,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -13525,7 +13525,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -13551,7 +13551,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.0625</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -13577,7 +13577,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.09375</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -13603,7 +13603,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -13629,7 +13629,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -13655,7 +13655,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -13707,7 +13707,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -13733,7 +13733,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.0625</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -13759,7 +13759,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -13785,7 +13785,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -13811,7 +13811,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -13863,7 +13863,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -13889,7 +13889,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -13967,7 +13967,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -13993,7 +13993,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -14019,7 +14019,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -14072,7 +14072,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -14126,7 +14126,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.15625</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -14180,7 +14180,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -14288,7 +14288,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -14315,7 +14315,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.15625</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -14921,7 +14921,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.125</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -14947,7 +14947,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.09375</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -14973,7 +14973,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -14999,7 +14999,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -15051,7 +15051,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.09375</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -15077,7 +15077,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.1145833333333333</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -15155,7 +15155,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -15181,7 +15181,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -15207,7 +15207,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -15233,7 +15233,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -15259,7 +15259,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -15285,7 +15285,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.07291666666666667</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -15311,7 +15311,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.125</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -15337,7 +15337,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -15415,7 +15415,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -15441,7 +15441,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -15468,7 +15468,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.0625</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -15522,7 +15522,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -15576,7 +15576,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -15603,7 +15603,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.09375</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -15630,7 +15630,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -15657,7 +15657,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -15684,7 +15684,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -15711,7 +15711,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -16317,7 +16317,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -16369,7 +16369,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -16395,7 +16395,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -16447,7 +16447,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.125</v>
+        <v>0.1458333333333333</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -16473,7 +16473,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -16499,7 +16499,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -16525,7 +16525,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -16551,7 +16551,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -16603,7 +16603,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -16629,7 +16629,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -16681,7 +16681,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -16707,7 +16707,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.05208333333333334</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -16733,7 +16733,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -16759,7 +16759,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -16811,7 +16811,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -16837,7 +16837,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.09375</v>
+        <v>0.1354166666666667</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -16864,7 +16864,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -16891,7 +16891,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -16918,7 +16918,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.0625</v>
+        <v>0.05208333333333334</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -16945,7 +16945,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.07291666666666667</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -16972,7 +16972,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -16999,7 +16999,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -17026,7 +17026,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -17053,7 +17053,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -17080,7 +17080,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.1041666666666667</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>

</xml_diff>

<commit_message>
Restructure the hour generation
The current way is much more stable and should also allow for event
days.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1238,7 +1238,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -1311,7 +1313,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -1337,7 +1339,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.2395833333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -1363,7 +1365,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -1388,7 +1390,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -1412,7 +1416,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -1485,7 +1491,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -1511,7 +1517,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -1537,7 +1543,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -1562,7 +1568,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -1586,7 +1594,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -1659,7 +1669,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -1685,7 +1695,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -1711,7 +1721,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -1736,7 +1746,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -1761,7 +1773,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -1837,7 +1851,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -1864,7 +1878,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.09375</v>
+        <v>0.125</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -1917,7 +1931,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -1942,7 +1958,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -2596,7 +2614,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -2669,7 +2689,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -2695,7 +2715,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -2721,7 +2741,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -2746,7 +2766,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -2770,7 +2792,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -2843,7 +2867,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -2869,7 +2893,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -2895,7 +2919,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -2920,7 +2944,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -2944,7 +2970,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -3017,7 +3045,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.1875</v>
+        <v>0.125</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -3043,7 +3071,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.1979166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -3069,7 +3097,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -3094,7 +3122,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -3119,7 +3149,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -3195,7 +3227,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -3222,7 +3254,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -3249,7 +3281,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -3275,7 +3307,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -3300,7 +3334,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -3955,7 +3991,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -3981,7 +4017,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -4007,7 +4043,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -4032,7 +4068,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -4056,7 +4094,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -4129,7 +4169,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -4155,7 +4195,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -4181,7 +4221,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -4206,7 +4246,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -4230,7 +4272,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -4303,7 +4347,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -4329,7 +4373,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -4355,7 +4399,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -4380,7 +4424,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -4404,7 +4450,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -4478,7 +4526,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -4505,7 +4553,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -4532,7 +4580,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.15625</v>
+        <v>0.125</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -4558,7 +4606,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -4583,7 +4633,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -4659,7 +4711,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -4686,7 +4738,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -5317,7 +5369,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -5342,7 +5394,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -5366,7 +5420,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -5439,7 +5495,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -5465,7 +5521,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.2395833333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -5491,7 +5547,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -5516,7 +5572,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -5540,7 +5598,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -5613,7 +5673,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -5639,7 +5699,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -5665,7 +5725,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -5690,7 +5750,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -5714,7 +5776,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -5787,7 +5851,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -5813,7 +5877,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.1979166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -5840,7 +5904,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -5866,7 +5930,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -5891,7 +5957,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -5967,7 +6035,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -5994,7 +6062,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.15625</v>
+        <v>0.125</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -6021,7 +6089,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -6047,7 +6115,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -6072,7 +6142,9 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n"/>
+      <c r="C37" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -6677,7 +6749,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -6703,7 +6775,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -6729,7 +6801,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.15625</v>
+        <v>0.125</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -6754,7 +6826,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -6778,7 +6852,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -6877,7 +6953,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -6903,7 +6979,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -6928,7 +7004,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -6952,7 +7030,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -7025,7 +7105,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -7051,7 +7131,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.21875</v>
+        <v>0.125</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -7077,7 +7157,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -7102,7 +7182,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -7126,7 +7208,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -7200,7 +7284,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.1979166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -7227,7 +7311,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.1875</v>
+        <v>0.125</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -7254,7 +7338,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -7280,7 +7364,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -7305,7 +7391,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -8035,7 +8123,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -8061,7 +8149,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -8087,7 +8175,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -8112,7 +8200,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -8136,7 +8226,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -8209,7 +8301,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -8235,7 +8327,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -8261,7 +8353,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -8286,7 +8378,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -8310,7 +8404,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -8383,7 +8479,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -8409,7 +8505,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -8435,7 +8531,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.21875</v>
+        <v>0.125</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -8460,7 +8556,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -8484,7 +8582,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -8558,7 +8658,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -8585,7 +8685,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -8612,7 +8712,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -8638,7 +8738,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -8663,7 +8765,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -8739,7 +8843,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -8766,7 +8870,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -8793,7 +8897,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -9398,7 +9502,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -9422,7 +9528,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -9495,7 +9603,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -9521,7 +9629,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -9547,7 +9655,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -9572,7 +9680,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -9596,7 +9706,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -9669,7 +9781,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -9695,7 +9807,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -9746,7 +9858,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -9770,7 +9884,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -9843,7 +9959,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -9921,7 +10037,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -9946,7 +10064,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -10049,7 +10169,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1770833333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -10076,7 +10196,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -10102,7 +10222,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -10127,7 +10249,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -10805,7 +10929,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -10857,7 +10981,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -10882,7 +11006,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -10906,7 +11032,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -10979,7 +11107,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.1770833333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -11031,7 +11159,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.1979166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -11056,7 +11184,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -11080,7 +11210,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -11153,7 +11285,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -11179,7 +11311,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -11205,7 +11337,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -11230,7 +11362,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -11254,7 +11388,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -11330,7 +11466,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.1979166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -11357,7 +11493,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -11384,7 +11520,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -11410,7 +11546,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -11435,7 +11573,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -11511,7 +11651,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -12143,7 +12283,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.1770833333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -12168,7 +12308,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -12192,7 +12334,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -12265,7 +12409,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -12291,7 +12435,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -12317,7 +12461,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.21875</v>
+        <v>0.125</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -12342,7 +12486,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -12366,7 +12512,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -12439,7 +12587,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -12465,7 +12613,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -12491,7 +12639,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -12516,7 +12664,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -12540,7 +12690,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -12613,7 +12765,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.15625</v>
+        <v>0.125</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -12640,7 +12792,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -12667,7 +12819,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -12693,7 +12845,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -12718,7 +12872,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -12794,7 +12950,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.21875</v>
+        <v>0.125</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -12821,7 +12977,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -12848,7 +13004,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -13478,7 +13634,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -13502,7 +13660,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -13575,7 +13735,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -13627,7 +13787,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -13652,7 +13812,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -13676,7 +13838,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -13749,7 +13913,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -13775,7 +13939,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -13801,7 +13965,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -13826,7 +13990,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -13850,7 +14016,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -13923,7 +14091,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -13949,7 +14117,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -13975,7 +14143,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -14001,7 +14169,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -14026,7 +14196,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -14102,7 +14274,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -14129,7 +14301,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.1354166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -14156,7 +14328,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.15625</v>
+        <v>0.125</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -14182,7 +14354,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -14207,7 +14381,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -14861,7 +15037,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -14887,7 +15063,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -14913,7 +15089,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.25</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -14938,7 +15114,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -14962,7 +15140,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -15035,7 +15215,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -15061,7 +15241,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -15087,7 +15267,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -15112,7 +15292,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -15136,7 +15318,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -15209,7 +15393,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -15235,7 +15419,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.2291666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -15261,7 +15445,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -15286,7 +15470,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -15310,7 +15496,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -15385,7 +15573,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.1458333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -15412,7 +15600,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.04166666666666666</v>
+        <v>0.125</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -15439,7 +15627,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.1875</v>
+        <v>0.125</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -15465,7 +15653,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -15490,7 +15680,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -15566,7 +15758,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.09375</v>
+        <v>0.125</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -15593,7 +15785,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -16199,7 +16391,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.1875</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -16224,7 +16416,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -16248,7 +16442,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.08333333333333333</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -16321,7 +16517,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -16347,7 +16543,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.1770833333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -16373,7 +16569,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.2083333333333333</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -16398,7 +16594,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -16422,7 +16620,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -16495,7 +16695,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -16547,7 +16747,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -16572,7 +16772,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -16596,7 +16798,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -16669,7 +16873,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -16695,7 +16899,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.1979166666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -16722,7 +16926,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -16748,7 +16952,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -16773,7 +16979,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -16849,7 +17057,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -16876,7 +17084,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.1041666666666667</v>
+        <v>0.125</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -16903,7 +17111,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.1145833333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -16929,7 +17137,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.125</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>

</xml_diff>

<commit_message>
Complete the hour generation process
The generation of the hours with the new method works now. Event days
and black days both work as well.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1238,9 +1238,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C7" s="69" t="n"/>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -1264,7 +1262,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -1288,7 +1288,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -1338,9 +1340,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -1364,9 +1364,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -1391,7 +1389,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -1416,9 +1414,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -1442,7 +1438,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -1466,7 +1464,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -1491,7 +1491,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -1516,9 +1516,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -1542,9 +1540,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -1569,7 +1565,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -1594,9 +1590,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C21" s="71" t="n"/>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -1620,7 +1614,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -1644,7 +1640,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -1669,7 +1667,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -1694,9 +1692,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -1720,9 +1716,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C26" s="73" t="n"/>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -1747,7 +1741,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -1773,9 +1767,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C28" s="71" t="n"/>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -1800,7 +1792,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -1825,7 +1819,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -1878,7 +1874,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -1904,9 +1900,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C33" s="73" t="n"/>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -1932,7 +1926,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -1958,9 +1952,7 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C35" s="71" t="n"/>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -1985,7 +1977,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -2010,7 +2004,9 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n"/>
+      <c r="C37" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -2614,9 +2610,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C7" s="69" t="n"/>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -2640,7 +2634,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -2664,7 +2660,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -2714,9 +2712,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -2740,9 +2736,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -2767,7 +2761,7 @@
         <v/>
       </c>
       <c r="C13" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
@@ -2792,9 +2786,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -2818,7 +2810,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -2842,7 +2836,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -2867,7 +2863,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -2892,9 +2888,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -2918,9 +2912,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -2945,7 +2937,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -2970,9 +2962,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C21" s="71" t="n"/>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -2996,7 +2986,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -3020,7 +3012,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -3045,7 +3039,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -3070,9 +3064,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -3096,9 +3088,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C26" s="73" t="n"/>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -3123,7 +3113,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -3149,9 +3139,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C28" s="71" t="n"/>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -3176,7 +3164,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -3201,7 +3191,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -3254,7 +3246,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -3280,9 +3272,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C33" s="73" t="n"/>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -3308,7 +3298,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -3334,9 +3324,7 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C35" s="71" t="n"/>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -3361,7 +3349,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -3386,7 +3376,9 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n"/>
+      <c r="C37" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -4016,9 +4008,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -4042,9 +4032,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -4069,7 +4057,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -4094,9 +4082,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -4120,7 +4106,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -4144,7 +4132,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -4194,9 +4184,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -4220,9 +4208,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -4247,7 +4233,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -4272,9 +4258,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -4298,7 +4282,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -4322,7 +4308,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -4373,7 +4361,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -4398,9 +4386,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -4425,7 +4411,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -4450,9 +4436,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -4476,7 +4460,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -4500,7 +4486,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -4553,7 +4541,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -4579,9 +4567,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -4607,7 +4593,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -4633,9 +4619,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C32" s="73" t="n"/>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -4660,7 +4644,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -4685,7 +4671,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -4738,7 +4726,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -5368,9 +5356,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C7" s="69" t="n"/>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -5395,7 +5381,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -5420,9 +5406,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -5446,7 +5430,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -5470,7 +5456,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -5520,9 +5508,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -5546,9 +5532,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -5573,7 +5557,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -5598,9 +5582,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -5624,7 +5606,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -5648,7 +5632,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -5673,7 +5659,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.125</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -5699,7 +5685,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -5724,9 +5710,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C21" s="71" t="n"/>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -5751,7 +5735,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -5776,9 +5760,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -5802,7 +5784,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -5826,7 +5810,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -5877,7 +5863,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -5903,9 +5889,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C28" s="71" t="n"/>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -5931,7 +5915,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -5957,9 +5941,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -5984,7 +5966,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -6009,7 +5993,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -6062,7 +6048,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -6088,9 +6074,7 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C35" s="71" t="n"/>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -6116,7 +6100,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -6142,9 +6126,7 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C37" s="73" t="n"/>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -6749,7 +6731,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -6774,9 +6756,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -6800,9 +6780,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -6827,7 +6805,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -6852,9 +6830,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -6878,7 +6854,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -6902,7 +6880,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -6927,7 +6907,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -6953,7 +6933,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -6978,9 +6958,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -7005,7 +6983,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -7030,9 +7008,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -7056,7 +7032,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -7080,7 +7058,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -7131,7 +7111,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -7156,9 +7136,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -7183,7 +7161,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -7208,9 +7186,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -7234,7 +7210,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -7258,7 +7236,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -7311,7 +7291,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -7337,9 +7317,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -7365,7 +7343,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -7391,9 +7369,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C32" s="73" t="n"/>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -7418,7 +7394,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -7443,7 +7421,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -8148,9 +8128,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -8174,9 +8152,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -8201,7 +8177,7 @@
         <v/>
       </c>
       <c r="C10" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
@@ -8226,9 +8202,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -8252,7 +8226,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -8276,7 +8252,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -8326,9 +8304,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -8352,9 +8328,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -8379,7 +8353,7 @@
         <v/>
       </c>
       <c r="C17" s="75" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
@@ -8404,9 +8378,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -8430,7 +8402,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -8454,7 +8428,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -8505,7 +8481,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -8530,9 +8506,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -8557,7 +8531,7 @@
         <v/>
       </c>
       <c r="C24" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
@@ -8582,9 +8556,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -8608,7 +8580,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -8632,7 +8606,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -8685,7 +8661,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -8711,9 +8687,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -8739,7 +8713,7 @@
         <v/>
       </c>
       <c r="C31" s="73" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
@@ -8765,9 +8739,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C32" s="73" t="n"/>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -8792,7 +8764,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -8817,7 +8791,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -8870,7 +8846,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
@@ -8896,9 +8872,7 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C37" s="73" t="n"/>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -9503,7 +9477,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -9528,9 +9502,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -9554,7 +9526,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -9578,7 +9552,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -9628,9 +9604,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -9654,9 +9628,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -9681,7 +9653,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -9706,9 +9678,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -9732,7 +9702,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -9756,7 +9728,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -9807,7 +9781,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -9832,9 +9806,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -9859,7 +9831,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -9884,9 +9856,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C22" s="71" t="n"/>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -9910,7 +9880,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -9934,7 +9906,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -9985,7 +9959,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -10010,9 +9984,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C27" s="73" t="n"/>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -10038,7 +10010,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -10064,9 +10036,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C29" s="71" t="n"/>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -10091,7 +10061,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -10116,7 +10088,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -10169,7 +10143,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -10195,9 +10169,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C34" s="73" t="n"/>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -10223,7 +10195,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -10249,9 +10221,7 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C36" s="71" t="n"/>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -10880,7 +10850,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -10904,7 +10876,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n"/>
+      <c r="C8" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -10954,9 +10928,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -10980,9 +10952,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C11" s="71" t="n"/>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -11007,7 +10977,7 @@
         <v/>
       </c>
       <c r="C12" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
@@ -11032,9 +11002,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -11058,7 +11026,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -11082,7 +11052,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n"/>
+      <c r="C15" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -11107,7 +11079,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -11132,9 +11104,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -11158,9 +11128,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C18" s="71" t="n"/>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -11185,7 +11153,7 @@
         <v/>
       </c>
       <c r="C19" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
@@ -11210,9 +11178,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -11236,7 +11202,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -11260,7 +11228,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n"/>
+      <c r="C22" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -11285,7 +11255,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -11310,9 +11280,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C24" s="71" t="n"/>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -11336,9 +11304,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C25" s="71" t="n"/>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -11363,7 +11329,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -11388,9 +11354,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C27" s="73" t="n"/>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -11415,7 +11379,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -11440,7 +11406,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n"/>
+      <c r="C29" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -11466,7 +11434,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -11492,9 +11460,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C31" s="73" t="n"/>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -11519,9 +11485,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C32" s="73" t="n"/>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -11547,7 +11511,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -11573,9 +11537,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C34" s="73" t="n"/>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -11600,7 +11562,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -11625,7 +11589,9 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n"/>
+      <c r="C36" s="71" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -12256,9 +12222,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C7" s="69" t="n"/>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -12282,9 +12246,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -12309,7 +12271,7 @@
         <v/>
       </c>
       <c r="C9" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
@@ -12334,9 +12296,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -12360,7 +12320,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -12384,7 +12346,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n"/>
+      <c r="C12" s="73" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -12434,9 +12398,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -12460,9 +12422,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -12487,7 +12447,7 @@
         <v/>
       </c>
       <c r="C16" s="74" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
@@ -12512,9 +12472,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -12538,7 +12496,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -12562,7 +12522,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n"/>
+      <c r="C19" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -12613,7 +12575,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -12638,9 +12600,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C22" s="71" t="n"/>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -12665,7 +12625,7 @@
         <v/>
       </c>
       <c r="C23" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
@@ -12690,9 +12650,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C24" s="71" t="n"/>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -12716,7 +12674,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -12740,7 +12700,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n"/>
+      <c r="C26" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -12792,7 +12754,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -12818,9 +12780,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C29" s="71" t="n"/>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -12846,7 +12806,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -12872,9 +12832,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C31" s="73" t="n"/>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -12899,7 +12857,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -12924,7 +12884,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n"/>
+      <c r="C33" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -12977,7 +12939,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -13003,9 +12965,7 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C36" s="71" t="n"/>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -13635,7 +13595,7 @@
         <v/>
       </c>
       <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
@@ -13660,9 +13620,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B7+1))</f>
         <v/>
       </c>
-      <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C8" s="71" t="n"/>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
       <c r="F8" s="49" t="n"/>
@@ -13686,7 +13644,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n"/>
+      <c r="C9" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -13710,7 +13670,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -13760,9 +13722,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -13786,9 +13746,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -13813,7 +13771,7 @@
         <v/>
       </c>
       <c r="C14" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
@@ -13838,9 +13796,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B14+1))</f>
         <v/>
       </c>
-      <c r="C15" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C15" s="71" t="n"/>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
       <c r="F15" s="49" t="n"/>
@@ -13864,7 +13820,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n"/>
+      <c r="C16" s="74" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -13888,7 +13846,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -13913,7 +13873,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -13938,9 +13898,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -13964,9 +13922,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C20" s="73" t="n"/>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -13991,7 +13947,7 @@
         <v/>
       </c>
       <c r="C21" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
@@ -14016,9 +13972,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B21+1))</f>
         <v/>
       </c>
-      <c r="C22" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C22" s="71" t="n"/>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
       <c r="F22" s="49" t="n"/>
@@ -14042,7 +13996,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n"/>
+      <c r="C23" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -14066,7 +14022,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -14117,7 +14075,7 @@
         <v/>
       </c>
       <c r="C26" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
@@ -14142,9 +14100,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C27" s="73" t="n"/>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -14170,7 +14126,7 @@
         <v/>
       </c>
       <c r="C28" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
@@ -14196,9 +14152,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B28+1))</f>
         <v/>
       </c>
-      <c r="C29" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C29" s="71" t="n"/>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
       <c r="F29" s="49" t="n"/>
@@ -14223,7 +14177,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n"/>
+      <c r="C30" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -14248,7 +14204,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -14301,7 +14259,7 @@
         <v/>
       </c>
       <c r="C33" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
@@ -14327,9 +14285,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C34" s="73" t="n"/>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -14355,7 +14311,7 @@
         <v/>
       </c>
       <c r="C35" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
@@ -14381,9 +14337,7 @@
         <f>IF(B35="","",IF(DAY(B35+1)&gt;MONTH($B$3),B35+1,""))</f>
         <v/>
       </c>
-      <c r="C36" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C36" s="71" t="n"/>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>
       <c r="F36" s="49" t="n"/>
@@ -14408,7 +14362,9 @@
         <f>IF(B36="","",IF(DAY(B36+1)&gt;MONTH($B$3),B36+1,""))</f>
         <v/>
       </c>
-      <c r="C37" s="73" t="n"/>
+      <c r="C37" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
       <c r="F37" s="49" t="n"/>
@@ -15012,7 +14968,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n"/>
+      <c r="C7" s="69" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -15062,9 +15020,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -15088,9 +15044,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C10" s="71" t="n"/>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -15115,7 +15069,7 @@
         <v/>
       </c>
       <c r="C11" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
@@ -15140,9 +15094,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B11+1))</f>
         <v/>
       </c>
-      <c r="C12" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C12" s="73" t="n"/>
       <c r="D12" s="49" t="n"/>
       <c r="E12" s="49" t="n"/>
       <c r="F12" s="49" t="n"/>
@@ -15166,7 +15118,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n"/>
+      <c r="C13" s="73" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -15190,7 +15144,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n"/>
+      <c r="C14" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -15240,9 +15196,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -15266,9 +15220,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C17" s="75" t="n"/>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -15293,7 +15245,7 @@
         <v/>
       </c>
       <c r="C18" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
@@ -15318,9 +15270,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B18+1))</f>
         <v/>
       </c>
-      <c r="C19" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C19" s="73" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
       <c r="F19" s="49" t="n"/>
@@ -15344,7 +15294,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B19+1))</f>
         <v/>
       </c>
-      <c r="C20" s="73" t="n"/>
+      <c r="C20" s="73" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
       <c r="F20" s="49" t="n"/>
@@ -15368,7 +15320,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n"/>
+      <c r="C21" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -15393,7 +15347,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -15418,9 +15372,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -15444,9 +15396,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C24" s="71" t="n"/>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -15471,7 +15421,7 @@
         <v/>
       </c>
       <c r="C25" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
@@ -15496,9 +15446,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B25+1))</f>
         <v/>
       </c>
-      <c r="C26" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C26" s="73" t="n"/>
       <c r="D26" s="49" t="n"/>
       <c r="E26" s="49" t="n"/>
       <c r="F26" s="49" t="n"/>
@@ -15522,7 +15470,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B26+1))</f>
         <v/>
       </c>
-      <c r="C27" s="73" t="n"/>
+      <c r="C27" s="73" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
       <c r="F27" s="49" t="n"/>
@@ -15547,7 +15497,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n"/>
+      <c r="C28" s="71" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -15600,7 +15552,7 @@
         <v/>
       </c>
       <c r="C30" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
@@ -15626,9 +15578,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C31" s="73" t="n"/>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -15654,7 +15604,7 @@
         <v/>
       </c>
       <c r="C32" s="73" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
@@ -15680,9 +15630,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B32+1))</f>
         <v/>
       </c>
-      <c r="C33" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C33" s="73" t="n"/>
       <c r="D33" s="49" t="n"/>
       <c r="E33" s="49" t="n"/>
       <c r="F33" s="49" t="n"/>
@@ -15707,7 +15655,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B33+1))</f>
         <v/>
       </c>
-      <c r="C34" s="73" t="n"/>
+      <c r="C34" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
       <c r="F34" s="49" t="n"/>
@@ -15732,7 +15682,9 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n"/>
+      <c r="C35" s="71" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -15785,7 +15737,7 @@
         <v/>
       </c>
       <c r="C37" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D37" s="49" t="n"/>
       <c r="E37" s="49" t="n"/>
@@ -16390,9 +16342,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B3))</f>
         <v/>
       </c>
-      <c r="C7" s="69" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C7" s="69" t="n"/>
       <c r="D7" s="49" t="n"/>
       <c r="E7" s="49" t="n"/>
       <c r="F7" s="49" t="n"/>
@@ -16417,7 +16367,7 @@
         <v/>
       </c>
       <c r="C8" s="71" t="n">
-        <v>0.08333333333333333</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D8" s="49" t="n"/>
       <c r="E8" s="49" t="n"/>
@@ -16442,9 +16392,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B8+1))</f>
         <v/>
       </c>
-      <c r="C9" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C9" s="71" t="n"/>
       <c r="D9" s="49" t="n"/>
       <c r="E9" s="49" t="n"/>
       <c r="F9" s="49" t="n"/>
@@ -16468,7 +16416,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B9+1))</f>
         <v/>
       </c>
-      <c r="C10" s="71" t="n"/>
+      <c r="C10" s="71" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D10" s="49" t="n"/>
       <c r="E10" s="49" t="n"/>
       <c r="F10" s="49" t="n"/>
@@ -16492,7 +16442,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B10+1))</f>
         <v/>
       </c>
-      <c r="C11" s="71" t="n"/>
+      <c r="C11" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D11" s="49" t="n"/>
       <c r="E11" s="49" t="n"/>
       <c r="F11" s="49" t="n"/>
@@ -16542,9 +16494,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B12+1))</f>
         <v/>
       </c>
-      <c r="C13" s="73" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C13" s="73" t="n"/>
       <c r="D13" s="49" t="n"/>
       <c r="E13" s="49" t="n"/>
       <c r="F13" s="49" t="n"/>
@@ -16568,9 +16518,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B13+1))</f>
         <v/>
       </c>
-      <c r="C14" s="71" t="n">
-        <v>0.08333333333333333</v>
-      </c>
+      <c r="C14" s="71" t="n"/>
       <c r="D14" s="49" t="n"/>
       <c r="E14" s="49" t="n"/>
       <c r="F14" s="49" t="n"/>
@@ -16595,7 +16543,7 @@
         <v/>
       </c>
       <c r="C15" s="71" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D15" s="49" t="n"/>
       <c r="E15" s="49" t="n"/>
@@ -16620,9 +16568,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B15+1))</f>
         <v/>
       </c>
-      <c r="C16" s="74" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C16" s="74" t="n"/>
       <c r="D16" s="49" t="n"/>
       <c r="E16" s="49" t="n"/>
       <c r="F16" s="49" t="n"/>
@@ -16646,7 +16592,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B16+1))</f>
         <v/>
       </c>
-      <c r="C17" s="75" t="n"/>
+      <c r="C17" s="75" t="n">
+        <v>0.15625</v>
+      </c>
       <c r="D17" s="49" t="n"/>
       <c r="E17" s="49" t="n"/>
       <c r="F17" s="49" t="n"/>
@@ -16670,7 +16618,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B17+1))</f>
         <v/>
       </c>
-      <c r="C18" s="71" t="n"/>
+      <c r="C18" s="71" t="n">
+        <v>0.1875</v>
+      </c>
       <c r="D18" s="49" t="n"/>
       <c r="E18" s="49" t="n"/>
       <c r="F18" s="49" t="n"/>
@@ -16721,7 +16671,7 @@
         <v/>
       </c>
       <c r="C20" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D20" s="49" t="n"/>
       <c r="E20" s="49" t="n"/>
@@ -16746,9 +16696,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B20+1))</f>
         <v/>
       </c>
-      <c r="C21" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C21" s="71" t="n"/>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
       <c r="F21" s="49" t="n"/>
@@ -16773,7 +16721,7 @@
         <v/>
       </c>
       <c r="C22" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D22" s="49" t="n"/>
       <c r="E22" s="49" t="n"/>
@@ -16798,9 +16746,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B22+1))</f>
         <v/>
       </c>
-      <c r="C23" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C23" s="71" t="n"/>
       <c r="D23" s="49" t="n"/>
       <c r="E23" s="49" t="n"/>
       <c r="F23" s="49" t="n"/>
@@ -16824,7 +16770,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B23+1))</f>
         <v/>
       </c>
-      <c r="C24" s="71" t="n"/>
+      <c r="C24" s="71" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D24" s="49" t="n"/>
       <c r="E24" s="49" t="n"/>
       <c r="F24" s="49" t="n"/>
@@ -16848,7 +16796,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B24+1))</f>
         <v/>
       </c>
-      <c r="C25" s="71" t="n"/>
+      <c r="C25" s="71" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D25" s="49" t="n"/>
       <c r="E25" s="49" t="n"/>
       <c r="F25" s="49" t="n"/>
@@ -16899,7 +16849,7 @@
         <v/>
       </c>
       <c r="C27" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D27" s="49" t="n"/>
       <c r="E27" s="49" t="n"/>
@@ -16925,9 +16875,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B27+1))</f>
         <v/>
       </c>
-      <c r="C28" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C28" s="71" t="n"/>
       <c r="D28" s="49" t="n"/>
       <c r="E28" s="49" t="n"/>
       <c r="F28" s="49" t="n"/>
@@ -16953,7 +16901,7 @@
         <v/>
       </c>
       <c r="C29" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D29" s="49" t="n"/>
       <c r="E29" s="49" t="n"/>
@@ -16979,9 +16927,7 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B29+1))</f>
         <v/>
       </c>
-      <c r="C30" s="73" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C30" s="73" t="n"/>
       <c r="D30" s="49" t="n"/>
       <c r="E30" s="49" t="n"/>
       <c r="F30" s="49" t="n"/>
@@ -17006,7 +16952,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B30+1))</f>
         <v/>
       </c>
-      <c r="C31" s="73" t="n"/>
+      <c r="C31" s="73" t="n">
+        <v>0.1979166666666667</v>
+      </c>
       <c r="D31" s="49" t="n"/>
       <c r="E31" s="49" t="n"/>
       <c r="F31" s="49" t="n"/>
@@ -17031,7 +16979,9 @@
         <f>DATE(YEAR($B$3),MONTH($B$3),DAY(B31+1))</f>
         <v/>
       </c>
-      <c r="C32" s="73" t="n"/>
+      <c r="C32" s="73" t="n">
+        <v>0.2291666666666667</v>
+      </c>
       <c r="D32" s="49" t="n"/>
       <c r="E32" s="49" t="n"/>
       <c r="F32" s="49" t="n"/>
@@ -17084,7 +17034,7 @@
         <v/>
       </c>
       <c r="C34" s="73" t="n">
-        <v>0.125</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="D34" s="49" t="n"/>
       <c r="E34" s="49" t="n"/>
@@ -17110,9 +17060,7 @@
         <f>IF(B34="","",IF(DAY(B34+1)&gt;MONTH($B$3),B34+1,""))</f>
         <v/>
       </c>
-      <c r="C35" s="71" t="n">
-        <v>0.125</v>
-      </c>
+      <c r="C35" s="71" t="n"/>
       <c r="D35" s="49" t="n"/>
       <c r="E35" s="49" t="n"/>
       <c r="F35" s="49" t="n"/>
@@ -17138,7 +17086,7 @@
         <v/>
       </c>
       <c r="C36" s="71" t="n">
-        <v>0.125</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="D36" s="49" t="n"/>
       <c r="E36" s="49" t="n"/>

</xml_diff>